<commit_message>
sales tmp logic beta added + salesproduction sp added in initstores section
</commit_message>
<xml_diff>
--- a/templates/Sales_Purchase_Contract.xlsx
+++ b/templates/Sales_Purchase_Contract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F75A6DF-BA49-4FA8-9FA5-01286D5FEA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F38A94-F4D6-4A9C-8825-F572B6A6D3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
+    <workbookView xWindow="-50325" yWindow="3105" windowWidth="13440" windowHeight="7500" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales_Contract" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <definedName name="nonComNo">#REF!</definedName>
     <definedName name="№_пп">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Contract!$A$1:$E$83</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sales_Contract!$A$1:$E$79</definedName>
     <definedName name="Product_VR">'[1]Внутренний рынок'!$P$2</definedName>
     <definedName name="Product_VR_Spisok">'[1]Внутренний рынок'!$B$1</definedName>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="119">
   <si>
     <t>SALES AND PURCHASE CONTRACT</t>
   </si>
@@ -458,10 +458,6 @@
     <t>REQUEST FOR PAYMENT OF FOLLOWING IN TABLE GOODS</t>
   </si>
   <si>
-    <t>Opilio Snow Crab Live
-(Filling 80-90%)</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -479,9 +475,6 @@
   <si>
     <t>Blue King Crab Live
 (Filling 80-90%)</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>1 634 382,40 $</t>
@@ -1009,13 +1002,34 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1023,21 +1037,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1068,62 +1067,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1208,13 +1201,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>76202</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1228725</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>133353</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1296,6 +1289,7 @@
       <sheetName val="Продавец"/>
       <sheetName val="Вид операции"/>
       <sheetName val="Продукция"/>
+      <sheetName val="Движение ИНВОЙСЫ новое"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1381,6 +1375,7 @@
       <sheetData sheetId="24" refreshError="1"/>
       <sheetData sheetId="25" refreshError="1"/>
       <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1704,7 +1699,7 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="154" zoomScaleNormal="157" zoomScaleSheetLayoutView="154" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:E10"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1717,13 +1712,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="50.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="70"/>
@@ -1733,13 +1728,13 @@
       <c r="E2" s="70"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="75" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
+      <c r="A3" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="51" t="s">
@@ -1751,110 +1746,110 @@
       <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
       <c r="E6" s="54"/>
     </row>
     <row r="7" spans="1:5" s="50" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="77" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
+      <c r="A7" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
       <c r="E7" s="55"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
       <c r="E9" s="56"/>
     </row>
     <row r="10" spans="1:5" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
     </row>
     <row r="11" spans="1:5" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="71"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
     </row>
     <row r="12" spans="1:5" s="50" customFormat="1" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
     </row>
     <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
+      <c r="A13" s="74" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="52" t="s">
@@ -1864,7 +1859,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" s="52" t="s">
         <v>62</v>
@@ -1884,10 +1879,10 @@
         <v>18620</v>
       </c>
       <c r="D18" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E18" s="58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1901,10 +1896,10 @@
         <v>31200</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E19" s="58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1918,10 +1913,10 @@
         <v>19040</v>
       </c>
       <c r="D20" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E20" s="58" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1935,10 +1930,10 @@
         <v>2280</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E21" s="58" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1952,10 +1947,10 @@
         <v>260</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E22" s="58" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1972,7 +1967,7 @@
       </c>
       <c r="D23" s="52"/>
       <c r="E23" s="52" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1983,31 +1978,31 @@
       <c r="E24" s="58"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="73" t="s">
+      <c r="A25" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="73" t="s">
+      <c r="A27" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="73"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="52" t="s">
@@ -2017,7 +2012,7 @@
         <v>61</v>
       </c>
       <c r="C28" s="52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D28" s="52" t="s">
         <v>62</v>
@@ -2037,10 +2032,10 @@
         <v>18620</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2054,10 +2049,10 @@
         <v>31200</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2071,10 +2066,10 @@
         <v>19040</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E31" s="58" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2088,10 +2083,10 @@
         <v>2280</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E32" s="58" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2105,10 +2100,10 @@
         <v>260</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E33" s="58" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2125,7 +2120,7 @@
       </c>
       <c r="D34" s="52"/>
       <c r="E34" s="52" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2136,31 +2131,31 @@
       <c r="E35" s="58"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="73" t="s">
+      <c r="A36" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="73"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
+      <c r="B36" s="77"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="73" t="s">
+      <c r="A37" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="73"/>
-      <c r="C37" s="73"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
+      <c r="B37" s="77"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="73" t="s">
+      <c r="A38" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="73"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
+      <c r="B38" s="77"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="52" t="s">
@@ -2170,7 +2165,7 @@
         <v>61</v>
       </c>
       <c r="C39" s="52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D39" s="52" t="s">
         <v>62</v>
@@ -2190,10 +2185,10 @@
         <v>18620</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2207,10 +2202,10 @@
         <v>31200</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E41" s="58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2224,10 +2219,10 @@
         <v>19040</v>
       </c>
       <c r="D42" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E42" s="58" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2241,10 +2236,10 @@
         <v>2280</v>
       </c>
       <c r="D43" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E43" s="58" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -2258,10 +2253,10 @@
         <v>260</v>
       </c>
       <c r="D44" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E44" s="58" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2278,7 +2273,7 @@
       </c>
       <c r="D45" s="52"/>
       <c r="E45" s="52" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -2289,17 +2284,17 @@
       <c r="E46" s="58"/>
     </row>
     <row r="47" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="79" t="s">
+      <c r="A47" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="79"/>
-      <c r="C47" s="79"/>
-      <c r="D47" s="79"/>
-      <c r="E47" s="79"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
     </row>
     <row r="48" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="57" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B48" s="51"/>
       <c r="C48" s="51"/>
@@ -2339,29 +2334,29 @@
       <c r="E52" s="51"/>
     </row>
     <row r="53" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="76" t="s">
+      <c r="A53" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="76"/>
-      <c r="C53" s="76"/>
-      <c r="D53" s="76"/>
-      <c r="E53" s="76"/>
+      <c r="B53" s="72"/>
+      <c r="C53" s="72"/>
+      <c r="D53" s="72"/>
+      <c r="E53" s="72"/>
     </row>
     <row r="54" spans="1:5" s="3" customFormat="1" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="71" t="s">
+      <c r="A54" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="B54" s="71"/>
-      <c r="C54" s="71"/>
-      <c r="D54" s="71"/>
-      <c r="E54" s="71"/>
+      <c r="B54" s="74"/>
+      <c r="C54" s="74"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="91"/>
-      <c r="B55" s="91"/>
-      <c r="C55" s="91"/>
-      <c r="D55" s="91"/>
-      <c r="E55" s="91"/>
+      <c r="A55" s="79"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="79"/>
+      <c r="D55" s="79"/>
+      <c r="E55" s="79"/>
     </row>
     <row r="56" spans="1:5" s="50" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="68" t="s">
@@ -2373,22 +2368,22 @@
       <c r="E56" s="69"/>
     </row>
     <row r="57" spans="1:5" s="3" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="78" t="s">
-        <v>116</v>
-      </c>
-      <c r="B57" s="78"/>
-      <c r="C57" s="78"/>
-      <c r="D57" s="78"/>
-      <c r="E57" s="78"/>
+      <c r="A57" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" s="80"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="80"/>
+      <c r="E57" s="80"/>
     </row>
     <row r="58" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="71" t="s">
-        <v>117</v>
-      </c>
-      <c r="B58" s="71"/>
-      <c r="C58" s="71"/>
-      <c r="D58" s="71"/>
-      <c r="E58" s="71"/>
+      <c r="A58" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" s="74"/>
+      <c r="C58" s="74"/>
+      <c r="D58" s="74"/>
+      <c r="E58" s="74"/>
     </row>
     <row r="59" spans="1:5" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="64"/>
@@ -2398,67 +2393,67 @@
       <c r="E59" s="64"/>
     </row>
     <row r="60" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="73" t="s">
+      <c r="A60" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="73"/>
-      <c r="C60" s="73"/>
-      <c r="D60" s="73"/>
-      <c r="E60" s="73"/>
+      <c r="B60" s="77"/>
+      <c r="C60" s="77"/>
+      <c r="D60" s="77"/>
+      <c r="E60" s="77"/>
     </row>
     <row r="61" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="72" t="s">
+      <c r="A61" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="72"/>
-      <c r="C61" s="72"/>
-      <c r="D61" s="72"/>
-      <c r="E61" s="72"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="78"/>
+      <c r="D61" s="78"/>
+      <c r="E61" s="78"/>
     </row>
     <row r="62" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="71" t="s">
+      <c r="A62" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="71"/>
-      <c r="C62" s="71"/>
-      <c r="D62" s="71"/>
+      <c r="B62" s="74"/>
+      <c r="C62" s="74"/>
+      <c r="D62" s="74"/>
       <c r="E62" s="67"/>
     </row>
     <row r="63" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="79" t="s">
+      <c r="A63" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="B63" s="79"/>
-      <c r="C63" s="79"/>
-      <c r="D63" s="79"/>
-      <c r="E63" s="79"/>
+      <c r="B63" s="71"/>
+      <c r="C63" s="71"/>
+      <c r="D63" s="71"/>
+      <c r="E63" s="71"/>
     </row>
     <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="79" t="s">
+      <c r="A64" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B64" s="79"/>
-      <c r="C64" s="79"/>
-      <c r="D64" s="79"/>
-      <c r="E64" s="79"/>
+      <c r="B64" s="71"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="71"/>
     </row>
     <row r="65" spans="1:5" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="71" t="s">
+      <c r="A65" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="B65" s="71"/>
-      <c r="C65" s="71"/>
-      <c r="D65" s="71"/>
+      <c r="B65" s="74"/>
+      <c r="C65" s="74"/>
+      <c r="D65" s="74"/>
       <c r="E65" s="67"/>
     </row>
     <row r="66" spans="1:5" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="79" t="s">
+      <c r="A66" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="B66" s="79"/>
-      <c r="C66" s="79"/>
-      <c r="D66" s="79"/>
-      <c r="E66" s="79"/>
+      <c r="B66" s="71"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="71"/>
+      <c r="E66" s="71"/>
     </row>
     <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="64"/>
@@ -2477,49 +2472,49 @@
       <c r="E68" s="64"/>
     </row>
     <row r="69" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="72" t="s">
+      <c r="A69" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B69" s="72"/>
-      <c r="C69" s="72"/>
-      <c r="D69" s="72"/>
-      <c r="E69" s="72"/>
+      <c r="B69" s="78"/>
+      <c r="C69" s="78"/>
+      <c r="D69" s="78"/>
+      <c r="E69" s="78"/>
     </row>
     <row r="70" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="79" t="s">
+      <c r="A70" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="B70" s="79"/>
-      <c r="C70" s="79"/>
-      <c r="D70" s="79"/>
-      <c r="E70" s="79"/>
+      <c r="B70" s="71"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="71"/>
+      <c r="E70" s="71"/>
     </row>
     <row r="71" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="79" t="s">
+      <c r="A71" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B71" s="79"/>
-      <c r="C71" s="79"/>
-      <c r="D71" s="79"/>
-      <c r="E71" s="79"/>
+      <c r="B71" s="71"/>
+      <c r="C71" s="71"/>
+      <c r="D71" s="71"/>
+      <c r="E71" s="71"/>
     </row>
     <row r="72" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="79" t="s">
+      <c r="A72" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="B72" s="79"/>
-      <c r="C72" s="79"/>
-      <c r="D72" s="79"/>
-      <c r="E72" s="79"/>
+      <c r="B72" s="71"/>
+      <c r="C72" s="71"/>
+      <c r="D72" s="71"/>
+      <c r="E72" s="71"/>
     </row>
     <row r="73" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="79" t="s">
+      <c r="A73" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B73" s="79"/>
-      <c r="C73" s="79"/>
-      <c r="D73" s="79"/>
-      <c r="E73" s="79"/>
+      <c r="B73" s="71"/>
+      <c r="C73" s="71"/>
+      <c r="D73" s="71"/>
+      <c r="E73" s="71"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74" s="51"/>
@@ -2550,29 +2545,55 @@
       <c r="E77" s="64"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A78" s="80" t="s">
+      <c r="A78" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="B78" s="80"/>
+      <c r="B78" s="76"/>
       <c r="C78" s="65"/>
-      <c r="D78" s="80" t="s">
-        <v>118</v>
-      </c>
-      <c r="E78" s="80"/>
+      <c r="D78" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="E78" s="76"/>
     </row>
     <row r="79" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="92" t="s">
+      <c r="A79" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B79" s="92"/>
+      <c r="B79" s="73"/>
       <c r="C79" s="66"/>
-      <c r="D79" s="92" t="s">
+      <c r="D79" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="E79" s="92"/>
+      <c r="E79" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A69:E69"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A47:E47"/>
     <mergeCell ref="A70:E70"/>
     <mergeCell ref="A53:E53"/>
     <mergeCell ref="A79:B79"/>
@@ -2589,32 +2610,6 @@
     <mergeCell ref="A72:E72"/>
     <mergeCell ref="A73:E73"/>
     <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A69:E69"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A25:E25"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -2631,10 +2626,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2660,15 +2655,15 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
     </row>
     <row r="3" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="32" t="s">
@@ -2676,15 +2671,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="53.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
     </row>
     <row r="5" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="33"/>
@@ -2726,19 +2721,19 @@
         <v>88</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
     </row>
     <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="19"/>
@@ -2752,16 +2747,16 @@
         <v>85</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13" s="41" t="s">
         <v>63</v>
@@ -2772,13 +2767,13 @@
         <v>89</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E14" s="45">
         <v>56</v>
@@ -2790,243 +2785,174 @@
         <v>1410640</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="E15" s="45">
-        <v>39.200000000000003</v>
-      </c>
-      <c r="F15" s="38">
-        <v>1050</v>
-      </c>
-      <c r="G15" s="46">
-        <v>41160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="45">
-        <v>11</v>
-      </c>
-      <c r="F16" s="38">
-        <v>16128</v>
-      </c>
-      <c r="G16" s="46">
-        <v>177408</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="45">
-        <v>7.7</v>
-      </c>
-      <c r="F17" s="38">
-        <v>672</v>
-      </c>
-      <c r="G17" s="46">
-        <v>5174</v>
-      </c>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44"/>
+    </row>
+    <row r="17" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
+      <c r="A18" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
-    </row>
-    <row r="20" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="92" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="92"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="87" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="87"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="90" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" s="90"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="22"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="85" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="85"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="47" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="6.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="22"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="20"/>
-    </row>
-    <row r="25" spans="1:7" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
-    </row>
-    <row r="26" spans="1:7" s="17" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="87" t="s">
+      <c r="G20" s="47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="6.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="22"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="1:7" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
+      <c r="G22" s="88"/>
+    </row>
+    <row r="23" spans="1:7" s="17" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="87"/>
-      <c r="C26" s="87"/>
-    </row>
-    <row r="27" spans="1:7" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="88" t="s">
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
+    </row>
+    <row r="24" spans="1:7" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="88"/>
-      <c r="C27" s="88"/>
-    </row>
-    <row r="28" spans="1:7" s="17" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="81" t="s">
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+    </row>
+    <row r="25" spans="1:7" s="17" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="81"/>
-      <c r="C28" s="81"/>
-    </row>
-    <row r="29" spans="1:7" s="17" customFormat="1" ht="29.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="88" t="s">
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+    </row>
+    <row r="26" spans="1:7" s="17" customFormat="1" ht="29.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="88"/>
-      <c r="C29" s="88"/>
-    </row>
-    <row r="30" spans="1:7" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="88" t="s">
+      <c r="B26" s="90"/>
+      <c r="C26" s="90"/>
+    </row>
+    <row r="27" spans="1:7" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="88"/>
-      <c r="C30" s="88"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="30"/>
+    </row>
+    <row r="28" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="83"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="29"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D29" s="30"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D30" s="30"/>
     </row>
-    <row r="31" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="81"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="29"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="17"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D32" s="30"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D33" s="30"/>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D34" s="30"/>
-    </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="E39" s="17" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D31" s="30"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E36" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-    </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="E40" s="82" t="s">
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E37" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="82"/>
-      <c r="G40" s="82"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="E37:G37"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
@@ -3052,146 +2978,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
     </row>
     <row r="2" spans="1:5" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
     </row>
     <row r="5" spans="1:5" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="102"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
+      <c r="B7" s="97"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="93"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="104"/>
-      <c r="C9" s="104"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="104"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="100"/>
     </row>
     <row r="11" spans="1:5" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="103"/>
-      <c r="B11" s="103"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
+      <c r="A11" s="100"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="100"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="94"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="99"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="99"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="99"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="94" t="s">
+      <c r="A16" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="94"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="99"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
@@ -3201,7 +3127,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>62</v>
@@ -3221,10 +3147,10 @@
         <v>18620</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3238,10 +3164,10 @@
         <v>31200</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3255,10 +3181,10 @@
         <v>19040</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3272,10 +3198,10 @@
         <v>2280</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3289,10 +3215,10 @@
         <v>260</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3309,7 +3235,7 @@
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3320,31 +3246,31 @@
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="94"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="94"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="99"/>
+      <c r="E25" s="99"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="94" t="s">
+      <c r="A26" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="94"/>
-      <c r="C26" s="94"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="94"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="99"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="94" t="s">
+      <c r="A27" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="99"/>
+      <c r="E27" s="99"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
@@ -3354,7 +3280,7 @@
         <v>61</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>62</v>
@@ -3374,10 +3300,10 @@
         <v>18620</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3391,10 +3317,10 @@
         <v>31200</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3408,10 +3334,10 @@
         <v>19040</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3425,10 +3351,10 @@
         <v>2280</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3442,10 +3368,10 @@
         <v>260</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3462,7 +3388,7 @@
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3473,31 +3399,31 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="94" t="s">
+      <c r="A36" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="94"/>
-      <c r="C36" s="94"/>
-      <c r="D36" s="94"/>
-      <c r="E36" s="94"/>
+      <c r="B36" s="99"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="99"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="94"/>
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="94"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="99"/>
+      <c r="E37" s="99"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="94" t="s">
+      <c r="A38" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="94"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="94"/>
+      <c r="B38" s="99"/>
+      <c r="C38" s="99"/>
+      <c r="D38" s="99"/>
+      <c r="E38" s="99"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
@@ -3507,7 +3433,7 @@
         <v>61</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>62</v>
@@ -3527,10 +3453,10 @@
         <v>18620</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3544,10 +3470,10 @@
         <v>31200</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3561,10 +3487,10 @@
         <v>19040</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3578,10 +3504,10 @@
         <v>2280</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -3595,10 +3521,10 @@
         <v>260</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -3615,7 +3541,7 @@
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -3626,17 +3552,17 @@
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="93" t="s">
+      <c r="A47" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="93"/>
-      <c r="C47" s="93"/>
-      <c r="D47" s="93"/>
-      <c r="E47" s="93"/>
+      <c r="B47" s="96"/>
+      <c r="C47" s="96"/>
+      <c r="D47" s="96"/>
+      <c r="E47" s="96"/>
     </row>
     <row r="48" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -3669,29 +3595,29 @@
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" s="102" t="s">
+      <c r="A52" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="102"/>
-      <c r="C52" s="102"/>
-      <c r="D52" s="102"/>
-      <c r="E52" s="102"/>
+      <c r="B52" s="97"/>
+      <c r="C52" s="97"/>
+      <c r="D52" s="97"/>
+      <c r="E52" s="97"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53" s="103" t="s">
+      <c r="A53" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="103"/>
-      <c r="C53" s="103"/>
-      <c r="D53" s="103"/>
-      <c r="E53" s="103"/>
+      <c r="B53" s="100"/>
+      <c r="C53" s="100"/>
+      <c r="D53" s="100"/>
+      <c r="E53" s="100"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="95"/>
-      <c r="B54" s="95"/>
-      <c r="C54" s="95"/>
-      <c r="D54" s="95"/>
-      <c r="E54" s="95"/>
+      <c r="A54" s="106"/>
+      <c r="B54" s="106"/>
+      <c r="C54" s="106"/>
+      <c r="D54" s="106"/>
+      <c r="E54" s="106"/>
     </row>
     <row r="55" spans="1:5" s="3" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
@@ -3702,13 +3628,13 @@
       <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="101" t="s">
+      <c r="A56" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="101"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
-      <c r="E56" s="101"/>
+      <c r="B56" s="107"/>
+      <c r="C56" s="107"/>
+      <c r="D56" s="107"/>
+      <c r="E56" s="107"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
@@ -3719,167 +3645,149 @@
       <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" s="93" t="s">
+      <c r="A59" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="93"/>
-      <c r="C59" s="93"/>
-      <c r="D59" s="93"/>
-      <c r="E59" s="93"/>
+      <c r="B59" s="96"/>
+      <c r="C59" s="96"/>
+      <c r="D59" s="96"/>
+      <c r="E59" s="96"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" s="93" t="s">
+      <c r="A60" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="93"/>
-      <c r="C60" s="93"/>
-      <c r="D60" s="93"/>
-      <c r="E60" s="93"/>
+      <c r="B60" s="96"/>
+      <c r="C60" s="96"/>
+      <c r="D60" s="96"/>
+      <c r="E60" s="96"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" s="93" t="s">
+      <c r="A61" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="B61" s="93"/>
-      <c r="C61" s="93"/>
-      <c r="D61" s="93"/>
-      <c r="E61" s="93"/>
+      <c r="B61" s="96"/>
+      <c r="C61" s="96"/>
+      <c r="D61" s="96"/>
+      <c r="E61" s="96"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A62" s="93" t="s">
+      <c r="A62" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="B62" s="93"/>
-      <c r="C62" s="93"/>
-      <c r="D62" s="93"/>
-      <c r="E62" s="93"/>
+      <c r="B62" s="96"/>
+      <c r="C62" s="96"/>
+      <c r="D62" s="96"/>
+      <c r="E62" s="96"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A63" s="93" t="s">
+      <c r="A63" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="93"/>
-      <c r="C63" s="93"/>
-      <c r="D63" s="93"/>
-      <c r="E63" s="93"/>
+      <c r="B63" s="96"/>
+      <c r="C63" s="96"/>
+      <c r="D63" s="96"/>
+      <c r="E63" s="96"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A64" s="95"/>
-      <c r="B64" s="95"/>
-      <c r="C64" s="95"/>
-      <c r="D64" s="95"/>
-      <c r="E64" s="95"/>
+      <c r="A64" s="106"/>
+      <c r="B64" s="106"/>
+      <c r="C64" s="106"/>
+      <c r="D64" s="106"/>
+      <c r="E64" s="106"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A65" s="94" t="s">
+      <c r="A65" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="94"/>
-      <c r="C65" s="94"/>
-      <c r="D65" s="94"/>
-      <c r="E65" s="94"/>
+      <c r="B65" s="99"/>
+      <c r="C65" s="99"/>
+      <c r="D65" s="99"/>
+      <c r="E65" s="99"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A66" s="94" t="s">
+      <c r="A66" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="94"/>
-      <c r="C66" s="94"/>
-      <c r="D66" s="94"/>
-      <c r="E66" s="94"/>
+      <c r="B66" s="99"/>
+      <c r="C66" s="99"/>
+      <c r="D66" s="99"/>
+      <c r="E66" s="99"/>
     </row>
     <row r="67" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="96" t="s">
+      <c r="A67" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="96"/>
-      <c r="C67" s="96"/>
-      <c r="D67" s="96"/>
-      <c r="E67" s="96"/>
+      <c r="B67" s="101"/>
+      <c r="C67" s="101"/>
+      <c r="D67" s="101"/>
+      <c r="E67" s="101"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A68" s="94" t="s">
+      <c r="A68" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="94"/>
-      <c r="C68" s="94"/>
-      <c r="D68" s="94"/>
-      <c r="E68" s="94"/>
+      <c r="B68" s="99"/>
+      <c r="C68" s="99"/>
+      <c r="D68" s="99"/>
+      <c r="E68" s="99"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A69" s="94" t="s">
+      <c r="A69" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="94"/>
-      <c r="C69" s="94"/>
-      <c r="D69" s="94"/>
-      <c r="E69" s="94"/>
+      <c r="B69" s="99"/>
+      <c r="C69" s="99"/>
+      <c r="D69" s="99"/>
+      <c r="E69" s="99"/>
     </row>
     <row r="70" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="96" t="s">
+      <c r="A70" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="96"/>
-      <c r="C70" s="96"/>
-      <c r="D70" s="96"/>
-      <c r="E70" s="96"/>
+      <c r="B70" s="101"/>
+      <c r="C70" s="101"/>
+      <c r="D70" s="101"/>
+      <c r="E70" s="101"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A71" s="94" t="s">
+      <c r="A71" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="B71" s="94"/>
-      <c r="C71" s="94"/>
-      <c r="D71" s="94"/>
-      <c r="E71" s="94"/>
+      <c r="B71" s="99"/>
+      <c r="C71" s="99"/>
+      <c r="D71" s="99"/>
+      <c r="E71" s="99"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A82" s="100" t="s">
+      <c r="A82" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="100"/>
+      <c r="B82" s="105"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="98" t="s">
+      <c r="D82" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="E82" s="98"/>
+      <c r="E82" s="103"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A83" s="99" t="s">
+      <c r="A83" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="99"/>
+      <c r="B83" s="104"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="97" t="s">
+      <c r="D83" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="E83" s="97"/>
+      <c r="E83" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A54:E54"/>
     <mergeCell ref="A69:E69"/>
     <mergeCell ref="A70:E70"/>
     <mergeCell ref="A71:E71"/>
@@ -3896,11 +3804,29 @@
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -3925,108 +3851,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
+      <c r="B1" s="94"/>
     </row>
     <row r="2" spans="1:2" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="106"/>
+      <c r="B2" s="95"/>
     </row>
     <row r="3" spans="1:2" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="109"/>
+      <c r="B3" s="108"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="102"/>
+      <c r="B4" s="97"/>
     </row>
     <row r="5" spans="1:2" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="107"/>
+      <c r="B5" s="98"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="104"/>
+      <c r="B6" s="93"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="102"/>
+      <c r="B7" s="97"/>
     </row>
     <row r="8" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="93"/>
+      <c r="B8" s="96"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="104"/>
+      <c r="B9" s="93"/>
     </row>
     <row r="10" spans="1:2" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="103"/>
+      <c r="B10" s="100"/>
     </row>
     <row r="11" spans="1:2" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="103"/>
-      <c r="B11" s="103"/>
+      <c r="A11" s="100"/>
+      <c r="B11" s="100"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="94"/>
+      <c r="B12" s="99"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="93"/>
+      <c r="B13" s="96"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="95"/>
-      <c r="B14" s="95"/>
+      <c r="A14" s="106"/>
+      <c r="B14" s="106"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="94"/>
+      <c r="B15" s="99"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="93"/>
+      <c r="B16" s="96"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="93"/>
+      <c r="B17" s="96"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="93" t="s">
+      <c r="A18" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="93"/>
+      <c r="B18" s="96"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
@@ -4080,30 +4006,30 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="95"/>
-      <c r="B29" s="95"/>
+      <c r="A29" s="106"/>
+      <c r="B29" s="106"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="102" t="s">
+      <c r="A30" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="102"/>
+      <c r="B30" s="97"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="103"/>
+      <c r="B31" s="100"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="95"/>
-      <c r="B32" s="95"/>
+      <c r="A32" s="106"/>
+      <c r="B32" s="106"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="94" t="s">
+      <c r="A33" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="94"/>
+      <c r="B33" s="99"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
@@ -4111,10 +4037,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="108" t="s">
+      <c r="A35" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="108"/>
+      <c r="B35" s="109"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
@@ -4122,8 +4048,8 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="95"/>
-      <c r="B37" s="95"/>
+      <c r="A37" s="106"/>
+      <c r="B37" s="106"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
@@ -4131,10 +4057,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="103" t="s">
+      <c r="A39" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="103"/>
+      <c r="B39" s="100"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
@@ -4147,16 +4073,16 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="93" t="s">
+      <c r="A43" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="93"/>
+      <c r="B43" s="96"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="93" t="s">
+      <c r="A44" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="93"/>
+      <c r="B44" s="96"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
@@ -4165,110 +4091,110 @@
       <c r="B45" s="14"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="93" t="s">
+      <c r="A46" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="93"/>
+      <c r="B46" s="96"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" s="93" t="s">
+      <c r="A47" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="93"/>
+      <c r="B47" s="96"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" s="93" t="s">
+      <c r="A48" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="93"/>
+      <c r="B48" s="96"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" s="93" t="s">
+      <c r="A49" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="93"/>
+      <c r="B49" s="96"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" s="93" t="s">
+      <c r="A50" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="93"/>
+      <c r="B50" s="96"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="93" t="s">
+      <c r="A51" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="93"/>
+      <c r="B51" s="96"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" s="93" t="s">
+      <c r="A52" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="93"/>
+      <c r="B52" s="96"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="93" t="s">
+      <c r="A53" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="93"/>
+      <c r="B53" s="96"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" s="93" t="s">
+      <c r="A54" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="93"/>
+      <c r="B54" s="96"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" s="93" t="s">
+      <c r="A55" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="93"/>
+      <c r="B55" s="96"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" s="95"/>
-      <c r="B56" s="95"/>
+      <c r="A56" s="106"/>
+      <c r="B56" s="106"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" s="94" t="s">
+      <c r="A57" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="94"/>
+      <c r="B57" s="99"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" s="94" t="s">
+      <c r="A58" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="94"/>
+      <c r="B58" s="99"/>
     </row>
     <row r="59" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="96" t="s">
+      <c r="A59" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="96"/>
+      <c r="B59" s="101"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" s="94" t="s">
+      <c r="A60" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="94"/>
+      <c r="B60" s="99"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" s="94" t="s">
+      <c r="A61" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="94"/>
+      <c r="B61" s="99"/>
     </row>
     <row r="62" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="96" t="s">
+      <c r="A62" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="96"/>
+      <c r="B62" s="101"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" s="94" t="s">
+      <c r="A63" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="94"/>
+      <c r="B63" s="99"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
@@ -4288,20 +4214,22 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A30:B30"/>
@@ -4318,22 +4246,20 @@
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bl bug several rows beta fixed
</commit_message>
<xml_diff>
--- a/templates/Sales_Purchase_Contract.xlsx
+++ b/templates/Sales_Purchase_Contract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F38A94-F4D6-4A9C-8825-F572B6A6D3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1602FD4-22A5-4307-BF00-2162A459DFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50325" yWindow="3105" windowWidth="13440" windowHeight="7500" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales_Contract" sheetId="4" r:id="rId1"/>
@@ -24,13 +24,10 @@
   <definedNames>
     <definedName name="_Hlk38966714" localSheetId="2">Contract!#REF!</definedName>
     <definedName name="_Hlk38966714" localSheetId="3">'Contract Old'!$A$21</definedName>
-    <definedName name="_Hlk38966714" localSheetId="0">Sales_Contract!#REF!</definedName>
     <definedName name="_Hlk39074976" localSheetId="2">Contract!$A$15</definedName>
     <definedName name="_Hlk39074976" localSheetId="3">'Contract Old'!$A$18</definedName>
-    <definedName name="_Hlk39074976" localSheetId="0">Sales_Contract!$A$15</definedName>
     <definedName name="_Hlk39404391" localSheetId="2">Contract!#REF!</definedName>
     <definedName name="_Hlk39404391" localSheetId="3">'Contract Old'!$A$34</definedName>
-    <definedName name="_Hlk39404391" localSheetId="0">Sales_Contract!#REF!</definedName>
     <definedName name="Agr_No_EXP">#REF!</definedName>
     <definedName name="AgreementHidden">#REF!</definedName>
     <definedName name="AgrNo">#REF!</definedName>
@@ -47,11 +44,11 @@
     <definedName name="№_пп">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Contract!$A$1:$E$83</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sales_Contract!$A$1:$E$79</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sales_Contract!$A$1:$E$56</definedName>
     <definedName name="Product_VR">'[1]Внутренний рынок'!$P$2</definedName>
     <definedName name="Product_VR_Spisok">'[1]Внутренний рынок'!$B$1</definedName>
-    <definedName name="Sign_seller_end">#REF!</definedName>
-    <definedName name="Sign_seller_start">#REF!</definedName>
+    <definedName name="Sign_seller_end">Sales_Contract!$B$54</definedName>
+    <definedName name="Sign_seller_start">Sales_Contract!$A$54</definedName>
     <definedName name="Svod_EXP">[1]Экспорт!$O$36</definedName>
     <definedName name="Vessel_EXP">[1]Экспорт!$AC$1</definedName>
     <definedName name="Vessel_VR">'[1]Внутренний рынок'!$N$2</definedName>
@@ -71,25 +68,26 @@
     <definedName name="Клиенты">#REF!</definedName>
     <definedName name="КОЛ_ВО_ЭКС">#REF!</definedName>
     <definedName name="Коносамент_ВР">'[1]Внутренний рынок'!$M$2</definedName>
-    <definedName name="Контракт_адреса_банк">#REF!</definedName>
-    <definedName name="Контракт_адреса_банк_адрес">#REF!</definedName>
-    <definedName name="Контракт_адреса_банк_свифт">#REF!</definedName>
-    <definedName name="Контракт_адреса_продавец">#REF!</definedName>
-    <definedName name="Контракт_адреса_продавец_адрес">#REF!</definedName>
-    <definedName name="Контракт_адреса_счет">#REF!</definedName>
-    <definedName name="Контракт_дата">#REF!</definedName>
-    <definedName name="Контракт_доставка">#REF!</definedName>
+    <definedName name="Контракт_адреса_банк">Sales_Contract!$A$42</definedName>
+    <definedName name="Контракт_адреса_банк_адрес">Sales_Contract!$A$43</definedName>
+    <definedName name="Контракт_адреса_банк_свифт">Sales_Contract!$A$44</definedName>
+    <definedName name="Контракт_адреса_продавец">Sales_Contract!$A$39</definedName>
+    <definedName name="Контракт_адреса_продавец_адрес">Sales_Contract!$A$40</definedName>
+    <definedName name="Контракт_адреса_счет">Sales_Contract!$A$41</definedName>
+    <definedName name="Контракт_всего_цена">Sales_Contract!$A$26</definedName>
+    <definedName name="Контракт_дата">Sales_Contract!$A$4</definedName>
+    <definedName name="Контракт_доставка">Sales_Contract!$A$29</definedName>
     <definedName name="Контракт_ЕТА">#REF!</definedName>
-    <definedName name="Контракт_номер">#REF!</definedName>
-    <definedName name="Контракт_оплата">#REF!</definedName>
-    <definedName name="Контракт_покупатель">#REF!</definedName>
-    <definedName name="Контракт_покупатель_адрес">#REF!</definedName>
-    <definedName name="Контракт_покупатель_печать_подвал">#REF!</definedName>
-    <definedName name="Контракт_предмет">#REF!</definedName>
-    <definedName name="Контракт_предмет_массив">#REF!</definedName>
-    <definedName name="Контракт_продавец">#REF!</definedName>
-    <definedName name="Контракт_продавец_адрес">#REF!</definedName>
-    <definedName name="Контракт_продавец_печать_подвал">#REF!</definedName>
+    <definedName name="Контракт_номер">Sales_Contract!$A$3</definedName>
+    <definedName name="Контракт_оплата">Sales_Contract!$A$35</definedName>
+    <definedName name="Контракт_покупатель">Sales_Contract!$A$8</definedName>
+    <definedName name="Контракт_покупатель_адрес">Sales_Contract!$A$9</definedName>
+    <definedName name="Контракт_покупатель_печать_подвал">Sales_Contract!$D$56</definedName>
+    <definedName name="Контракт_предмет">Sales_Contract!$A$13</definedName>
+    <definedName name="Контракт_предмет_массив">Sales_Contract!$A$14</definedName>
+    <definedName name="Контракт_продавец">Sales_Contract!$A$5</definedName>
+    <definedName name="Контракт_продавец_адрес">Sales_Contract!$A$6</definedName>
+    <definedName name="Контракт_продавец_печать_подвал">Sales_Contract!$A$56</definedName>
     <definedName name="Краткое_наименование">#REF!</definedName>
     <definedName name="Область_печати_1">#REF!</definedName>
     <definedName name="Область_печати1">#REF!</definedName>
@@ -145,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="119">
   <si>
     <t>SALES AND PURCHASE CONTRACT</t>
   </si>
@@ -1001,17 +999,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1019,24 +1035,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1068,6 +1066,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1077,46 +1108,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1136,66 +1134,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>31295</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>572899</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 3" descr="A close-up of a sign&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99067E17-E39F-45A7-89A7-3A3D851D83D8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9525" y="16573499"/>
-          <a:ext cx="3193595" cy="1187263"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1696,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FEBAA7-C719-4E24-ABD3-2BE3A9A1FFF7}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="154" zoomScaleNormal="157" zoomScaleSheetLayoutView="154" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="154" zoomScaleNormal="157" zoomScaleSheetLayoutView="154" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1712,13 +1650,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="50.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="70"/>
@@ -1728,13 +1666,13 @@
       <c r="E2" s="70"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="51" t="s">
@@ -1746,110 +1684,110 @@
       <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
       <c r="E6" s="54"/>
     </row>
     <row r="7" spans="1:5" s="50" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
       <c r="E7" s="55"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
       <c r="E9" s="56"/>
     </row>
     <row r="10" spans="1:5" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
     </row>
     <row r="11" spans="1:5" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="74"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
     </row>
     <row r="12" spans="1:5" s="50" customFormat="1" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
     </row>
     <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="52" t="s">
@@ -1977,601 +1915,315 @@
       <c r="D24" s="58"/>
       <c r="E24" s="58"/>
     </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="77"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="77" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="77"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="77" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="77"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="52" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="58" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="58">
-        <v>931</v>
-      </c>
-      <c r="C29" s="60">
-        <v>18620</v>
-      </c>
-      <c r="D29" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E29" s="58" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="60">
-        <v>1560</v>
-      </c>
-      <c r="C30" s="60">
-        <v>31200</v>
-      </c>
-      <c r="D30" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E30" s="58" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="60">
-        <v>952</v>
-      </c>
-      <c r="C31" s="60">
-        <v>19040</v>
-      </c>
-      <c r="D31" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E31" s="58" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="60">
+    <row r="25" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+    </row>
+    <row r="26" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+    </row>
+    <row r="27" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="57"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+    </row>
+    <row r="28" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+    </row>
+    <row r="29" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+    </row>
+    <row r="30" spans="1:5" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="57"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+    </row>
+    <row r="31" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="76"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+    </row>
+    <row r="34" spans="1:5" s="50" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="69"/>
+    </row>
+    <row r="35" spans="1:5" s="3" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="78" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="60">
-        <v>2280</v>
-      </c>
-      <c r="D32" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E32" s="58" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="60">
-        <v>13</v>
-      </c>
-      <c r="C33" s="60">
-        <v>260</v>
-      </c>
-      <c r="D33" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E33" s="58" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="61">
-        <f>SUM(B29:B33)</f>
-        <v>3570</v>
-      </c>
-      <c r="C34" s="62">
-        <f xml:space="preserve"> SUM(C29:C33)</f>
-        <v>71400</v>
-      </c>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="58"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-    </row>
-    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="77"/>
-      <c r="C36" s="77"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-    </row>
-    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="77" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
-    </row>
-    <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="77"/>
-    </row>
-    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="E39" s="52" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="58" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" s="58">
-        <v>931</v>
-      </c>
-      <c r="C40" s="60">
-        <v>18620</v>
-      </c>
-      <c r="D40" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E40" s="58" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="60">
-        <v>1560</v>
-      </c>
-      <c r="C41" s="60">
-        <v>31200</v>
-      </c>
-      <c r="D41" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E41" s="58" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="60">
-        <v>952</v>
-      </c>
-      <c r="C42" s="60">
-        <v>19040</v>
-      </c>
-      <c r="D42" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E42" s="58" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="60">
-        <v>114</v>
-      </c>
-      <c r="C43" s="60">
-        <v>2280</v>
-      </c>
-      <c r="D43" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E43" s="58" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="60">
-        <v>13</v>
-      </c>
-      <c r="C44" s="60">
-        <v>260</v>
-      </c>
-      <c r="D44" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E44" s="58" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="61">
-        <f>SUM(B40:B44)</f>
-        <v>3570</v>
-      </c>
-      <c r="C45" s="62">
-        <f xml:space="preserve"> SUM(C40:C44)</f>
-        <v>71400</v>
-      </c>
-      <c r="D45" s="52"/>
-      <c r="E45" s="52" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="58"/>
-      <c r="B46" s="60"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-    </row>
-    <row r="47" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="71" t="s">
-        <v>72</v>
-      </c>
-      <c r="B47" s="71"/>
-      <c r="C47" s="71"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
-    </row>
-    <row r="48" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="57" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" s="51"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="51"/>
-    </row>
-    <row r="49" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="57"/>
-      <c r="B49" s="51"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="51"/>
-    </row>
-    <row r="50" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" s="51"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-    </row>
-    <row r="51" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
-    </row>
-    <row r="52" spans="1:5" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="57"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+    </row>
+    <row r="36" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="76" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="76"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+    </row>
+    <row r="37" spans="1:5" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="64"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+    </row>
+    <row r="38" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="74"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+    </row>
+    <row r="39" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="75"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
+    </row>
+    <row r="40" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="76"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="67"/>
+    </row>
+    <row r="41" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="79"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="79"/>
+    </row>
+    <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="79" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="79"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="79"/>
+      <c r="E42" s="79"/>
+    </row>
+    <row r="43" spans="1:5" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="76"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="67"/>
+    </row>
+    <row r="44" spans="1:5" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="79"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="79"/>
+      <c r="E44" s="79"/>
+    </row>
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="64"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+    </row>
+    <row r="46" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="63"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="64"/>
+    </row>
+    <row r="47" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="75"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
+    </row>
+    <row r="48" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="79"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="79"/>
+      <c r="E48" s="79"/>
+    </row>
+    <row r="49" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="79"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="79"/>
+      <c r="E49" s="79"/>
+    </row>
+    <row r="50" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="79"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="79"/>
+      <c r="E50" s="79"/>
+    </row>
+    <row r="51" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="79"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="79"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52" s="51"/>
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
     </row>
-    <row r="53" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="B53" s="72"/>
-      <c r="C53" s="72"/>
-      <c r="D53" s="72"/>
-      <c r="E53" s="72"/>
-    </row>
-    <row r="54" spans="1:5" s="3" customFormat="1" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" s="74"/>
-      <c r="C54" s="74"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-    </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="79"/>
-      <c r="B55" s="79"/>
-      <c r="C55" s="79"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="79"/>
-    </row>
-    <row r="56" spans="1:5" s="50" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="68"/>
-      <c r="C56" s="68"/>
-      <c r="D56" s="68"/>
-      <c r="E56" s="69"/>
-    </row>
-    <row r="57" spans="1:5" s="3" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="80" t="s">
-        <v>114</v>
-      </c>
-      <c r="B57" s="80"/>
-      <c r="C57" s="80"/>
-      <c r="D57" s="80"/>
-      <c r="E57" s="80"/>
-    </row>
-    <row r="58" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="74" t="s">
-        <v>115</v>
-      </c>
-      <c r="B58" s="74"/>
-      <c r="C58" s="74"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
-    </row>
-    <row r="59" spans="1:5" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="64"/>
-      <c r="B59" s="64"/>
-      <c r="C59" s="64"/>
-      <c r="D59" s="64"/>
-      <c r="E59" s="64"/>
-    </row>
-    <row r="60" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="B60" s="77"/>
-      <c r="C60" s="77"/>
-      <c r="D60" s="77"/>
-      <c r="E60" s="77"/>
-    </row>
-    <row r="61" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="78" t="s">
+    <row r="53" spans="1:5" ht="87.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="51"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51"/>
+    </row>
+    <row r="54" spans="1:5" ht="98.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="64"/>
+      <c r="D54" s="64"/>
+      <c r="E54" s="64"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="82"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55" s="82"/>
+    </row>
+    <row r="56" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="78"/>
-      <c r="C61" s="78"/>
-      <c r="D61" s="78"/>
-      <c r="E61" s="78"/>
-    </row>
-    <row r="62" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="74" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62" s="74"/>
-      <c r="C62" s="74"/>
-      <c r="D62" s="74"/>
-      <c r="E62" s="67"/>
-    </row>
-    <row r="63" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="B63" s="71"/>
-      <c r="C63" s="71"/>
-      <c r="D63" s="71"/>
-      <c r="E63" s="71"/>
-    </row>
-    <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="71" t="s">
-        <v>53</v>
-      </c>
-      <c r="B64" s="71"/>
-      <c r="C64" s="71"/>
-      <c r="D64" s="71"/>
-      <c r="E64" s="71"/>
-    </row>
-    <row r="65" spans="1:5" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="74" t="s">
-        <v>54</v>
-      </c>
-      <c r="B65" s="74"/>
-      <c r="C65" s="74"/>
-      <c r="D65" s="74"/>
-      <c r="E65" s="67"/>
-    </row>
-    <row r="66" spans="1:5" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="71" t="s">
-        <v>55</v>
-      </c>
-      <c r="B66" s="71"/>
-      <c r="C66" s="71"/>
-      <c r="D66" s="71"/>
-      <c r="E66" s="71"/>
-    </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="64"/>
-      <c r="B67" s="64"/>
-      <c r="C67" s="64"/>
-      <c r="D67" s="64"/>
-      <c r="E67" s="64"/>
-    </row>
-    <row r="68" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="63" t="s">
-        <v>36</v>
-      </c>
-      <c r="B68" s="63"/>
-      <c r="C68" s="63"/>
-      <c r="D68" s="63"/>
-      <c r="E68" s="64"/>
-    </row>
-    <row r="69" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="78" t="s">
-        <v>37</v>
-      </c>
-      <c r="B69" s="78"/>
-      <c r="C69" s="78"/>
-      <c r="D69" s="78"/>
-      <c r="E69" s="78"/>
-    </row>
-    <row r="70" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="B70" s="71"/>
-      <c r="C70" s="71"/>
-      <c r="D70" s="71"/>
-      <c r="E70" s="71"/>
-    </row>
-    <row r="71" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="B71" s="71"/>
-      <c r="C71" s="71"/>
-      <c r="D71" s="71"/>
-      <c r="E71" s="71"/>
-    </row>
-    <row r="72" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="71" t="s">
-        <v>42</v>
-      </c>
-      <c r="B72" s="71"/>
-      <c r="C72" s="71"/>
-      <c r="D72" s="71"/>
-      <c r="E72" s="71"/>
-    </row>
-    <row r="73" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="B73" s="71"/>
-      <c r="C73" s="71"/>
-      <c r="D73" s="71"/>
-      <c r="E73" s="71"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A74" s="51"/>
-      <c r="B74" s="51"/>
-      <c r="C74" s="51"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="51"/>
-    </row>
-    <row r="75" spans="1:5" ht="87.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="51"/>
-      <c r="B75" s="51"/>
-      <c r="C75" s="51"/>
-      <c r="D75" s="51"/>
-      <c r="E75" s="51"/>
-    </row>
-    <row r="76" spans="1:5" ht="50.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="64"/>
-      <c r="B76" s="64"/>
-      <c r="C76" s="64"/>
-      <c r="D76" s="64"/>
-      <c r="E76" s="64"/>
-    </row>
-    <row r="77" spans="1:5" ht="46.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="64"/>
-      <c r="B77" s="64"/>
-      <c r="C77" s="64"/>
-      <c r="D77" s="64"/>
-      <c r="E77" s="64"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A78" s="76" t="s">
-        <v>57</v>
-      </c>
-      <c r="B78" s="76"/>
-      <c r="C78" s="65"/>
-      <c r="D78" s="76" t="s">
-        <v>116</v>
-      </c>
-      <c r="E78" s="76"/>
-    </row>
-    <row r="79" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="73" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" s="73"/>
-      <c r="C79" s="66"/>
-      <c r="D79" s="73" t="s">
+      <c r="B56" s="80"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="E79" s="73"/>
+      <c r="E56" s="80"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="36">
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A39:E39"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A26:E26"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:E11"/>
@@ -2581,43 +2233,13 @@
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A69:E69"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A70:E70"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A71:E71"/>
-    <mergeCell ref="A72:E72"/>
-    <mergeCell ref="A73:E73"/>
-    <mergeCell ref="A60:E60"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="92" fitToHeight="2" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="51" max="4" man="1"/>
+    <brk id="29" max="4" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2978,146 +2600,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
     </row>
     <row r="2" spans="1:5" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
     </row>
     <row r="5" spans="1:5" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="97"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
+      <c r="B8" s="93"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
+      <c r="B9" s="104"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="100" t="s">
+      <c r="A10" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="100"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="100"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
     </row>
     <row r="11" spans="1:5" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="100"/>
-      <c r="B11" s="100"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
+      <c r="A11" s="103"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="99" t="s">
+      <c r="A12" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="99"/>
-      <c r="C12" s="99"/>
-      <c r="D12" s="99"/>
-      <c r="E12" s="99"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="96" t="s">
+      <c r="A13" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="96"/>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="99" t="s">
+      <c r="A14" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="99"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="99"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="99" t="s">
+      <c r="A15" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="99"/>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="99"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="99"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
@@ -3246,31 +2868,31 @@
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="99" t="s">
+      <c r="A25" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="99"/>
-      <c r="C25" s="99"/>
-      <c r="D25" s="99"/>
-      <c r="E25" s="99"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="99" t="s">
+      <c r="A26" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="99"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="99"/>
-      <c r="E26" s="99"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
+      <c r="E26" s="94"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="99" t="s">
+      <c r="A27" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="99"/>
-      <c r="C27" s="99"/>
-      <c r="D27" s="99"/>
-      <c r="E27" s="99"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
@@ -3399,31 +3021,31 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="99" t="s">
+      <c r="A36" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="99"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="99"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="94"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="99" t="s">
+      <c r="A37" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="99"/>
-      <c r="C37" s="99"/>
-      <c r="D37" s="99"/>
-      <c r="E37" s="99"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="99" t="s">
+      <c r="A38" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="99"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="99"/>
+      <c r="B38" s="94"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="94"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
@@ -3552,13 +3174,13 @@
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="96" t="s">
+      <c r="A47" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="96"/>
-      <c r="C47" s="96"/>
-      <c r="D47" s="96"/>
-      <c r="E47" s="96"/>
+      <c r="B47" s="93"/>
+      <c r="C47" s="93"/>
+      <c r="D47" s="93"/>
+      <c r="E47" s="93"/>
     </row>
     <row r="48" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
@@ -3595,29 +3217,29 @@
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" s="97" t="s">
+      <c r="A52" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="97"/>
-      <c r="C52" s="97"/>
-      <c r="D52" s="97"/>
-      <c r="E52" s="97"/>
+      <c r="B52" s="102"/>
+      <c r="C52" s="102"/>
+      <c r="D52" s="102"/>
+      <c r="E52" s="102"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53" s="100" t="s">
+      <c r="A53" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="100"/>
-      <c r="C53" s="100"/>
-      <c r="D53" s="100"/>
-      <c r="E53" s="100"/>
+      <c r="B53" s="103"/>
+      <c r="C53" s="103"/>
+      <c r="D53" s="103"/>
+      <c r="E53" s="103"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="106"/>
-      <c r="B54" s="106"/>
-      <c r="C54" s="106"/>
-      <c r="D54" s="106"/>
-      <c r="E54" s="106"/>
+      <c r="A54" s="95"/>
+      <c r="B54" s="95"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="95"/>
+      <c r="E54" s="95"/>
     </row>
     <row r="55" spans="1:5" s="3" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
@@ -3628,13 +3250,13 @@
       <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="107" t="s">
+      <c r="A56" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="107"/>
-      <c r="C56" s="107"/>
-      <c r="D56" s="107"/>
-      <c r="E56" s="107"/>
+      <c r="B56" s="101"/>
+      <c r="C56" s="101"/>
+      <c r="D56" s="101"/>
+      <c r="E56" s="101"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
@@ -3645,149 +3267,167 @@
       <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" s="96" t="s">
+      <c r="A59" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="96"/>
-      <c r="C59" s="96"/>
-      <c r="D59" s="96"/>
-      <c r="E59" s="96"/>
+      <c r="B59" s="93"/>
+      <c r="C59" s="93"/>
+      <c r="D59" s="93"/>
+      <c r="E59" s="93"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" s="96" t="s">
+      <c r="A60" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="96"/>
-      <c r="C60" s="96"/>
-      <c r="D60" s="96"/>
-      <c r="E60" s="96"/>
+      <c r="B60" s="93"/>
+      <c r="C60" s="93"/>
+      <c r="D60" s="93"/>
+      <c r="E60" s="93"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" s="96" t="s">
+      <c r="A61" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="B61" s="96"/>
-      <c r="C61" s="96"/>
-      <c r="D61" s="96"/>
-      <c r="E61" s="96"/>
+      <c r="B61" s="93"/>
+      <c r="C61" s="93"/>
+      <c r="D61" s="93"/>
+      <c r="E61" s="93"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A62" s="96" t="s">
+      <c r="A62" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="B62" s="96"/>
-      <c r="C62" s="96"/>
-      <c r="D62" s="96"/>
-      <c r="E62" s="96"/>
+      <c r="B62" s="93"/>
+      <c r="C62" s="93"/>
+      <c r="D62" s="93"/>
+      <c r="E62" s="93"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A63" s="96" t="s">
+      <c r="A63" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="96"/>
-      <c r="C63" s="96"/>
-      <c r="D63" s="96"/>
-      <c r="E63" s="96"/>
+      <c r="B63" s="93"/>
+      <c r="C63" s="93"/>
+      <c r="D63" s="93"/>
+      <c r="E63" s="93"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A64" s="106"/>
-      <c r="B64" s="106"/>
-      <c r="C64" s="106"/>
-      <c r="D64" s="106"/>
-      <c r="E64" s="106"/>
+      <c r="A64" s="95"/>
+      <c r="B64" s="95"/>
+      <c r="C64" s="95"/>
+      <c r="D64" s="95"/>
+      <c r="E64" s="95"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A65" s="99" t="s">
+      <c r="A65" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="99"/>
-      <c r="C65" s="99"/>
-      <c r="D65" s="99"/>
-      <c r="E65" s="99"/>
+      <c r="B65" s="94"/>
+      <c r="C65" s="94"/>
+      <c r="D65" s="94"/>
+      <c r="E65" s="94"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A66" s="99" t="s">
+      <c r="A66" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="99"/>
-      <c r="C66" s="99"/>
-      <c r="D66" s="99"/>
-      <c r="E66" s="99"/>
+      <c r="B66" s="94"/>
+      <c r="C66" s="94"/>
+      <c r="D66" s="94"/>
+      <c r="E66" s="94"/>
     </row>
     <row r="67" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="101" t="s">
+      <c r="A67" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="101"/>
-      <c r="C67" s="101"/>
-      <c r="D67" s="101"/>
-      <c r="E67" s="101"/>
+      <c r="B67" s="96"/>
+      <c r="C67" s="96"/>
+      <c r="D67" s="96"/>
+      <c r="E67" s="96"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A68" s="99" t="s">
+      <c r="A68" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="99"/>
-      <c r="C68" s="99"/>
-      <c r="D68" s="99"/>
-      <c r="E68" s="99"/>
+      <c r="B68" s="94"/>
+      <c r="C68" s="94"/>
+      <c r="D68" s="94"/>
+      <c r="E68" s="94"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A69" s="99" t="s">
+      <c r="A69" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="99"/>
-      <c r="C69" s="99"/>
-      <c r="D69" s="99"/>
-      <c r="E69" s="99"/>
+      <c r="B69" s="94"/>
+      <c r="C69" s="94"/>
+      <c r="D69" s="94"/>
+      <c r="E69" s="94"/>
     </row>
     <row r="70" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="101" t="s">
+      <c r="A70" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="101"/>
-      <c r="C70" s="101"/>
-      <c r="D70" s="101"/>
-      <c r="E70" s="101"/>
+      <c r="B70" s="96"/>
+      <c r="C70" s="96"/>
+      <c r="D70" s="96"/>
+      <c r="E70" s="96"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A71" s="99" t="s">
+      <c r="A71" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="B71" s="99"/>
-      <c r="C71" s="99"/>
-      <c r="D71" s="99"/>
-      <c r="E71" s="99"/>
+      <c r="B71" s="94"/>
+      <c r="C71" s="94"/>
+      <c r="D71" s="94"/>
+      <c r="E71" s="94"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A82" s="105" t="s">
+      <c r="A82" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="105"/>
+      <c r="B82" s="100"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="103" t="s">
+      <c r="D82" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="E82" s="103"/>
+      <c r="E82" s="98"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A83" s="104" t="s">
+      <c r="A83" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="104"/>
+      <c r="B83" s="99"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="102" t="s">
+      <c r="D83" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="E83" s="102"/>
+      <c r="E83" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A47:E47"/>
     <mergeCell ref="A69:E69"/>
     <mergeCell ref="A70:E70"/>
     <mergeCell ref="A71:E71"/>
@@ -3804,29 +3444,11 @@
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A54:E54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -3851,108 +3473,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="94"/>
+      <c r="B1" s="105"/>
     </row>
     <row r="2" spans="1:2" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="106"/>
     </row>
     <row r="3" spans="1:2" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="108"/>
+      <c r="B3" s="109"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="97"/>
+      <c r="B4" s="102"/>
     </row>
     <row r="5" spans="1:2" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="98"/>
+      <c r="B5" s="107"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="93"/>
+      <c r="B6" s="104"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="97"/>
+      <c r="B7" s="102"/>
     </row>
     <row r="8" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="96"/>
+      <c r="B8" s="93"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="93"/>
+      <c r="B9" s="104"/>
     </row>
     <row r="10" spans="1:2" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="100" t="s">
+      <c r="A10" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="100"/>
+      <c r="B10" s="103"/>
     </row>
     <row r="11" spans="1:2" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="100"/>
-      <c r="B11" s="100"/>
+      <c r="A11" s="103"/>
+      <c r="B11" s="103"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="99" t="s">
+      <c r="A12" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="99"/>
+      <c r="B12" s="94"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="96" t="s">
+      <c r="A13" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="96"/>
+      <c r="B13" s="93"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="106"/>
-      <c r="B14" s="106"/>
+      <c r="A14" s="95"/>
+      <c r="B14" s="95"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="99" t="s">
+      <c r="A15" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="99"/>
+      <c r="B15" s="94"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="96" t="s">
+      <c r="A16" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="96"/>
+      <c r="B16" s="93"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="96" t="s">
+      <c r="A17" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="96"/>
+      <c r="B17" s="93"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="96" t="s">
+      <c r="A18" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="96"/>
+      <c r="B18" s="93"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
@@ -4006,30 +3628,30 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="106"/>
-      <c r="B29" s="106"/>
+      <c r="A29" s="95"/>
+      <c r="B29" s="95"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="97" t="s">
+      <c r="A30" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="97"/>
+      <c r="B30" s="102"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="100" t="s">
+      <c r="A31" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="100"/>
+      <c r="B31" s="103"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="106"/>
-      <c r="B32" s="106"/>
+      <c r="A32" s="95"/>
+      <c r="B32" s="95"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="99" t="s">
+      <c r="A33" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="99"/>
+      <c r="B33" s="94"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
@@ -4037,10 +3659,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="109" t="s">
+      <c r="A35" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="109"/>
+      <c r="B35" s="108"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
@@ -4048,8 +3670,8 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="106"/>
-      <c r="B37" s="106"/>
+      <c r="A37" s="95"/>
+      <c r="B37" s="95"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
@@ -4057,10 +3679,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="100" t="s">
+      <c r="A39" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="100"/>
+      <c r="B39" s="103"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
@@ -4073,16 +3695,16 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="96" t="s">
+      <c r="A43" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="96"/>
+      <c r="B43" s="93"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="96" t="s">
+      <c r="A44" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="96"/>
+      <c r="B44" s="93"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
@@ -4091,110 +3713,110 @@
       <c r="B45" s="14"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="96" t="s">
+      <c r="A46" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="96"/>
+      <c r="B46" s="93"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" s="96" t="s">
+      <c r="A47" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="96"/>
+      <c r="B47" s="93"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" s="96" t="s">
+      <c r="A48" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="96"/>
+      <c r="B48" s="93"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" s="96" t="s">
+      <c r="A49" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="96"/>
+      <c r="B49" s="93"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" s="96" t="s">
+      <c r="A50" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="96"/>
+      <c r="B50" s="93"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="96" t="s">
+      <c r="A51" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="96"/>
+      <c r="B51" s="93"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" s="96" t="s">
+      <c r="A52" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="96"/>
+      <c r="B52" s="93"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="96" t="s">
+      <c r="A53" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="96"/>
+      <c r="B53" s="93"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" s="96" t="s">
+      <c r="A54" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="96"/>
+      <c r="B54" s="93"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" s="96" t="s">
+      <c r="A55" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="96"/>
+      <c r="B55" s="93"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" s="106"/>
-      <c r="B56" s="106"/>
+      <c r="A56" s="95"/>
+      <c r="B56" s="95"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" s="99" t="s">
+      <c r="A57" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="99"/>
+      <c r="B57" s="94"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" s="99" t="s">
+      <c r="A58" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="99"/>
+      <c r="B58" s="94"/>
     </row>
     <row r="59" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="101" t="s">
+      <c r="A59" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="101"/>
+      <c r="B59" s="96"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" s="99" t="s">
+      <c r="A60" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="99"/>
+      <c r="B60" s="94"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" s="99" t="s">
+      <c r="A61" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="99"/>
+      <c r="B61" s="94"/>
     </row>
     <row r="62" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="101" t="s">
+      <c r="A62" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="101"/>
+      <c r="B62" s="96"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" s="99" t="s">
+      <c r="A63" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="99"/>
+      <c r="B63" s="94"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
@@ -4214,6 +3836,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A58:B58"/>
@@ -4230,36 +3882,6 @@
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
beta salescontractdefault tmp implemented
</commit_message>
<xml_diff>
--- a/templates/Sales_Purchase_Contract.xlsx
+++ b/templates/Sales_Purchase_Contract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1602FD4-22A5-4307-BF00-2162A459DFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED51279F-C366-4839-B161-6812D78C9724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
   </bookViews>
@@ -18,9 +18,6 @@
     <sheet name="Contract" sheetId="2" state="hidden" r:id="rId3"/>
     <sheet name="Contract Old" sheetId="1" state="hidden" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_Hlk38966714" localSheetId="2">Contract!#REF!</definedName>
     <definedName name="_Hlk38966714" localSheetId="3">'Contract Old'!$A$21</definedName>
@@ -28,99 +25,29 @@
     <definedName name="_Hlk39074976" localSheetId="3">'Contract Old'!$A$18</definedName>
     <definedName name="_Hlk39404391" localSheetId="2">Contract!#REF!</definedName>
     <definedName name="_Hlk39404391" localSheetId="3">'Contract Old'!$A$34</definedName>
-    <definedName name="Agr_No_EXP">#REF!</definedName>
-    <definedName name="AgreementHidden">#REF!</definedName>
-    <definedName name="AgrNo">#REF!</definedName>
-    <definedName name="BL_Key">#REF!</definedName>
-    <definedName name="BL_List">#REF!</definedName>
-    <definedName name="Disch_BL">'[1]Инвойсы выгрузка'!$O$2</definedName>
-    <definedName name="Dop_EXP">[1]Экспорт!$U$35</definedName>
-    <definedName name="ID_AGR_STR">#REF!</definedName>
-    <definedName name="ID_EKSPORT">#REF!</definedName>
-    <definedName name="ID_Эксп_ДОП">#REF!</definedName>
-    <definedName name="Konosament_EXP">[1]Экспорт!$B$36</definedName>
-    <definedName name="logo">INDEX([1]Б!$A$1:$A$2,MATCH(Порт_Компания,[1]Б!$B$1:$B$2,0))</definedName>
-    <definedName name="nonComNo">#REF!</definedName>
-    <definedName name="№_пп">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Contract!$A$1:$E$83</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sales_Contract!$A$1:$E$56</definedName>
-    <definedName name="Product_VR">'[1]Внутренний рынок'!$P$2</definedName>
-    <definedName name="Product_VR_Spisok">'[1]Внутренний рынок'!$B$1</definedName>
-    <definedName name="Sign_seller_end">Sales_Contract!$B$54</definedName>
-    <definedName name="Sign_seller_start">Sales_Contract!$A$54</definedName>
-    <definedName name="Svod_EXP">[1]Экспорт!$O$36</definedName>
-    <definedName name="Vessel_EXP">[1]Экспорт!$AC$1</definedName>
-    <definedName name="Vessel_VR">'[1]Внутренний рынок'!$N$2</definedName>
-    <definedName name="Vessel_VV">'[1]Внутренний рынок'!$A$1</definedName>
-    <definedName name="ВМРП">#REF!</definedName>
-    <definedName name="ДалькомХолод">#REF!</definedName>
-    <definedName name="ДВ_Порт">#REF!</definedName>
-    <definedName name="ДоговорНомер">#REF!</definedName>
-    <definedName name="Допы_Хранение">#REF!</definedName>
-    <definedName name="Заявка">#REF!</definedName>
-    <definedName name="Заявка_Изготовитель">#REF!</definedName>
-    <definedName name="Заявка_наименование">#REF!</definedName>
-    <definedName name="Заявка_Покупатель">#REF!</definedName>
-    <definedName name="Заявка_Сорт">#REF!</definedName>
-    <definedName name="Заявка_Упаковка">#REF!</definedName>
-    <definedName name="Инвойс_Заявка">#REF!</definedName>
-    <definedName name="Клиенты">#REF!</definedName>
-    <definedName name="КОЛ_ВО_ЭКС">#REF!</definedName>
-    <definedName name="Коносамент_ВР">'[1]Внутренний рынок'!$M$2</definedName>
-    <definedName name="Контракт_адреса_банк">Sales_Contract!$A$42</definedName>
-    <definedName name="Контракт_адреса_банк_адрес">Sales_Contract!$A$43</definedName>
-    <definedName name="Контракт_адреса_банк_свифт">Sales_Contract!$A$44</definedName>
-    <definedName name="Контракт_адреса_продавец">Sales_Contract!$A$39</definedName>
-    <definedName name="Контракт_адреса_продавец_адрес">Sales_Contract!$A$40</definedName>
-    <definedName name="Контракт_адреса_счет">Sales_Contract!$A$41</definedName>
-    <definedName name="Контракт_всего_цена">Sales_Contract!$A$26</definedName>
+    <definedName name="Sign_seller_end">Sales_Contract!$B$53</definedName>
+    <definedName name="Sign_seller_start">Sales_Contract!$A$53</definedName>
+    <definedName name="Документация_BL">Sales_Contract!$A$50</definedName>
+    <definedName name="Контракт_адреса_банк">Sales_Contract!$A$41</definedName>
+    <definedName name="Контракт_адреса_банк_адрес">Sales_Contract!$A$42</definedName>
+    <definedName name="Контракт_адреса_банк_свифт">Sales_Contract!$A$43</definedName>
+    <definedName name="Контракт_адреса_продавец">Sales_Contract!$A$38</definedName>
+    <definedName name="Контракт_адреса_продавец_адрес">Sales_Contract!$A$39</definedName>
+    <definedName name="Контракт_адреса_счет">Sales_Contract!$A$40</definedName>
+    <definedName name="Контракт_всего_цена">Sales_Contract!$A$25</definedName>
     <definedName name="Контракт_дата">Sales_Contract!$A$4</definedName>
-    <definedName name="Контракт_доставка">Sales_Contract!$A$29</definedName>
-    <definedName name="Контракт_ЕТА">#REF!</definedName>
+    <definedName name="Контракт_доставка">Sales_Contract!$A$28</definedName>
     <definedName name="Контракт_номер">Sales_Contract!$A$3</definedName>
-    <definedName name="Контракт_оплата">Sales_Contract!$A$35</definedName>
+    <definedName name="Контракт_оплата">Sales_Contract!$A$34</definedName>
     <definedName name="Контракт_покупатель">Sales_Contract!$A$8</definedName>
     <definedName name="Контракт_покупатель_адрес">Sales_Contract!$A$9</definedName>
-    <definedName name="Контракт_покупатель_печать_подвал">Sales_Contract!$D$56</definedName>
+    <definedName name="Контракт_покупатель_печать_подвал">Sales_Contract!$D$55</definedName>
     <definedName name="Контракт_предмет">Sales_Contract!$A$13</definedName>
     <definedName name="Контракт_предмет_массив">Sales_Contract!$A$14</definedName>
     <definedName name="Контракт_продавец">Sales_Contract!$A$5</definedName>
     <definedName name="Контракт_продавец_адрес">Sales_Contract!$A$6</definedName>
-    <definedName name="Контракт_продавец_печать_подвал">Sales_Contract!$A$56</definedName>
-    <definedName name="Краткое_наименование">#REF!</definedName>
-    <definedName name="Область_печати_1">#REF!</definedName>
-    <definedName name="Область_печати1">#REF!</definedName>
-    <definedName name="Письмо">#REF!</definedName>
-    <definedName name="Письмо_в_Порт">#REF!</definedName>
-    <definedName name="Полное_наименование">#REF!</definedName>
-    <definedName name="Порт_Договор">#REF!</definedName>
-    <definedName name="Порт_Договор_Фильтр">#REF!</definedName>
-    <definedName name="Порт_Компания">#REF!</definedName>
-    <definedName name="Порт_Магадан">[1]!SPTamozhnya[Порт]</definedName>
-    <definedName name="Прод_тест">[1]Коносаменты!#REF!</definedName>
-    <definedName name="ПРОД_ЭКС">#REF!</definedName>
-    <definedName name="ПРОД_ЭКС_1">#REF!</definedName>
-    <definedName name="ПРОД_ЭКС_2">#REF!</definedName>
-    <definedName name="ПРОД_ЭКС2">#REF!</definedName>
-    <definedName name="Руководство">#REF!</definedName>
-    <definedName name="СОРТ_ЭКСП">#REF!</definedName>
-    <definedName name="СУММ_ЭКСП">#REF!</definedName>
-    <definedName name="Сумма_Тов">#REF!</definedName>
-    <definedName name="Телефон">#REF!</definedName>
-    <definedName name="ТОВ_1">#REF!</definedName>
-    <definedName name="ХР_BL">#REF!</definedName>
-    <definedName name="ХР_ID">#REF!</definedName>
-    <definedName name="ХР_Product">#REF!</definedName>
-    <definedName name="ХР_Колво">#REF!</definedName>
-    <definedName name="ХР_Объем">#REF!</definedName>
-    <definedName name="ХР_Продукция">#REF!</definedName>
-    <definedName name="ХР_Сумма">#REF!</definedName>
-    <definedName name="ХР_Упаковка">#REF!</definedName>
-    <definedName name="ХР_Цена">#REF!</definedName>
-    <definedName name="Хранение_продукция">'[1]Экспорт Хранение'!$AF$1</definedName>
-    <definedName name="Хранение_Суда">'[1]Экспорт Хранение'!$AE$1</definedName>
-    <definedName name="ЦЕНА_ЭКСП">#REF!</definedName>
+    <definedName name="Контракт_продавец_печать_подвал">Sales_Contract!$A$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -143,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="119">
   <si>
     <t>SALES AND PURCHASE CONTRACT</t>
   </si>
@@ -508,16 +435,10 @@
     <t>(hereafter called “Seller”)</t>
   </si>
   <si>
-    <t>1.1. The Seller agrees to sell and the Buyer agrees to purchase Frozen Opilio Snow Crab with the following terms and conditions:</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.1 The payment to be in US Dollar 100% value should be made by T.T. to the designated the Seller’s or Agent’s bank account within 5 banking days after the all parties signed the contract. </t>
   </si>
   <si>
     <t>4.2 The Seller performs production tittle transfer after 100% payment to Seller’s banking account.</t>
-  </si>
-  <si>
-    <t>____________________________________________</t>
   </si>
   <si>
     <r>
@@ -547,6 +468,12 @@
   </si>
   <si>
     <t>Price/kg</t>
+  </si>
+  <si>
+    <t>_____________________________________________________</t>
+  </si>
+  <si>
+    <t>1.1. The Seller agrees to sell and the Buyer agrees to purchase goods with following in table assortment and condititions:</t>
   </si>
 </sst>
 </file>
@@ -999,42 +926,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1066,55 +987,61 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1191,132 +1118,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Картинки"/>
-      <sheetName val="SPSortAssortiment"/>
-      <sheetName val="SPPackage"/>
-      <sheetName val="Инвойсы хранение"/>
-      <sheetName val="Инвойсы выгрузка"/>
-      <sheetName val="Коносаменты"/>
-      <sheetName val="№рейса_справочник"/>
-      <sheetName val="Образцы"/>
-      <sheetName val="Транспорта"/>
-      <sheetName val="Экспорт"/>
-      <sheetName val="Экспорт Хранение"/>
-      <sheetName val="Внутренний рынок"/>
-      <sheetName val="SP_Consignee"/>
-      <sheetName val="SPContract"/>
-      <sheetName val="SPAgent"/>
-      <sheetName val="SPBankProdavec"/>
-      <sheetName val="SPPortZarubezh"/>
-      <sheetName val="SPRekvizitBankProdavec"/>
-      <sheetName val="SPTamozhnya"/>
-      <sheetName val="SPPodpisant"/>
-      <sheetName val="SPPort"/>
-      <sheetName val="SPClientsSell"/>
-      <sheetName val="Б"/>
-      <sheetName val="Суда"/>
-      <sheetName val="Продавец"/>
-      <sheetName val="Вид операции"/>
-      <sheetName val="Продукция"/>
-      <sheetName val="Движение ИНВОЙСЫ новое"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4">
-        <row r="2">
-          <cell r="O2" t="str">
-            <v>BNWE-52T</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9">
-        <row r="1">
-          <cell r="AC1" t="str">
-            <v>РШ "Харбиз"</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="U35">
-            <v>59</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36" t="str">
-            <v/>
-          </cell>
-          <cell r="O36" t="e">
-            <v>#VALUE!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v/>
-          </cell>
-          <cell r="B1" t="str">
-            <v/>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="M2" t="str">
-            <v/>
-          </cell>
-          <cell r="N2" t="str">
-            <v/>
-          </cell>
-          <cell r="P2" t="str">
-            <v/>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>ТРК</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>МСИ</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1634,10 +1435,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FEBAA7-C719-4E24-ABD3-2BE3A9A1FFF7}">
-  <dimension ref="A1:E56"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="154" zoomScaleNormal="157" zoomScaleSheetLayoutView="154" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="154" zoomScaleNormal="157" zoomScaleSheetLayoutView="154" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1650,13 +1454,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="50.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="70"/>
@@ -1666,13 +1470,13 @@
       <c r="E2" s="70"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="72" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
+      <c r="A3" s="80" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="51" t="s">
@@ -1684,110 +1488,110 @@
       <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="54"/>
     </row>
     <row r="7" spans="1:5" s="50" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
       <c r="E7" s="55"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="56"/>
     </row>
     <row r="10" spans="1:5" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
     </row>
     <row r="11" spans="1:5" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="76"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
     </row>
     <row r="12" spans="1:5" s="50" customFormat="1" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
     </row>
     <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="76" t="s">
-        <v>113</v>
-      </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
+      <c r="A13" s="73" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="52" t="s">
@@ -1908,319 +1712,289 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="58"/>
       <c r="B24" s="60"/>
       <c r="C24" s="60"/>
       <c r="D24" s="58"/>
       <c r="E24" s="58"/>
     </row>
-    <row r="25" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="79" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-    </row>
-    <row r="26" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="57" t="s">
+    <row r="25" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="57" t="s">
         <v>111</v>
       </c>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+    </row>
+    <row r="26" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="57"/>
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
     </row>
-    <row r="27" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="57"/>
+    <row r="27" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="57" t="s">
+        <v>80</v>
+      </c>
       <c r="B27" s="51"/>
       <c r="C27" s="51"/>
       <c r="D27" s="51"/>
       <c r="E27" s="51"/>
     </row>
-    <row r="28" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="57" t="s">
-        <v>80</v>
+    <row r="28" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="51" t="s">
+        <v>81</v>
       </c>
       <c r="B28" s="51"/>
       <c r="C28" s="51"/>
       <c r="D28" s="51"/>
       <c r="E28" s="51"/>
     </row>
-    <row r="29" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="51" t="s">
-        <v>81</v>
-      </c>
+    <row r="29" spans="1:5" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="57"/>
       <c r="B29" s="51"/>
       <c r="C29" s="51"/>
       <c r="D29" s="51"/>
       <c r="E29" s="51"/>
     </row>
-    <row r="30" spans="1:5" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="57"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-    </row>
-    <row r="31" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="73" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" s="73"/>
       <c r="C31" s="73"/>
       <c r="D31" s="73"/>
       <c r="E31" s="73"/>
     </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="76" t="s">
-        <v>29</v>
-      </c>
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="76"/>
       <c r="B32" s="76"/>
       <c r="C32" s="76"/>
       <c r="D32" s="76"/>
       <c r="E32" s="76"/>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="77"/>
-      <c r="B33" s="77"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-    </row>
-    <row r="34" spans="1:5" s="50" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="68" t="s">
+    <row r="33" spans="1:5" s="50" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="69"/>
-    </row>
-    <row r="35" spans="1:5" s="3" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="78" t="s">
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="69"/>
+    </row>
+    <row r="34" spans="1:5" s="3" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="78"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+    </row>
+    <row r="35" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-    </row>
-    <row r="36" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="76" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" s="76"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-    </row>
-    <row r="37" spans="1:5" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="64"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-    </row>
-    <row r="38" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="74" t="s">
+      <c r="B35" s="73"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+    </row>
+    <row r="36" spans="1:5" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="64"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+    </row>
+    <row r="37" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="74"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-    </row>
-    <row r="39" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="75" t="s">
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+    </row>
+    <row r="38" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="75"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="75"/>
-      <c r="E39" s="75"/>
-    </row>
-    <row r="40" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="76" t="s">
+      <c r="B38" s="77"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+    </row>
+    <row r="39" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="76"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="67"/>
-    </row>
-    <row r="41" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="79" t="s">
+      <c r="B39" s="73"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="67"/>
+    </row>
+    <row r="40" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="79"/>
-      <c r="C41" s="79"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="79"/>
-    </row>
-    <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="79" t="s">
+      <c r="B40" s="71"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+    </row>
+    <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="79"/>
-      <c r="C42" s="79"/>
-      <c r="D42" s="79"/>
-      <c r="E42" s="79"/>
-    </row>
-    <row r="43" spans="1:5" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="76" t="s">
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+    </row>
+    <row r="42" spans="1:5" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="76"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="67"/>
-    </row>
-    <row r="44" spans="1:5" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="79" t="s">
+      <c r="B42" s="73"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="67"/>
+    </row>
+    <row r="43" spans="1:5" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="79"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="79"/>
-      <c r="E44" s="79"/>
-    </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="64"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
+      <c r="B43" s="71"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+    </row>
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="64"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+    </row>
+    <row r="45" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="63"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
       <c r="E45" s="64"/>
     </row>
-    <row r="46" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="63" t="s">
-        <v>36</v>
-      </c>
-      <c r="B46" s="63"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="64"/>
+    <row r="46" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="77"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="77"/>
+      <c r="E46" s="77"/>
     </row>
     <row r="47" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="75" t="s">
-        <v>37</v>
-      </c>
-      <c r="B47" s="75"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
+      <c r="A47" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="71"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
     </row>
     <row r="48" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="79" t="s">
-        <v>38</v>
-      </c>
-      <c r="B48" s="79"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="79"/>
-      <c r="E48" s="79"/>
+      <c r="A48" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="71"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="71"/>
     </row>
     <row r="49" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="79" t="s">
-        <v>41</v>
-      </c>
-      <c r="B49" s="79"/>
-      <c r="C49" s="79"/>
-      <c r="D49" s="79"/>
-      <c r="E49" s="79"/>
+      <c r="A49" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="71"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="71"/>
     </row>
     <row r="50" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="79" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" s="79"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="79"/>
-    </row>
-    <row r="51" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="79" t="s">
+      <c r="A50" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="79"/>
-      <c r="C51" s="79"/>
-      <c r="D51" s="79"/>
-      <c r="E51" s="79"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B50" s="71"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="71"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51" s="51"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+    </row>
+    <row r="52" spans="1:5" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="51"/>
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
     </row>
-    <row r="53" spans="1:5" ht="87.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="51"/>
-      <c r="B53" s="51"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51"/>
-    </row>
-    <row r="54" spans="1:5" ht="98.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="64" t="s">
+    <row r="53" spans="1:5" ht="98.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="64" t="s">
+      <c r="B53" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="64"/>
-      <c r="D54" s="64"/>
-      <c r="E54" s="64"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A55" s="82" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="82"/>
-      <c r="C55" s="65"/>
-      <c r="D55" s="82" t="s">
-        <v>116</v>
-      </c>
-      <c r="E55" s="82"/>
-    </row>
-    <row r="56" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="80" t="s">
+      <c r="C53" s="64"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="64"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54" s="109" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" s="109"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="109" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="109"/>
+    </row>
+    <row r="55" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="80"/>
-      <c r="C56" s="66"/>
-      <c r="D56" s="80" t="s">
+      <c r="B55" s="108"/>
+      <c r="C55" s="66"/>
+      <c r="D55" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="E56" s="80"/>
+      <c r="E55" s="108"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A51:E51"/>
+  <mergeCells count="31">
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A34:E34"/>
     <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A39:E39"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A5:E5"/>
@@ -2233,12 +2007,28 @@
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A37:E37"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="92" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="93" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="29" max="4" man="1"/>
+    <brk id="28" max="4" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -2277,15 +2067,15 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
     </row>
     <row r="3" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="32" t="s">
@@ -2293,15 +2083,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="53.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
     </row>
     <row r="5" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="33"/>
@@ -2350,12 +2140,12 @@
       <c r="A11" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
     </row>
     <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="19"/>
@@ -2375,7 +2165,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F13" s="40" t="s">
         <v>97</v>
@@ -2450,23 +2240,23 @@
       <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="92" t="s">
+      <c r="A19" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="92"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
-      <c r="G19" s="92"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="22"/>
       <c r="B20" s="26"/>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="87"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="47" t="s">
@@ -2483,53 +2273,53 @@
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D22" s="88"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
     </row>
     <row r="23" spans="1:7" s="17" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="89" t="s">
+      <c r="A23" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="89"/>
-      <c r="C23" s="89"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="87"/>
     </row>
     <row r="24" spans="1:7" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="90"/>
-      <c r="C24" s="90"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
     </row>
     <row r="25" spans="1:7" s="17" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="83" t="s">
+      <c r="A25" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
     </row>
     <row r="26" spans="1:7" s="17" customFormat="1" ht="29.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="90" t="s">
+      <c r="A26" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="90"/>
-      <c r="C26" s="90"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="88"/>
     </row>
     <row r="27" spans="1:7" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="90" t="s">
+      <c r="A27" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="90"/>
-      <c r="C27" s="90"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="88"/>
       <c r="D27" s="30"/>
     </row>
     <row r="28" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="83" t="s">
+      <c r="A28" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="83"/>
-      <c r="C28" s="83"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="81"/>
       <c r="D28" s="29"/>
       <c r="F28" s="27"/>
       <c r="G28" s="17"/>
@@ -2554,11 +2344,11 @@
       <c r="G36" s="17"/>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E37" s="84" t="s">
+      <c r="E37" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F37" s="84"/>
-      <c r="G37" s="84"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2600,146 +2390,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
     </row>
     <row r="2" spans="1:5" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
     </row>
     <row r="5" spans="1:5" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="102"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="93"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="104"/>
-      <c r="C9" s="104"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="104"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
     </row>
     <row r="11" spans="1:5" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="103"/>
-      <c r="B11" s="103"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="97" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="94"/>
+      <c r="B12" s="97"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="97"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
+      <c r="B14" s="97"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
+      <c r="B15" s="97"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="94" t="s">
+      <c r="A16" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="94"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="97"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
@@ -2868,31 +2658,31 @@
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="94"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="94"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="97"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="94" t="s">
+      <c r="A26" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="94"/>
-      <c r="C26" s="94"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="94"/>
+      <c r="B26" s="97"/>
+      <c r="C26" s="97"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="97"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="94" t="s">
+      <c r="A27" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
+      <c r="B27" s="97"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
@@ -3021,31 +2811,31 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="94" t="s">
+      <c r="A36" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="94"/>
-      <c r="C36" s="94"/>
-      <c r="D36" s="94"/>
-      <c r="E36" s="94"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="97"/>
+      <c r="D36" s="97"/>
+      <c r="E36" s="97"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="94"/>
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="94"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="97"/>
+      <c r="D37" s="97"/>
+      <c r="E37" s="97"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="94" t="s">
+      <c r="A38" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="94"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="94"/>
+      <c r="B38" s="97"/>
+      <c r="C38" s="97"/>
+      <c r="D38" s="97"/>
+      <c r="E38" s="97"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
@@ -3174,13 +2964,13 @@
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="93" t="s">
+      <c r="A47" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="93"/>
-      <c r="C47" s="93"/>
-      <c r="D47" s="93"/>
-      <c r="E47" s="93"/>
+      <c r="B47" s="94"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="94"/>
+      <c r="E47" s="94"/>
     </row>
     <row r="48" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
@@ -3217,29 +3007,29 @@
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" s="102" t="s">
+      <c r="A52" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="102"/>
-      <c r="C52" s="102"/>
-      <c r="D52" s="102"/>
-      <c r="E52" s="102"/>
+      <c r="B52" s="95"/>
+      <c r="C52" s="95"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="95"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53" s="103" t="s">
+      <c r="A53" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="103"/>
-      <c r="C53" s="103"/>
-      <c r="D53" s="103"/>
-      <c r="E53" s="103"/>
+      <c r="B53" s="98"/>
+      <c r="C53" s="98"/>
+      <c r="D53" s="98"/>
+      <c r="E53" s="98"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="95"/>
-      <c r="B54" s="95"/>
-      <c r="C54" s="95"/>
-      <c r="D54" s="95"/>
-      <c r="E54" s="95"/>
+      <c r="A54" s="104"/>
+      <c r="B54" s="104"/>
+      <c r="C54" s="104"/>
+      <c r="D54" s="104"/>
+      <c r="E54" s="104"/>
     </row>
     <row r="55" spans="1:5" s="3" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
@@ -3250,13 +3040,13 @@
       <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="101" t="s">
+      <c r="A56" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="101"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
-      <c r="E56" s="101"/>
+      <c r="B56" s="105"/>
+      <c r="C56" s="105"/>
+      <c r="D56" s="105"/>
+      <c r="E56" s="105"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
@@ -3267,167 +3057,149 @@
       <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" s="93" t="s">
+      <c r="A59" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="93"/>
-      <c r="C59" s="93"/>
-      <c r="D59" s="93"/>
-      <c r="E59" s="93"/>
+      <c r="B59" s="94"/>
+      <c r="C59" s="94"/>
+      <c r="D59" s="94"/>
+      <c r="E59" s="94"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" s="93" t="s">
+      <c r="A60" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="93"/>
-      <c r="C60" s="93"/>
-      <c r="D60" s="93"/>
-      <c r="E60" s="93"/>
+      <c r="B60" s="94"/>
+      <c r="C60" s="94"/>
+      <c r="D60" s="94"/>
+      <c r="E60" s="94"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" s="93" t="s">
+      <c r="A61" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B61" s="93"/>
-      <c r="C61" s="93"/>
-      <c r="D61" s="93"/>
-      <c r="E61" s="93"/>
+      <c r="B61" s="94"/>
+      <c r="C61" s="94"/>
+      <c r="D61" s="94"/>
+      <c r="E61" s="94"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A62" s="93" t="s">
+      <c r="A62" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B62" s="93"/>
-      <c r="C62" s="93"/>
-      <c r="D62" s="93"/>
-      <c r="E62" s="93"/>
+      <c r="B62" s="94"/>
+      <c r="C62" s="94"/>
+      <c r="D62" s="94"/>
+      <c r="E62" s="94"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A63" s="93" t="s">
+      <c r="A63" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="93"/>
-      <c r="C63" s="93"/>
-      <c r="D63" s="93"/>
-      <c r="E63" s="93"/>
+      <c r="B63" s="94"/>
+      <c r="C63" s="94"/>
+      <c r="D63" s="94"/>
+      <c r="E63" s="94"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A64" s="95"/>
-      <c r="B64" s="95"/>
-      <c r="C64" s="95"/>
-      <c r="D64" s="95"/>
-      <c r="E64" s="95"/>
+      <c r="A64" s="104"/>
+      <c r="B64" s="104"/>
+      <c r="C64" s="104"/>
+      <c r="D64" s="104"/>
+      <c r="E64" s="104"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A65" s="94" t="s">
+      <c r="A65" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="94"/>
-      <c r="C65" s="94"/>
-      <c r="D65" s="94"/>
-      <c r="E65" s="94"/>
+      <c r="B65" s="97"/>
+      <c r="C65" s="97"/>
+      <c r="D65" s="97"/>
+      <c r="E65" s="97"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A66" s="94" t="s">
+      <c r="A66" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="94"/>
-      <c r="C66" s="94"/>
-      <c r="D66" s="94"/>
-      <c r="E66" s="94"/>
+      <c r="B66" s="97"/>
+      <c r="C66" s="97"/>
+      <c r="D66" s="97"/>
+      <c r="E66" s="97"/>
     </row>
     <row r="67" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="96" t="s">
+      <c r="A67" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="96"/>
-      <c r="C67" s="96"/>
-      <c r="D67" s="96"/>
-      <c r="E67" s="96"/>
+      <c r="B67" s="99"/>
+      <c r="C67" s="99"/>
+      <c r="D67" s="99"/>
+      <c r="E67" s="99"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A68" s="94" t="s">
+      <c r="A68" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="94"/>
-      <c r="C68" s="94"/>
-      <c r="D68" s="94"/>
-      <c r="E68" s="94"/>
+      <c r="B68" s="97"/>
+      <c r="C68" s="97"/>
+      <c r="D68" s="97"/>
+      <c r="E68" s="97"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A69" s="94" t="s">
+      <c r="A69" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="94"/>
-      <c r="C69" s="94"/>
-      <c r="D69" s="94"/>
-      <c r="E69" s="94"/>
+      <c r="B69" s="97"/>
+      <c r="C69" s="97"/>
+      <c r="D69" s="97"/>
+      <c r="E69" s="97"/>
     </row>
     <row r="70" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="96" t="s">
+      <c r="A70" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="96"/>
-      <c r="C70" s="96"/>
-      <c r="D70" s="96"/>
-      <c r="E70" s="96"/>
+      <c r="B70" s="99"/>
+      <c r="C70" s="99"/>
+      <c r="D70" s="99"/>
+      <c r="E70" s="99"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A71" s="94" t="s">
+      <c r="A71" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="B71" s="94"/>
-      <c r="C71" s="94"/>
-      <c r="D71" s="94"/>
-      <c r="E71" s="94"/>
+      <c r="B71" s="97"/>
+      <c r="C71" s="97"/>
+      <c r="D71" s="97"/>
+      <c r="E71" s="97"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A82" s="100" t="s">
+      <c r="A82" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="100"/>
+      <c r="B82" s="103"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="98" t="s">
+      <c r="D82" s="101" t="s">
         <v>58</v>
       </c>
-      <c r="E82" s="98"/>
+      <c r="E82" s="101"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A83" s="99" t="s">
+      <c r="A83" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="99"/>
+      <c r="B83" s="102"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="97" t="s">
+      <c r="D83" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="E83" s="97"/>
+      <c r="E83" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A54:E54"/>
     <mergeCell ref="A69:E69"/>
     <mergeCell ref="A70:E70"/>
     <mergeCell ref="A71:E71"/>
@@ -3444,11 +3216,29 @@
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -3473,108 +3263,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
+      <c r="B1" s="92"/>
     </row>
     <row r="2" spans="1:2" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="106"/>
+      <c r="B2" s="93"/>
     </row>
     <row r="3" spans="1:2" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="109"/>
+      <c r="B3" s="106"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="102"/>
+      <c r="B4" s="95"/>
     </row>
     <row r="5" spans="1:2" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="107"/>
+      <c r="B5" s="96"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="104"/>
+      <c r="B6" s="91"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="102"/>
+      <c r="B7" s="95"/>
     </row>
     <row r="8" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="93"/>
+      <c r="B8" s="94"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="104"/>
+      <c r="B9" s="91"/>
     </row>
     <row r="10" spans="1:2" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="103"/>
+      <c r="B10" s="98"/>
     </row>
     <row r="11" spans="1:2" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="103"/>
-      <c r="B11" s="103"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="98"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="94"/>
+      <c r="B12" s="97"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="93"/>
+      <c r="B13" s="94"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="95"/>
-      <c r="B14" s="95"/>
+      <c r="A14" s="104"/>
+      <c r="B14" s="104"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="94"/>
+      <c r="B15" s="97"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="93"/>
+      <c r="B16" s="94"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="93"/>
+      <c r="B17" s="94"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="93" t="s">
+      <c r="A18" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="93"/>
+      <c r="B18" s="94"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
@@ -3628,30 +3418,30 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="95"/>
-      <c r="B29" s="95"/>
+      <c r="A29" s="104"/>
+      <c r="B29" s="104"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="102" t="s">
+      <c r="A30" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="102"/>
+      <c r="B30" s="95"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="103"/>
+      <c r="B31" s="98"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="95"/>
-      <c r="B32" s="95"/>
+      <c r="A32" s="104"/>
+      <c r="B32" s="104"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="94" t="s">
+      <c r="A33" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="94"/>
+      <c r="B33" s="97"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
@@ -3659,10 +3449,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="108" t="s">
+      <c r="A35" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="108"/>
+      <c r="B35" s="107"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
@@ -3670,8 +3460,8 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="95"/>
-      <c r="B37" s="95"/>
+      <c r="A37" s="104"/>
+      <c r="B37" s="104"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
@@ -3679,10 +3469,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="103" t="s">
+      <c r="A39" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="103"/>
+      <c r="B39" s="98"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
@@ -3695,16 +3485,16 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="93" t="s">
+      <c r="A43" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="93"/>
+      <c r="B43" s="94"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="93" t="s">
+      <c r="A44" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="93"/>
+      <c r="B44" s="94"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
@@ -3713,110 +3503,110 @@
       <c r="B45" s="14"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="93" t="s">
+      <c r="A46" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="93"/>
+      <c r="B46" s="94"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" s="93" t="s">
+      <c r="A47" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="93"/>
+      <c r="B47" s="94"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" s="93" t="s">
+      <c r="A48" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="93"/>
+      <c r="B48" s="94"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" s="93" t="s">
+      <c r="A49" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="93"/>
+      <c r="B49" s="94"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" s="93" t="s">
+      <c r="A50" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="93"/>
+      <c r="B50" s="94"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="93" t="s">
+      <c r="A51" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="93"/>
+      <c r="B51" s="94"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" s="93" t="s">
+      <c r="A52" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="93"/>
+      <c r="B52" s="94"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="93" t="s">
+      <c r="A53" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="93"/>
+      <c r="B53" s="94"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" s="93" t="s">
+      <c r="A54" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="93"/>
+      <c r="B54" s="94"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" s="93" t="s">
+      <c r="A55" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="93"/>
+      <c r="B55" s="94"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" s="95"/>
-      <c r="B56" s="95"/>
+      <c r="A56" s="104"/>
+      <c r="B56" s="104"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" s="94" t="s">
+      <c r="A57" s="97" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="94"/>
+      <c r="B57" s="97"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" s="94" t="s">
+      <c r="A58" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="94"/>
+      <c r="B58" s="97"/>
     </row>
     <row r="59" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="96" t="s">
+      <c r="A59" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="96"/>
+      <c r="B59" s="99"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" s="94" t="s">
+      <c r="A60" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="94"/>
+      <c r="B60" s="97"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" s="94" t="s">
+      <c r="A61" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="94"/>
+      <c r="B61" s="97"/>
     </row>
     <row r="62" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="96" t="s">
+      <c r="A62" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="96"/>
+      <c r="B62" s="99"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" s="94" t="s">
+      <c r="A63" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="94"/>
+      <c r="B63" s="97"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
@@ -3836,20 +3626,22 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A30:B30"/>
@@ -3866,22 +3658,20 @@
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
working on sales invoice tmp, added noRouteMatchFileName error handling
</commit_message>
<xml_diff>
--- a/templates/Sales_Purchase_Contract.xlsx
+++ b/templates/Sales_Purchase_Contract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED51279F-C366-4839-B161-6812D78C9724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F28E975-4B7A-44FC-96C4-E0C6447E11E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" activeTab="1" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales_Contract" sheetId="4" r:id="rId1"/>
@@ -926,36 +926,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -987,6 +993,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -996,52 +1035,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1440,8 +1440,8 @@
   </sheetPr>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="154" zoomScaleNormal="157" zoomScaleSheetLayoutView="154" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E14"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A9" zoomScale="154" zoomScaleNormal="157" zoomScaleSheetLayoutView="154" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1454,13 +1454,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="50.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="70"/>
@@ -1470,13 +1470,13 @@
       <c r="E2" s="70"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="51" t="s">
@@ -1488,110 +1488,110 @@
       <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
       <c r="E6" s="54"/>
     </row>
     <row r="7" spans="1:5" s="50" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
       <c r="E7" s="55"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-    </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="73" t="s">
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
       <c r="E9" s="56"/>
     </row>
     <row r="10" spans="1:5" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
     </row>
     <row r="11" spans="1:5" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="73"/>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
+      <c r="A11" s="78"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
     </row>
     <row r="12" spans="1:5" s="50" customFormat="1" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
     </row>
     <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="75" t="s">
+      <c r="A15" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="75" t="s">
+      <c r="A16" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="52" t="s">
@@ -1761,29 +1761,29 @@
       <c r="E29" s="51"/>
     </row>
     <row r="30" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="72" t="s">
+      <c r="A30" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="73" t="s">
+      <c r="A31" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="76"/>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
+      <c r="A32" s="80"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
     </row>
     <row r="33" spans="1:5" s="50" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="68" t="s">
@@ -1795,22 +1795,22 @@
       <c r="E33" s="69"/>
     </row>
     <row r="34" spans="1:5" s="3" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="78" t="s">
+      <c r="A34" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
     </row>
     <row r="35" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="73" t="s">
+      <c r="A35" s="78" t="s">
         <v>114</v>
       </c>
-      <c r="B35" s="73"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
     </row>
     <row r="36" spans="1:5" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="64"/>
@@ -1820,67 +1820,67 @@
       <c r="E36" s="64"/>
     </row>
     <row r="37" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="75" t="s">
+      <c r="A37" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
+      <c r="B37" s="79"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
     </row>
     <row r="38" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="77" t="s">
+      <c r="A38" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="77"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
     </row>
     <row r="39" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="73" t="s">
+      <c r="A39" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="73"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
       <c r="E39" s="67"/>
     </row>
     <row r="40" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="71" t="s">
+      <c r="A40" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="71"/>
-      <c r="C40" s="71"/>
-      <c r="D40" s="71"/>
-      <c r="E40" s="71"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
     </row>
     <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="71" t="s">
+      <c r="A41" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="71"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
     </row>
     <row r="42" spans="1:5" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="73" t="s">
+      <c r="A42" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="73"/>
-      <c r="C42" s="73"/>
-      <c r="D42" s="73"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="78"/>
+      <c r="D42" s="78"/>
       <c r="E42" s="67"/>
     </row>
     <row r="43" spans="1:5" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="71" t="s">
+      <c r="A43" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="71"/>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="81"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="81"/>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="64"/>
@@ -1899,49 +1899,49 @@
       <c r="E45" s="64"/>
     </row>
     <row r="46" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="77" t="s">
+      <c r="A46" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="77"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="77"/>
-      <c r="E46" s="77"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
     </row>
     <row r="47" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="71" t="s">
+      <c r="A47" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="71"/>
-      <c r="C47" s="71"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="81"/>
     </row>
     <row r="48" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="71" t="s">
+      <c r="A48" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="71"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="81"/>
     </row>
     <row r="49" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="71" t="s">
+      <c r="A49" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="71"/>
-      <c r="C49" s="71"/>
-      <c r="D49" s="71"/>
-      <c r="E49" s="71"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
     </row>
     <row r="50" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="71" t="s">
+      <c r="A50" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="71"/>
-      <c r="C50" s="71"/>
-      <c r="D50" s="71"/>
-      <c r="E50" s="71"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="81"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="51"/>
@@ -1969,29 +1969,44 @@
       <c r="E53" s="64"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="109" t="s">
+      <c r="A54" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="109"/>
+      <c r="B54" s="72"/>
       <c r="C54" s="65"/>
-      <c r="D54" s="109" t="s">
+      <c r="D54" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="E54" s="109"/>
+      <c r="E54" s="72"/>
     </row>
     <row r="55" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="108" t="s">
+      <c r="A55" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="108"/>
+      <c r="B55" s="71"/>
       <c r="C55" s="66"/>
-      <c r="D55" s="108" t="s">
+      <c r="D55" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="108"/>
+      <c r="E55" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A30:E30"/>
     <mergeCell ref="A46:E46"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="A38:E38"/>
@@ -2008,21 +2023,6 @@
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A37:E37"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -2040,8 +2040,8 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2067,15 +2067,15 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
     </row>
     <row r="3" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="32" t="s">
@@ -2083,15 +2083,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="53.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
     </row>
     <row r="5" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="33"/>
@@ -2140,12 +2140,12 @@
       <c r="A11" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
     </row>
     <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="19"/>
@@ -2240,23 +2240,23 @@
       <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="90"/>
-      <c r="C19" s="90"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="90"/>
-      <c r="G19" s="90"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="22"/>
       <c r="B20" s="26"/>
-      <c r="C20" s="85" t="s">
+      <c r="C20" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="85"/>
+      <c r="D20" s="87"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="47" t="s">
@@ -2273,53 +2273,53 @@
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
+      <c r="G22" s="88"/>
     </row>
     <row r="23" spans="1:7" s="17" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="87" t="s">
+      <c r="A23" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="87"/>
-      <c r="C23" s="87"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
     </row>
     <row r="24" spans="1:7" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="88" t="s">
+      <c r="A24" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="88"/>
-      <c r="C24" s="88"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
     </row>
     <row r="25" spans="1:7" s="17" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="81" t="s">
+      <c r="A25" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
     </row>
     <row r="26" spans="1:7" s="17" customFormat="1" ht="29.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="88"/>
-      <c r="C26" s="88"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="90"/>
     </row>
     <row r="27" spans="1:7" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="88" t="s">
+      <c r="A27" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="88"/>
-      <c r="C27" s="88"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="90"/>
       <c r="D27" s="30"/>
     </row>
     <row r="28" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="81" t="s">
+      <c r="A28" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="81"/>
-      <c r="C28" s="81"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="83"/>
       <c r="D28" s="29"/>
       <c r="F28" s="27"/>
       <c r="G28" s="17"/>
@@ -2344,11 +2344,11 @@
       <c r="G36" s="17"/>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E37" s="82" t="s">
+      <c r="E37" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2390,146 +2390,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
     </row>
     <row r="2" spans="1:5" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="95"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
     </row>
     <row r="5" spans="1:5" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="95"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
+      <c r="B8" s="93"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="91"/>
-      <c r="C9" s="91"/>
-      <c r="D9" s="91"/>
-      <c r="E9" s="91"/>
+      <c r="B9" s="104"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
     </row>
     <row r="11" spans="1:5" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="98"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
+      <c r="A11" s="103"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="97" t="s">
+      <c r="A12" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="97"/>
-      <c r="C14" s="97"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="97"/>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="97"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="97"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
@@ -2658,31 +2658,31 @@
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="97" t="s">
+      <c r="A25" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="97"/>
-      <c r="C25" s="97"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="97"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="97" t="s">
+      <c r="A26" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="97"/>
-      <c r="C26" s="97"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="97"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
+      <c r="E26" s="94"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="97" t="s">
+      <c r="A27" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="97"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
@@ -2811,31 +2811,31 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="97" t="s">
+      <c r="A36" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="97"/>
-      <c r="C36" s="97"/>
-      <c r="D36" s="97"/>
-      <c r="E36" s="97"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="94"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="97" t="s">
+      <c r="A37" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="97"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="97"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="97" t="s">
+      <c r="A38" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="97"/>
-      <c r="C38" s="97"/>
-      <c r="D38" s="97"/>
-      <c r="E38" s="97"/>
+      <c r="B38" s="94"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="94"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
@@ -2964,13 +2964,13 @@
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="94" t="s">
+      <c r="A47" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="94"/>
-      <c r="C47" s="94"/>
-      <c r="D47" s="94"/>
-      <c r="E47" s="94"/>
+      <c r="B47" s="93"/>
+      <c r="C47" s="93"/>
+      <c r="D47" s="93"/>
+      <c r="E47" s="93"/>
     </row>
     <row r="48" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
@@ -3007,29 +3007,29 @@
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" s="95" t="s">
+      <c r="A52" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="95"/>
-      <c r="C52" s="95"/>
-      <c r="D52" s="95"/>
-      <c r="E52" s="95"/>
+      <c r="B52" s="102"/>
+      <c r="C52" s="102"/>
+      <c r="D52" s="102"/>
+      <c r="E52" s="102"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53" s="98" t="s">
+      <c r="A53" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="98"/>
-      <c r="C53" s="98"/>
-      <c r="D53" s="98"/>
-      <c r="E53" s="98"/>
+      <c r="B53" s="103"/>
+      <c r="C53" s="103"/>
+      <c r="D53" s="103"/>
+      <c r="E53" s="103"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="104"/>
-      <c r="B54" s="104"/>
-      <c r="C54" s="104"/>
-      <c r="D54" s="104"/>
-      <c r="E54" s="104"/>
+      <c r="A54" s="95"/>
+      <c r="B54" s="95"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="95"/>
+      <c r="E54" s="95"/>
     </row>
     <row r="55" spans="1:5" s="3" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
@@ -3040,13 +3040,13 @@
       <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="105" t="s">
+      <c r="A56" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="105"/>
-      <c r="C56" s="105"/>
-      <c r="D56" s="105"/>
-      <c r="E56" s="105"/>
+      <c r="B56" s="101"/>
+      <c r="C56" s="101"/>
+      <c r="D56" s="101"/>
+      <c r="E56" s="101"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
@@ -3057,149 +3057,167 @@
       <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" s="94" t="s">
+      <c r="A59" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="94"/>
-      <c r="C59" s="94"/>
-      <c r="D59" s="94"/>
-      <c r="E59" s="94"/>
+      <c r="B59" s="93"/>
+      <c r="C59" s="93"/>
+      <c r="D59" s="93"/>
+      <c r="E59" s="93"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" s="94" t="s">
+      <c r="A60" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="94"/>
-      <c r="C60" s="94"/>
-      <c r="D60" s="94"/>
-      <c r="E60" s="94"/>
+      <c r="B60" s="93"/>
+      <c r="C60" s="93"/>
+      <c r="D60" s="93"/>
+      <c r="E60" s="93"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" s="94" t="s">
+      <c r="A61" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="B61" s="94"/>
-      <c r="C61" s="94"/>
-      <c r="D61" s="94"/>
-      <c r="E61" s="94"/>
+      <c r="B61" s="93"/>
+      <c r="C61" s="93"/>
+      <c r="D61" s="93"/>
+      <c r="E61" s="93"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A62" s="94" t="s">
+      <c r="A62" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="B62" s="94"/>
-      <c r="C62" s="94"/>
-      <c r="D62" s="94"/>
-      <c r="E62" s="94"/>
+      <c r="B62" s="93"/>
+      <c r="C62" s="93"/>
+      <c r="D62" s="93"/>
+      <c r="E62" s="93"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A63" s="94" t="s">
+      <c r="A63" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="94"/>
-      <c r="C63" s="94"/>
-      <c r="D63" s="94"/>
-      <c r="E63" s="94"/>
+      <c r="B63" s="93"/>
+      <c r="C63" s="93"/>
+      <c r="D63" s="93"/>
+      <c r="E63" s="93"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A64" s="104"/>
-      <c r="B64" s="104"/>
-      <c r="C64" s="104"/>
-      <c r="D64" s="104"/>
-      <c r="E64" s="104"/>
+      <c r="A64" s="95"/>
+      <c r="B64" s="95"/>
+      <c r="C64" s="95"/>
+      <c r="D64" s="95"/>
+      <c r="E64" s="95"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A65" s="97" t="s">
+      <c r="A65" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="97"/>
-      <c r="C65" s="97"/>
-      <c r="D65" s="97"/>
-      <c r="E65" s="97"/>
+      <c r="B65" s="94"/>
+      <c r="C65" s="94"/>
+      <c r="D65" s="94"/>
+      <c r="E65" s="94"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A66" s="97" t="s">
+      <c r="A66" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="97"/>
-      <c r="C66" s="97"/>
-      <c r="D66" s="97"/>
-      <c r="E66" s="97"/>
+      <c r="B66" s="94"/>
+      <c r="C66" s="94"/>
+      <c r="D66" s="94"/>
+      <c r="E66" s="94"/>
     </row>
     <row r="67" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="99" t="s">
+      <c r="A67" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="99"/>
-      <c r="C67" s="99"/>
-      <c r="D67" s="99"/>
-      <c r="E67" s="99"/>
+      <c r="B67" s="96"/>
+      <c r="C67" s="96"/>
+      <c r="D67" s="96"/>
+      <c r="E67" s="96"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A68" s="97" t="s">
+      <c r="A68" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="97"/>
-      <c r="C68" s="97"/>
-      <c r="D68" s="97"/>
-      <c r="E68" s="97"/>
+      <c r="B68" s="94"/>
+      <c r="C68" s="94"/>
+      <c r="D68" s="94"/>
+      <c r="E68" s="94"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A69" s="97" t="s">
+      <c r="A69" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="97"/>
-      <c r="C69" s="97"/>
-      <c r="D69" s="97"/>
-      <c r="E69" s="97"/>
+      <c r="B69" s="94"/>
+      <c r="C69" s="94"/>
+      <c r="D69" s="94"/>
+      <c r="E69" s="94"/>
     </row>
     <row r="70" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="99" t="s">
+      <c r="A70" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="99"/>
-      <c r="C70" s="99"/>
-      <c r="D70" s="99"/>
-      <c r="E70" s="99"/>
+      <c r="B70" s="96"/>
+      <c r="C70" s="96"/>
+      <c r="D70" s="96"/>
+      <c r="E70" s="96"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A71" s="97" t="s">
+      <c r="A71" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="B71" s="97"/>
-      <c r="C71" s="97"/>
-      <c r="D71" s="97"/>
-      <c r="E71" s="97"/>
+      <c r="B71" s="94"/>
+      <c r="C71" s="94"/>
+      <c r="D71" s="94"/>
+      <c r="E71" s="94"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A82" s="103" t="s">
+      <c r="A82" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="103"/>
+      <c r="B82" s="100"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="101" t="s">
+      <c r="D82" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="E82" s="101"/>
+      <c r="E82" s="98"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A83" s="102" t="s">
+      <c r="A83" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="102"/>
+      <c r="B83" s="99"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="100" t="s">
+      <c r="D83" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="E83" s="100"/>
+      <c r="E83" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A47:E47"/>
     <mergeCell ref="A69:E69"/>
     <mergeCell ref="A70:E70"/>
     <mergeCell ref="A71:E71"/>
@@ -3216,29 +3234,11 @@
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A54:E54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -3263,108 +3263,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92"/>
+      <c r="B1" s="105"/>
     </row>
     <row r="2" spans="1:2" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="93"/>
+      <c r="B2" s="106"/>
     </row>
     <row r="3" spans="1:2" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="106"/>
+      <c r="B3" s="109"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="95"/>
+      <c r="B4" s="102"/>
     </row>
     <row r="5" spans="1:2" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="96"/>
+      <c r="B5" s="107"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="91"/>
+      <c r="B6" s="104"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="102"/>
     </row>
     <row r="8" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="94"/>
+      <c r="B8" s="93"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="91"/>
+      <c r="B9" s="104"/>
     </row>
     <row r="10" spans="1:2" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="98"/>
+      <c r="B10" s="103"/>
     </row>
     <row r="11" spans="1:2" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="98"/>
-      <c r="B11" s="98"/>
+      <c r="A11" s="103"/>
+      <c r="B11" s="103"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="97" t="s">
+      <c r="A12" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="97"/>
+      <c r="B12" s="94"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="94"/>
+      <c r="B13" s="93"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="104"/>
-      <c r="B14" s="104"/>
+      <c r="A14" s="95"/>
+      <c r="B14" s="95"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="97"/>
+      <c r="B15" s="94"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="94" t="s">
+      <c r="A16" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="94"/>
+      <c r="B16" s="93"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="94" t="s">
+      <c r="A17" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="94"/>
+      <c r="B17" s="93"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="94" t="s">
+      <c r="A18" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="94"/>
+      <c r="B18" s="93"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
@@ -3418,30 +3418,30 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="104"/>
-      <c r="B29" s="104"/>
+      <c r="A29" s="95"/>
+      <c r="B29" s="95"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="95" t="s">
+      <c r="A30" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="95"/>
+      <c r="B30" s="102"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="98" t="s">
+      <c r="A31" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="98"/>
+      <c r="B31" s="103"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="104"/>
-      <c r="B32" s="104"/>
+      <c r="A32" s="95"/>
+      <c r="B32" s="95"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="97" t="s">
+      <c r="A33" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="97"/>
+      <c r="B33" s="94"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
@@ -3449,10 +3449,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="107" t="s">
+      <c r="A35" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="107"/>
+      <c r="B35" s="108"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
@@ -3460,8 +3460,8 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="104"/>
-      <c r="B37" s="104"/>
+      <c r="A37" s="95"/>
+      <c r="B37" s="95"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
@@ -3469,10 +3469,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="98" t="s">
+      <c r="A39" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="98"/>
+      <c r="B39" s="103"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
@@ -3485,16 +3485,16 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="94" t="s">
+      <c r="A43" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="94"/>
+      <c r="B43" s="93"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="94" t="s">
+      <c r="A44" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="94"/>
+      <c r="B44" s="93"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
@@ -3503,110 +3503,110 @@
       <c r="B45" s="14"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="94" t="s">
+      <c r="A46" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="94"/>
+      <c r="B46" s="93"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" s="94" t="s">
+      <c r="A47" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="94"/>
+      <c r="B47" s="93"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" s="94" t="s">
+      <c r="A48" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="94"/>
+      <c r="B48" s="93"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" s="94" t="s">
+      <c r="A49" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="94"/>
+      <c r="B49" s="93"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" s="94" t="s">
+      <c r="A50" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="94"/>
+      <c r="B50" s="93"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="94" t="s">
+      <c r="A51" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="94"/>
+      <c r="B51" s="93"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" s="94" t="s">
+      <c r="A52" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="94"/>
+      <c r="B52" s="93"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="94" t="s">
+      <c r="A53" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="94"/>
+      <c r="B53" s="93"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" s="94" t="s">
+      <c r="A54" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="94"/>
+      <c r="B54" s="93"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" s="94" t="s">
+      <c r="A55" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="94"/>
+      <c r="B55" s="93"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" s="104"/>
-      <c r="B56" s="104"/>
+      <c r="A56" s="95"/>
+      <c r="B56" s="95"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" s="97" t="s">
+      <c r="A57" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="97"/>
+      <c r="B57" s="94"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" s="97" t="s">
+      <c r="A58" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="97"/>
+      <c r="B58" s="94"/>
     </row>
     <row r="59" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="99" t="s">
+      <c r="A59" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="99"/>
+      <c r="B59" s="96"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" s="97" t="s">
+      <c r="A60" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="97"/>
+      <c r="B60" s="94"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" s="97" t="s">
+      <c r="A61" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="97"/>
+      <c r="B61" s="94"/>
     </row>
     <row r="62" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="99" t="s">
+      <c r="A62" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="99"/>
+      <c r="B62" s="96"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" s="97" t="s">
+      <c r="A63" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="97"/>
+      <c r="B63" s="94"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
@@ -3626,6 +3626,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A58:B58"/>
@@ -3642,36 +3672,6 @@
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
beta sales contracts implemented
</commit_message>
<xml_diff>
--- a/templates/Sales_Purchase_Contract.xlsx
+++ b/templates/Sales_Purchase_Contract.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F28E975-4B7A-44FC-96C4-E0C6447E11E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD087B2C-778B-4757-8EA8-E8F667EE5D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" activeTab="1" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
+    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sales_Contract" sheetId="4" r:id="rId1"/>
-    <sheet name="Invoice" sheetId="3" r:id="rId2"/>
+    <sheet name="Invoice" sheetId="5" r:id="rId1"/>
+    <sheet name="Sales_Contract" sheetId="4" r:id="rId2"/>
     <sheet name="Contract" sheetId="2" state="hidden" r:id="rId3"/>
     <sheet name="Contract Old" sheetId="1" state="hidden" r:id="rId4"/>
   </sheets>
@@ -25,10 +25,30 @@
     <definedName name="_Hlk39074976" localSheetId="3">'Contract Old'!$A$18</definedName>
     <definedName name="_Hlk39404391" localSheetId="2">Contract!#REF!</definedName>
     <definedName name="_Hlk39404391" localSheetId="3">'Contract Old'!$A$34</definedName>
+    <definedName name="Invoice_sign_seller_end">Invoice!$G$30</definedName>
+    <definedName name="Invoice_sign_seller_start">Invoice!$E$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Contract!$A$1:$E$83</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$G$32</definedName>
     <definedName name="Sign_seller_end">Sales_Contract!$B$53</definedName>
     <definedName name="Sign_seller_start">Sales_Contract!$A$53</definedName>
     <definedName name="Документация_BL">Sales_Contract!$A$50</definedName>
+    <definedName name="Инвойс_адреса_адрес">Invoice!$A$24</definedName>
+    <definedName name="Инвойс_адреса_банк">Invoice!$A$26</definedName>
+    <definedName name="Инвойс_адреса_банк_адрес">Invoice!$A$27</definedName>
+    <definedName name="Инвойс_адреса_банк_свифт">Invoice!$A$28</definedName>
+    <definedName name="Инвойс_адреса_продавец">Invoice!$A$23</definedName>
+    <definedName name="Инвойс_адреса_счет">Invoice!$A$25</definedName>
+    <definedName name="Инвойс_всего_места">Invoice!$C$20</definedName>
+    <definedName name="Инвойс_всего_цена">Invoice!$G$20</definedName>
+    <definedName name="Инвойс_дата">Invoice!$G$6</definedName>
+    <definedName name="Инвойс_заголовок_продавец">Invoice!$A$1</definedName>
+    <definedName name="Инвойс_заголовок_продавец_адрес">Invoice!$A$2</definedName>
+    <definedName name="Инвойс_номер">Invoice!$G$7</definedName>
+    <definedName name="Инвойс_покупатель">Invoice!$B$8</definedName>
+    <definedName name="Инвойс_предмет_массив">Invoice!$A$14</definedName>
+    <definedName name="Инвойс_продавец">Invoice!$B$9</definedName>
+    <definedName name="Инвойс_продавец_печать_подвал">Invoice!$E$32</definedName>
+    <definedName name="Инвойс_условия_доставки">Invoice!$B$10</definedName>
     <definedName name="Контракт_адреса_банк">Sales_Contract!$A$41</definedName>
     <definedName name="Контракт_адреса_банк_адрес">Sales_Contract!$A$42</definedName>
     <definedName name="Контракт_адреса_банк_свифт">Sales_Contract!$A$43</definedName>
@@ -70,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="119">
   <si>
     <t>SALES AND PURCHASE CONTRACT</t>
   </si>
@@ -371,9 +391,6 @@
     <t>____________________________________________________</t>
   </si>
   <si>
-    <t>______________________________________________________________________________________________________________________</t>
-  </si>
-  <si>
     <t xml:space="preserve">* Payment: </t>
   </si>
   <si>
@@ -474,6 +491,9 @@
   </si>
   <si>
     <t>1.1. The Seller agrees to sell and the Buyer agrees to purchase goods with following in table assortment and condititions:</t>
+  </si>
+  <si>
+    <t>_________________________________________________________________________________________________________________________</t>
   </si>
 </sst>
 </file>
@@ -724,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -813,9 +833,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -932,6 +949,60 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -944,104 +1015,56 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1058,66 +1081,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>76202</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1228725</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>133353</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 3" descr="A close-up of a sign&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{655C0B08-F270-110A-8F1E-4CC2C2CF060F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5305427" y="10510838"/>
-          <a:ext cx="3195636" cy="1190628"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1434,14 +1397,358 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF949AA7-515D-4019-85D4-70C92EC5672B}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScale="127" zoomScaleNormal="100" zoomScaleSheetLayoutView="127" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.9296875" customWidth="1"/>
+    <col min="2" max="2" width="32.53125" customWidth="1"/>
+    <col min="3" max="3" width="19.73046875" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="13.1328125" customWidth="1"/>
+    <col min="6" max="6" width="15.46484375" customWidth="1"/>
+    <col min="7" max="7" width="18.06640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+    </row>
+    <row r="3" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" ht="53.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+    </row>
+    <row r="5" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+    </row>
+    <row r="6" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G6" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G7" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="81" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+    </row>
+    <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+    </row>
+    <row r="13" spans="1:7" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="44">
+        <v>56</v>
+      </c>
+      <c r="F14" s="37">
+        <v>25190</v>
+      </c>
+      <c r="G14" s="45">
+        <v>1410640</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="43"/>
+    </row>
+    <row r="17" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="22"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="75"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="6.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="22"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="1:7" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+    </row>
+    <row r="23" spans="1:7" s="17" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="83"/>
+      <c r="C23" s="83"/>
+    </row>
+    <row r="24" spans="1:7" s="17" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+    </row>
+    <row r="25" spans="1:7" s="17" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+    </row>
+    <row r="26" spans="1:7" s="17" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="78" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
+    </row>
+    <row r="27" spans="1:7" s="17" customFormat="1" ht="36.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="78" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="30"/>
+    </row>
+    <row r="28" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="79"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="29"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:7" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="72"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="29"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="1:7" ht="100.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D30" s="30"/>
+      <c r="E30" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="8.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E31" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="1:7" ht="30.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E32" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FEBAA7-C719-4E24-ABD3-2BE3A9A1FFF7}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A9" zoomScale="154" zoomScaleNormal="157" zoomScaleSheetLayoutView="154" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A35" zoomScale="106" zoomScaleNormal="157" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1454,544 +1761,559 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="50.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="76" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
+      <c r="A3" s="93" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="52"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="51"/>
     </row>
     <row r="5" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="54"/>
-    </row>
-    <row r="7" spans="1:5" s="50" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="82" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="55"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="53"/>
+    </row>
+    <row r="7" spans="1:5" s="49" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="54"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="56"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="55"/>
     </row>
     <row r="10" spans="1:5" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
     </row>
     <row r="11" spans="1:5" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-    </row>
-    <row r="12" spans="1:5" s="50" customFormat="1" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="79" t="s">
+      <c r="A11" s="86"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+    </row>
+    <row r="12" spans="1:5" s="49" customFormat="1" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
     </row>
     <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="78" t="s">
-        <v>118</v>
-      </c>
-      <c r="B13" s="78"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
+      <c r="A13" s="86" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="52" t="s">
+      <c r="C17" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="51" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="58">
+      <c r="B18" s="57">
         <v>931</v>
       </c>
-      <c r="C18" s="59">
+      <c r="C18" s="58">
         <v>18620</v>
       </c>
-      <c r="D18" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="58" t="s">
+      <c r="D18" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="57" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="59">
+        <v>1560</v>
+      </c>
+      <c r="C19" s="58">
+        <v>31200</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="57" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="60">
-        <v>1560</v>
-      </c>
-      <c r="C19" s="59">
-        <v>31200</v>
-      </c>
-      <c r="D19" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" s="58" t="s">
+    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="59">
+        <v>952</v>
+      </c>
+      <c r="C20" s="58">
+        <v>19040</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="57" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="60">
-        <v>952</v>
-      </c>
-      <c r="C20" s="59">
-        <v>19040</v>
-      </c>
-      <c r="D20" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" s="58" t="s">
+    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="59">
+        <v>114</v>
+      </c>
+      <c r="C21" s="58">
+        <v>2280</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="57" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="60">
-        <v>114</v>
-      </c>
-      <c r="C21" s="59">
-        <v>2280</v>
-      </c>
-      <c r="D21" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="58" t="s">
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="59">
+        <v>13</v>
+      </c>
+      <c r="C22" s="58">
+        <v>260</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="57" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="60">
-        <v>13</v>
-      </c>
-      <c r="C22" s="59">
-        <v>260</v>
-      </c>
-      <c r="D22" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" s="58" t="s">
-        <v>108</v>
-      </c>
-    </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="61">
+      <c r="B23" s="60">
         <f>SUM(B18:B22)</f>
         <v>3570</v>
       </c>
-      <c r="C23" s="62">
+      <c r="C23" s="61">
         <f xml:space="preserve"> SUM(C18:C22)</f>
         <v>71400</v>
       </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52" t="s">
-        <v>109</v>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="58"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
     </row>
     <row r="25" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="57" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
+      <c r="A25" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
     </row>
     <row r="26" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="57"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
     </row>
     <row r="27" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
     </row>
     <row r="28" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
     </row>
     <row r="29" spans="1:5" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="57"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
+      <c r="A29" s="56"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
     </row>
     <row r="30" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="77"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="77"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="78" t="s">
+      <c r="A31" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="78"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="80"/>
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-    </row>
-    <row r="33" spans="1:5" s="50" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="68" t="s">
+      <c r="A32" s="88"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="88"/>
+    </row>
+    <row r="33" spans="1:5" s="49" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="69"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="68"/>
     </row>
     <row r="34" spans="1:5" s="3" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="74" t="s">
+      <c r="A34" s="91" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="91"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="91"/>
+      <c r="E34" s="91"/>
+    </row>
+    <row r="35" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="B34" s="74"/>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-    </row>
-    <row r="35" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
     </row>
     <row r="36" spans="1:5" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="64"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
+      <c r="A36" s="63"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
     </row>
     <row r="37" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="79" t="s">
+      <c r="A37" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="79"/>
-      <c r="C37" s="79"/>
-      <c r="D37" s="79"/>
-      <c r="E37" s="79"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="85"/>
     </row>
     <row r="38" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="73" t="s">
+      <c r="A38" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="73"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="90"/>
+      <c r="D38" s="90"/>
+      <c r="E38" s="90"/>
     </row>
     <row r="39" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="78" t="s">
+      <c r="A39" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="78"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="67"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="66"/>
     </row>
     <row r="40" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="81"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="84"/>
     </row>
     <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="81" t="s">
+      <c r="A41" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="81"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
+      <c r="B41" s="84"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="84"/>
     </row>
     <row r="42" spans="1:5" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="78" t="s">
+      <c r="A42" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="78"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="67"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="66"/>
     </row>
     <row r="43" spans="1:5" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="81" t="s">
+      <c r="A43" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="81"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
+      <c r="B43" s="84"/>
+      <c r="C43" s="84"/>
+      <c r="D43" s="84"/>
+      <c r="E43" s="84"/>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="64"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
+      <c r="A44" s="63"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
     </row>
     <row r="45" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="63" t="s">
+      <c r="A45" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="64"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="63"/>
     </row>
     <row r="46" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="73" t="s">
+      <c r="A46" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="73"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
+      <c r="B46" s="90"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="90"/>
     </row>
     <row r="47" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="81" t="s">
+      <c r="A47" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="81"/>
-      <c r="C47" s="81"/>
-      <c r="D47" s="81"/>
-      <c r="E47" s="81"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="84"/>
     </row>
     <row r="48" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="81" t="s">
+      <c r="A48" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="81"/>
-      <c r="C48" s="81"/>
-      <c r="D48" s="81"/>
-      <c r="E48" s="81"/>
+      <c r="B48" s="84"/>
+      <c r="C48" s="84"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="84"/>
     </row>
     <row r="49" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="81"/>
-      <c r="C49" s="81"/>
-      <c r="D49" s="81"/>
-      <c r="E49" s="81"/>
+      <c r="B49" s="84"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="84"/>
     </row>
     <row r="50" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="81" t="s">
+      <c r="A50" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="81"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="81"/>
+      <c r="B50" s="84"/>
+      <c r="C50" s="84"/>
+      <c r="D50" s="84"/>
+      <c r="E50" s="84"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A51" s="51"/>
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
+      <c r="A51" s="50"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
     </row>
     <row r="52" spans="1:5" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="51"/>
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-    </row>
-    <row r="53" spans="1:5" ht="98.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="64" t="s">
+      <c r="A52" s="50"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+    </row>
+    <row r="53" spans="1:5" ht="100.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="64" t="s">
+      <c r="B53" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
+      <c r="C53" s="63"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="63"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="72" t="s">
-        <v>117</v>
-      </c>
-      <c r="B54" s="72"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="72" t="s">
-        <v>117</v>
-      </c>
-      <c r="E54" s="72"/>
+      <c r="A54" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="71"/>
+      <c r="C54" s="64"/>
+      <c r="D54" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="E54" s="71"/>
     </row>
     <row r="55" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="71" t="s">
+      <c r="A55" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="71"/>
-      <c r="C55" s="66"/>
-      <c r="D55" s="71" t="s">
+      <c r="B55" s="70"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="71"/>
+      <c r="E55" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A49:E49"/>
     <mergeCell ref="A50:E50"/>
@@ -2008,21 +2330,6 @@
     <mergeCell ref="A47:E47"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A39:D39"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -2030,345 +2337,6 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="28" max="4" man="1"/>
   </rowBreaks>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53258B38-3BED-4121-92B6-93190B007EF2}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:G37"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="12.9296875" customWidth="1"/>
-    <col min="2" max="2" width="32.53125" customWidth="1"/>
-    <col min="3" max="3" width="19.73046875" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="13.1328125" customWidth="1"/>
-    <col min="6" max="6" width="15.46484375" customWidth="1"/>
-    <col min="7" max="7" width="18.06640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="30.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="85" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-    </row>
-    <row r="3" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="53.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="91" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-    </row>
-    <row r="5" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-    </row>
-    <row r="6" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G6" s="28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G7" s="28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" s="86" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-    </row>
-    <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-    </row>
-    <row r="13" spans="1:7" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="45">
-        <v>56</v>
-      </c>
-      <c r="F14" s="38">
-        <v>25190</v>
-      </c>
-      <c r="G14" s="46">
-        <v>1410640</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
-    </row>
-    <row r="17" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="92" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="92"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
-      <c r="G19" s="92"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="22"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="87" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="87"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="47" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="6.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="22"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="20"/>
-    </row>
-    <row r="22" spans="1:7" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D22" s="88"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
-    </row>
-    <row r="23" spans="1:7" s="17" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="89" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="89"/>
-      <c r="C23" s="89"/>
-    </row>
-    <row r="24" spans="1:7" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="90" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="90"/>
-      <c r="C24" s="90"/>
-    </row>
-    <row r="25" spans="1:7" s="17" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="83" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-    </row>
-    <row r="26" spans="1:7" s="17" customFormat="1" ht="29.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="90"/>
-      <c r="C26" s="90"/>
-    </row>
-    <row r="27" spans="1:7" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="90" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="90"/>
-      <c r="C27" s="90"/>
-      <c r="D27" s="30"/>
-    </row>
-    <row r="28" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="83"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="29"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D29" s="30"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D30" s="30"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D31" s="30"/>
-    </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E36" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-    </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E37" s="84" t="s">
-        <v>3</v>
-      </c>
-      <c r="F37" s="84"/>
-      <c r="G37" s="84"/>
-    </row>
-  </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A19:G19"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2390,146 +2358,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
     </row>
     <row r="2" spans="1:5" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
     </row>
     <row r="5" spans="1:5" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="102"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="93"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="104"/>
-      <c r="C9" s="104"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="104"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="101"/>
     </row>
     <row r="11" spans="1:5" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="103"/>
-      <c r="B11" s="103"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="101"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="101"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="94"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="100"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="100"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="94" t="s">
+      <c r="A16" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="94"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="100"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
@@ -2539,7 +2507,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>62</v>
@@ -2555,14 +2523,14 @@
       <c r="B18" s="6">
         <v>931</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="47">
         <v>18620</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2572,14 +2540,14 @@
       <c r="B19" s="15">
         <v>1560</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C19" s="47">
         <v>31200</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2589,14 +2557,14 @@
       <c r="B20" s="15">
         <v>952</v>
       </c>
-      <c r="C20" s="48">
+      <c r="C20" s="47">
         <v>19040</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2606,14 +2574,14 @@
       <c r="B21" s="15">
         <v>114</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C21" s="47">
         <v>2280</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2623,14 +2591,14 @@
       <c r="B22" s="15">
         <v>13</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="47">
         <v>260</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2641,13 +2609,13 @@
         <f>SUM(B18:B22)</f>
         <v>3570</v>
       </c>
-      <c r="C23" s="49">
+      <c r="C23" s="48">
         <f xml:space="preserve"> SUM(C18:C22)</f>
         <v>71400</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2658,31 +2626,31 @@
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="94"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="94"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="94" t="s">
+      <c r="A26" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="94"/>
-      <c r="C26" s="94"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="94"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="100"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="94" t="s">
+      <c r="A27" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="100"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="100"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
@@ -2692,7 +2660,7 @@
         <v>61</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>62</v>
@@ -2712,10 +2680,10 @@
         <v>18620</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2729,10 +2697,10 @@
         <v>31200</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2746,10 +2714,10 @@
         <v>19040</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2763,10 +2731,10 @@
         <v>2280</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2780,10 +2748,10 @@
         <v>260</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2794,13 +2762,13 @@
         <f>SUM(B29:B33)</f>
         <v>3570</v>
       </c>
-      <c r="C34" s="49">
+      <c r="C34" s="48">
         <f xml:space="preserve"> SUM(C29:C33)</f>
         <v>71400</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2811,31 +2779,31 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="94" t="s">
+      <c r="A36" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="94"/>
-      <c r="C36" s="94"/>
-      <c r="D36" s="94"/>
-      <c r="E36" s="94"/>
+      <c r="B36" s="100"/>
+      <c r="C36" s="100"/>
+      <c r="D36" s="100"/>
+      <c r="E36" s="100"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="94"/>
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="94"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="100"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="94" t="s">
+      <c r="A38" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="94"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="94"/>
+      <c r="B38" s="100"/>
+      <c r="C38" s="100"/>
+      <c r="D38" s="100"/>
+      <c r="E38" s="100"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
@@ -2845,7 +2813,7 @@
         <v>61</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>62</v>
@@ -2865,10 +2833,10 @@
         <v>18620</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2882,10 +2850,10 @@
         <v>31200</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2899,10 +2867,10 @@
         <v>19040</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2916,10 +2884,10 @@
         <v>2280</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -2933,10 +2901,10 @@
         <v>260</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2947,13 +2915,13 @@
         <f>SUM(B40:B44)</f>
         <v>3570</v>
       </c>
-      <c r="C45" s="49">
+      <c r="C45" s="48">
         <f xml:space="preserve"> SUM(C40:C44)</f>
         <v>71400</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -2964,17 +2932,17 @@
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="93" t="s">
+      <c r="A47" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="93"/>
-      <c r="C47" s="93"/>
-      <c r="D47" s="93"/>
-      <c r="E47" s="93"/>
+      <c r="B47" s="97"/>
+      <c r="C47" s="97"/>
+      <c r="D47" s="97"/>
+      <c r="E47" s="97"/>
     </row>
     <row r="48" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -3007,29 +2975,29 @@
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" s="102" t="s">
+      <c r="A52" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="102"/>
-      <c r="C52" s="102"/>
-      <c r="D52" s="102"/>
-      <c r="E52" s="102"/>
+      <c r="B52" s="98"/>
+      <c r="C52" s="98"/>
+      <c r="D52" s="98"/>
+      <c r="E52" s="98"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53" s="103" t="s">
+      <c r="A53" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="103"/>
-      <c r="C53" s="103"/>
-      <c r="D53" s="103"/>
-      <c r="E53" s="103"/>
+      <c r="B53" s="101"/>
+      <c r="C53" s="101"/>
+      <c r="D53" s="101"/>
+      <c r="E53" s="101"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="95"/>
-      <c r="B54" s="95"/>
-      <c r="C54" s="95"/>
-      <c r="D54" s="95"/>
-      <c r="E54" s="95"/>
+      <c r="A54" s="107"/>
+      <c r="B54" s="107"/>
+      <c r="C54" s="107"/>
+      <c r="D54" s="107"/>
+      <c r="E54" s="107"/>
     </row>
     <row r="55" spans="1:5" s="3" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
@@ -3040,13 +3008,13 @@
       <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="101" t="s">
+      <c r="A56" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="101"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
-      <c r="E56" s="101"/>
+      <c r="B56" s="108"/>
+      <c r="C56" s="108"/>
+      <c r="D56" s="108"/>
+      <c r="E56" s="108"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
@@ -3057,167 +3025,149 @@
       <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" s="93" t="s">
+      <c r="A59" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="93"/>
-      <c r="C59" s="93"/>
-      <c r="D59" s="93"/>
-      <c r="E59" s="93"/>
+      <c r="B59" s="97"/>
+      <c r="C59" s="97"/>
+      <c r="D59" s="97"/>
+      <c r="E59" s="97"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" s="93" t="s">
+      <c r="A60" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="93"/>
-      <c r="C60" s="93"/>
-      <c r="D60" s="93"/>
-      <c r="E60" s="93"/>
+      <c r="B60" s="97"/>
+      <c r="C60" s="97"/>
+      <c r="D60" s="97"/>
+      <c r="E60" s="97"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" s="93" t="s">
+      <c r="A61" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="B61" s="93"/>
-      <c r="C61" s="93"/>
-      <c r="D61" s="93"/>
-      <c r="E61" s="93"/>
+      <c r="B61" s="97"/>
+      <c r="C61" s="97"/>
+      <c r="D61" s="97"/>
+      <c r="E61" s="97"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A62" s="93" t="s">
+      <c r="A62" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="B62" s="93"/>
-      <c r="C62" s="93"/>
-      <c r="D62" s="93"/>
-      <c r="E62" s="93"/>
+      <c r="B62" s="97"/>
+      <c r="C62" s="97"/>
+      <c r="D62" s="97"/>
+      <c r="E62" s="97"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A63" s="93" t="s">
+      <c r="A63" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="93"/>
-      <c r="C63" s="93"/>
-      <c r="D63" s="93"/>
-      <c r="E63" s="93"/>
+      <c r="B63" s="97"/>
+      <c r="C63" s="97"/>
+      <c r="D63" s="97"/>
+      <c r="E63" s="97"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A64" s="95"/>
-      <c r="B64" s="95"/>
-      <c r="C64" s="95"/>
-      <c r="D64" s="95"/>
-      <c r="E64" s="95"/>
+      <c r="A64" s="107"/>
+      <c r="B64" s="107"/>
+      <c r="C64" s="107"/>
+      <c r="D64" s="107"/>
+      <c r="E64" s="107"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A65" s="94" t="s">
+      <c r="A65" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="94"/>
-      <c r="C65" s="94"/>
-      <c r="D65" s="94"/>
-      <c r="E65" s="94"/>
+      <c r="B65" s="100"/>
+      <c r="C65" s="100"/>
+      <c r="D65" s="100"/>
+      <c r="E65" s="100"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A66" s="94" t="s">
+      <c r="A66" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="94"/>
-      <c r="C66" s="94"/>
-      <c r="D66" s="94"/>
-      <c r="E66" s="94"/>
+      <c r="B66" s="100"/>
+      <c r="C66" s="100"/>
+      <c r="D66" s="100"/>
+      <c r="E66" s="100"/>
     </row>
     <row r="67" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="96" t="s">
+      <c r="A67" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="96"/>
-      <c r="C67" s="96"/>
-      <c r="D67" s="96"/>
-      <c r="E67" s="96"/>
+      <c r="B67" s="102"/>
+      <c r="C67" s="102"/>
+      <c r="D67" s="102"/>
+      <c r="E67" s="102"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A68" s="94" t="s">
+      <c r="A68" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="94"/>
-      <c r="C68" s="94"/>
-      <c r="D68" s="94"/>
-      <c r="E68" s="94"/>
+      <c r="B68" s="100"/>
+      <c r="C68" s="100"/>
+      <c r="D68" s="100"/>
+      <c r="E68" s="100"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A69" s="94" t="s">
+      <c r="A69" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="94"/>
-      <c r="C69" s="94"/>
-      <c r="D69" s="94"/>
-      <c r="E69" s="94"/>
+      <c r="B69" s="100"/>
+      <c r="C69" s="100"/>
+      <c r="D69" s="100"/>
+      <c r="E69" s="100"/>
     </row>
     <row r="70" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="96" t="s">
+      <c r="A70" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="96"/>
-      <c r="C70" s="96"/>
-      <c r="D70" s="96"/>
-      <c r="E70" s="96"/>
+      <c r="B70" s="102"/>
+      <c r="C70" s="102"/>
+      <c r="D70" s="102"/>
+      <c r="E70" s="102"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A71" s="94" t="s">
+      <c r="A71" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="B71" s="94"/>
-      <c r="C71" s="94"/>
-      <c r="D71" s="94"/>
-      <c r="E71" s="94"/>
+      <c r="B71" s="100"/>
+      <c r="C71" s="100"/>
+      <c r="D71" s="100"/>
+      <c r="E71" s="100"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A82" s="100" t="s">
+      <c r="A82" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="100"/>
+      <c r="B82" s="106"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="98" t="s">
+      <c r="D82" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="E82" s="98"/>
+      <c r="E82" s="104"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A83" s="99" t="s">
+      <c r="A83" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="99"/>
+      <c r="B83" s="105"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="97" t="s">
+      <c r="D83" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="E83" s="97"/>
+      <c r="E83" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A54:E54"/>
     <mergeCell ref="A69:E69"/>
     <mergeCell ref="A70:E70"/>
     <mergeCell ref="A71:E71"/>
@@ -3234,11 +3184,29 @@
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -3263,16 +3231,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
+      <c r="B1" s="95"/>
     </row>
     <row r="2" spans="1:2" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="106"/>
+      <c r="B2" s="96"/>
     </row>
     <row r="3" spans="1:2" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="109" t="s">
@@ -3281,90 +3249,90 @@
       <c r="B3" s="109"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="102"/>
+      <c r="B4" s="98"/>
     </row>
     <row r="5" spans="1:2" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="107"/>
+      <c r="B5" s="99"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="104"/>
+      <c r="B6" s="94"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="102"/>
+      <c r="B7" s="98"/>
     </row>
     <row r="8" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="93"/>
+      <c r="B8" s="97"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="104"/>
+      <c r="B9" s="94"/>
     </row>
     <row r="10" spans="1:2" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="103"/>
+      <c r="B10" s="101"/>
     </row>
     <row r="11" spans="1:2" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="103"/>
-      <c r="B11" s="103"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="101"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="94"/>
+      <c r="B12" s="100"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="93"/>
+      <c r="B13" s="97"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="95"/>
-      <c r="B14" s="95"/>
+      <c r="A14" s="107"/>
+      <c r="B14" s="107"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="94"/>
+      <c r="B15" s="100"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="93"/>
+      <c r="B16" s="97"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="93"/>
+      <c r="B17" s="97"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="93" t="s">
+      <c r="A18" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="93"/>
+      <c r="B18" s="97"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
@@ -3418,30 +3386,30 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="95"/>
-      <c r="B29" s="95"/>
+      <c r="A29" s="107"/>
+      <c r="B29" s="107"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="102" t="s">
+      <c r="A30" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="102"/>
+      <c r="B30" s="98"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="103"/>
+      <c r="B31" s="101"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="95"/>
-      <c r="B32" s="95"/>
+      <c r="A32" s="107"/>
+      <c r="B32" s="107"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="94" t="s">
+      <c r="A33" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="94"/>
+      <c r="B33" s="100"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
@@ -3449,10 +3417,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="108" t="s">
+      <c r="A35" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="108"/>
+      <c r="B35" s="110"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
@@ -3460,8 +3428,8 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="95"/>
-      <c r="B37" s="95"/>
+      <c r="A37" s="107"/>
+      <c r="B37" s="107"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
@@ -3469,10 +3437,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="103" t="s">
+      <c r="A39" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="103"/>
+      <c r="B39" s="101"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
@@ -3485,16 +3453,16 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="93" t="s">
+      <c r="A43" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="93"/>
+      <c r="B43" s="97"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="93" t="s">
+      <c r="A44" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="93"/>
+      <c r="B44" s="97"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
@@ -3503,110 +3471,110 @@
       <c r="B45" s="14"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="93" t="s">
+      <c r="A46" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="93"/>
+      <c r="B46" s="97"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" s="93" t="s">
+      <c r="A47" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="93"/>
+      <c r="B47" s="97"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" s="93" t="s">
+      <c r="A48" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="93"/>
+      <c r="B48" s="97"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" s="93" t="s">
+      <c r="A49" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="93"/>
+      <c r="B49" s="97"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" s="93" t="s">
+      <c r="A50" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="93"/>
+      <c r="B50" s="97"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="93" t="s">
+      <c r="A51" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="93"/>
+      <c r="B51" s="97"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" s="93" t="s">
+      <c r="A52" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="93"/>
+      <c r="B52" s="97"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="93" t="s">
+      <c r="A53" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="93"/>
+      <c r="B53" s="97"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" s="93" t="s">
+      <c r="A54" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="93"/>
+      <c r="B54" s="97"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" s="93" t="s">
+      <c r="A55" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="93"/>
+      <c r="B55" s="97"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" s="95"/>
-      <c r="B56" s="95"/>
+      <c r="A56" s="107"/>
+      <c r="B56" s="107"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" s="94" t="s">
+      <c r="A57" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="94"/>
+      <c r="B57" s="100"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" s="94" t="s">
+      <c r="A58" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="94"/>
+      <c r="B58" s="100"/>
     </row>
     <row r="59" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="96" t="s">
+      <c r="A59" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="96"/>
+      <c r="B59" s="102"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" s="94" t="s">
+      <c r="A60" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="94"/>
+      <c r="B60" s="100"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" s="94" t="s">
+      <c r="A61" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="94"/>
+      <c r="B61" s="100"/>
     </row>
     <row r="62" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="96" t="s">
+      <c r="A62" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="96"/>
+      <c r="B62" s="102"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" s="94" t="s">
+      <c r="A63" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="94"/>
+      <c r="B63" s="100"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
@@ -3626,20 +3594,22 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A30:B30"/>
@@ -3656,22 +3626,20 @@
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
working on amount feature replacement with exceljs formatting, sales contract templates refactored + small fixes
</commit_message>
<xml_diff>
--- a/templates/Sales_Purchase_Contract.xlsx
+++ b/templates/Sales_Purchase_Contract.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD087B2C-778B-4757-8EA8-E8F667EE5D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12BBDC0-0E3E-4EDF-8350-2AE735A1A739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Invoice" sheetId="5" r:id="rId1"/>
-    <sheet name="Sales_Contract" sheetId="4" r:id="rId2"/>
+    <sheet name="Sales_Contract" sheetId="4" r:id="rId1"/>
+    <sheet name="Invoice" sheetId="5" r:id="rId2"/>
     <sheet name="Contract" sheetId="2" state="hidden" r:id="rId3"/>
     <sheet name="Contract Old" sheetId="1" state="hidden" r:id="rId4"/>
   </sheets>
@@ -28,10 +28,12 @@
     <definedName name="Invoice_sign_seller_end">Invoice!$G$30</definedName>
     <definedName name="Invoice_sign_seller_start">Invoice!$E$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Contract!$A$1:$E$83</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$G$32</definedName>
-    <definedName name="Sign_seller_end">Sales_Contract!$B$53</definedName>
-    <definedName name="Sign_seller_start">Sales_Contract!$A$53</definedName>
-    <definedName name="Документация_BL">Sales_Contract!$A$50</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$32</definedName>
+    <definedName name="Sign_seller_end_1">Sales_Contract!$B$27</definedName>
+    <definedName name="Sign_seller_end_2">Sales_Contract!$B$57</definedName>
+    <definedName name="Sign_seller_start_1">Sales_Contract!$A$27</definedName>
+    <definedName name="Sign_seller_start_2">Sales_Contract!$A$57</definedName>
+    <definedName name="Документация_BL">Sales_Contract!$A$54</definedName>
     <definedName name="Инвойс_адреса_адрес">Invoice!$A$24</definedName>
     <definedName name="Инвойс_адреса_банк">Invoice!$A$26</definedName>
     <definedName name="Инвойс_адреса_банк_адрес">Invoice!$A$27</definedName>
@@ -49,25 +51,27 @@
     <definedName name="Инвойс_продавец">Invoice!$B$9</definedName>
     <definedName name="Инвойс_продавец_печать_подвал">Invoice!$E$32</definedName>
     <definedName name="Инвойс_условия_доставки">Invoice!$B$10</definedName>
-    <definedName name="Контракт_адреса_банк">Sales_Contract!$A$41</definedName>
-    <definedName name="Контракт_адреса_банк_адрес">Sales_Contract!$A$42</definedName>
-    <definedName name="Контракт_адреса_банк_свифт">Sales_Contract!$A$43</definedName>
-    <definedName name="Контракт_адреса_продавец">Sales_Contract!$A$38</definedName>
-    <definedName name="Контракт_адреса_продавец_адрес">Sales_Contract!$A$39</definedName>
-    <definedName name="Контракт_адреса_счет">Sales_Contract!$A$40</definedName>
+    <definedName name="Контракт_адреса_банк">Sales_Contract!$A$45</definedName>
+    <definedName name="Контракт_адреса_банк_адрес">Sales_Contract!$A$46</definedName>
+    <definedName name="Контракт_адреса_банк_свифт">Sales_Contract!$A$47</definedName>
+    <definedName name="Контракт_адреса_продавец">Sales_Contract!$A$42</definedName>
+    <definedName name="Контракт_адреса_продавец_адрес">Sales_Contract!$A$43</definedName>
+    <definedName name="Контракт_адреса_счет">Sales_Contract!$A$44</definedName>
     <definedName name="Контракт_всего_цена">Sales_Contract!$A$25</definedName>
     <definedName name="Контракт_дата">Sales_Contract!$A$4</definedName>
-    <definedName name="Контракт_доставка">Sales_Contract!$A$28</definedName>
+    <definedName name="Контракт_доставка">Sales_Contract!$A$32</definedName>
     <definedName name="Контракт_номер">Sales_Contract!$A$3</definedName>
-    <definedName name="Контракт_оплата">Sales_Contract!$A$34</definedName>
+    <definedName name="Контракт_оплата">Sales_Contract!$A$38</definedName>
     <definedName name="Контракт_покупатель">Sales_Contract!$A$8</definedName>
     <definedName name="Контракт_покупатель_адрес">Sales_Contract!$A$9</definedName>
-    <definedName name="Контракт_покупатель_печать_подвал">Sales_Contract!$D$55</definedName>
+    <definedName name="Контракт_покупатель_печать_подвал_1">Sales_Contract!$D$29</definedName>
+    <definedName name="Контракт_покупатель_печать_подвал_2">Sales_Contract!$D$59</definedName>
     <definedName name="Контракт_предмет">Sales_Contract!$A$13</definedName>
     <definedName name="Контракт_предмет_массив">Sales_Contract!$A$14</definedName>
     <definedName name="Контракт_продавец">Sales_Contract!$A$5</definedName>
     <definedName name="Контракт_продавец_адрес">Sales_Contract!$A$6</definedName>
-    <definedName name="Контракт_продавец_печать_подвал">Sales_Contract!$A$55</definedName>
+    <definedName name="Контракт_продавец_печать_подвал_1">Sales_Contract!$A$29</definedName>
+    <definedName name="Контракт_продавец_печать_подвал_2">Sales_Contract!$A$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -90,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="119">
   <si>
     <t>SALES AND PURCHASE CONTRACT</t>
   </si>
@@ -744,7 +748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -967,6 +971,37 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -984,36 +1019,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1397,14 +1402,652 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FEBAA7-C719-4E24-ABD3-2BE3A9A1FFF7}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A36" zoomScale="106" zoomScaleNormal="157" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:E47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="20.3984375" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" customWidth="1"/>
+    <col min="4" max="4" width="19.796875" customWidth="1"/>
+    <col min="5" max="5" width="24.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="50.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+    </row>
+    <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="51"/>
+    </row>
+    <row r="5" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="53"/>
+    </row>
+    <row r="7" spans="1:5" s="49" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="54"/>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="55"/>
+    </row>
+    <row r="10" spans="1:5" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+    </row>
+    <row r="11" spans="1:5" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="81"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+    </row>
+    <row r="12" spans="1:5" s="49" customFormat="1" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="80" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+    </row>
+    <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="80" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+    </row>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="80" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="57">
+        <v>931</v>
+      </c>
+      <c r="C18" s="58">
+        <v>18620</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="57" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="59">
+        <v>1560</v>
+      </c>
+      <c r="C19" s="58">
+        <v>31200</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="57" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="59">
+        <v>952</v>
+      </c>
+      <c r="C20" s="58">
+        <v>19040</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="57" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="59">
+        <v>114</v>
+      </c>
+      <c r="C21" s="58">
+        <v>2280</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="59">
+        <v>13</v>
+      </c>
+      <c r="C22" s="58">
+        <v>260</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="60">
+        <f>SUM(B18:B22)</f>
+        <v>3570</v>
+      </c>
+      <c r="C23" s="61">
+        <f xml:space="preserve"> SUM(C18:C22)</f>
+        <v>71400</v>
+      </c>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="57"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+    </row>
+    <row r="25" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+    </row>
+    <row r="26" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="56"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+    </row>
+    <row r="27" spans="1:5" ht="100.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" s="71"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="71"/>
+    </row>
+    <row r="29" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="70"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="70"/>
+    </row>
+    <row r="30" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="56"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+    </row>
+    <row r="31" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+    </row>
+    <row r="32" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+    </row>
+    <row r="33" spans="1:5" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="56"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+    </row>
+    <row r="34" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="78"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+    </row>
+    <row r="35" spans="1:5" s="3" customFormat="1" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+    </row>
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="83"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="83"/>
+    </row>
+    <row r="37" spans="1:5" s="49" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="67"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="68"/>
+    </row>
+    <row r="38" spans="1:5" s="3" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" s="85"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="85"/>
+      <c r="E38" s="85"/>
+    </row>
+    <row r="39" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="81" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="81"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
+    </row>
+    <row r="40" spans="1:5" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="63"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+    </row>
+    <row r="41" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="80" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="80"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="80"/>
+      <c r="E41" s="80"/>
+    </row>
+    <row r="42" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="84"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="84"/>
+      <c r="E42" s="84"/>
+    </row>
+    <row r="43" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="81"/>
+      <c r="C43" s="81"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="66"/>
+    </row>
+    <row r="44" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="79"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="79"/>
+      <c r="E44" s="79"/>
+    </row>
+    <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="79" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="79"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="79"/>
+    </row>
+    <row r="46" spans="1:5" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="81"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="66"/>
+    </row>
+    <row r="47" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="79"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="79"/>
+      <c r="E47" s="79"/>
+    </row>
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="63"/>
+      <c r="B48" s="63"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
+    </row>
+    <row r="49" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="62"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="63"/>
+    </row>
+    <row r="50" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" s="84"/>
+      <c r="C50" s="84"/>
+      <c r="D50" s="84"/>
+      <c r="E50" s="84"/>
+    </row>
+    <row r="51" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" s="79"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="79"/>
+    </row>
+    <row r="52" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="79"/>
+      <c r="C52" s="79"/>
+      <c r="D52" s="79"/>
+      <c r="E52" s="79"/>
+    </row>
+    <row r="53" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="79"/>
+      <c r="C53" s="79"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="79"/>
+    </row>
+    <row r="54" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="79"/>
+      <c r="C54" s="79"/>
+      <c r="D54" s="79"/>
+      <c r="E54" s="79"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55" s="50"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
+    </row>
+    <row r="56" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="50"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
+    </row>
+    <row r="57" spans="1:5" ht="100.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="63"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="63"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="71"/>
+      <c r="C58" s="64"/>
+      <c r="D58" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="E58" s="71"/>
+    </row>
+    <row r="59" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="70"/>
+      <c r="C59" s="65"/>
+      <c r="D59" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="E59" s="70"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A38:E38"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="93" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="30" max="16383" man="1"/>
+  </rowBreaks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF949AA7-515D-4019-85D4-70C92EC5672B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScale="127" zoomScaleNormal="100" zoomScaleSheetLayoutView="127" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:C27"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A15" zoomScale="127" zoomScaleNormal="100" zoomScaleSheetLayoutView="127" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1452,15 +2095,15 @@
       <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="53.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
     </row>
     <row r="5" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="32"/>
@@ -1508,12 +2151,12 @@
       <c r="A11" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="92" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
     </row>
     <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="19"/>
@@ -1641,53 +2284,53 @@
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="82"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
     </row>
     <row r="23" spans="1:7" s="17" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="94"/>
     </row>
     <row r="24" spans="1:7" s="17" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="78"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
     </row>
     <row r="25" spans="1:7" s="17" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
     </row>
     <row r="26" spans="1:7" s="17" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="78" t="s">
+      <c r="A26" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="78"/>
-      <c r="C26" s="78"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
     </row>
     <row r="27" spans="1:7" s="17" customFormat="1" ht="36.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="78"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
       <c r="D27" s="30"/>
     </row>
     <row r="28" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="79" t="s">
+      <c r="A28" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="79"/>
-      <c r="C28" s="79"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
       <c r="D28" s="29"/>
       <c r="F28" s="27"/>
       <c r="G28" s="17"/>
@@ -1737,606 +2380,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FEBAA7-C719-4E24-ABD3-2BE3A9A1FFF7}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E55"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A35" zoomScale="106" zoomScaleNormal="157" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:XFD53"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="20.3984375" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" customWidth="1"/>
-    <col min="4" max="4" width="19.796875" customWidth="1"/>
-    <col min="5" max="5" width="24.86328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="50.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-    </row>
-    <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="93" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-    </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="51"/>
-    </row>
-    <row r="5" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="89" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="53"/>
-    </row>
-    <row r="7" spans="1:5" s="49" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="87" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="54"/>
-    </row>
-    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="89" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-    </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="55"/>
-    </row>
-    <row r="10" spans="1:5" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="90" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="90"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
-    </row>
-    <row r="11" spans="1:5" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-    </row>
-    <row r="12" spans="1:5" s="49" customFormat="1" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="85" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="85"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-    </row>
-    <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="86" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="85" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="85"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="85" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="85"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="85"/>
-    </row>
-    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="85" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="85"/>
-    </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="57">
-        <v>931</v>
-      </c>
-      <c r="C18" s="58">
-        <v>18620</v>
-      </c>
-      <c r="D18" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" s="57" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="59">
-        <v>1560</v>
-      </c>
-      <c r="C19" s="58">
-        <v>31200</v>
-      </c>
-      <c r="D19" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="57" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="57" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="59">
-        <v>952</v>
-      </c>
-      <c r="C20" s="58">
-        <v>19040</v>
-      </c>
-      <c r="D20" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="57" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="59">
-        <v>114</v>
-      </c>
-      <c r="C21" s="58">
-        <v>2280</v>
-      </c>
-      <c r="D21" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="57" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="57" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="59">
-        <v>13</v>
-      </c>
-      <c r="C22" s="58">
-        <v>260</v>
-      </c>
-      <c r="D22" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="57" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="60">
-        <f>SUM(B18:B22)</f>
-        <v>3570</v>
-      </c>
-      <c r="C23" s="61">
-        <f xml:space="preserve"> SUM(C18:C22)</f>
-        <v>71400</v>
-      </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="57"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-    </row>
-    <row r="25" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-    </row>
-    <row r="26" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="56"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-    </row>
-    <row r="27" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-    </row>
-    <row r="28" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-    </row>
-    <row r="29" spans="1:5" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="56"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-    </row>
-    <row r="30" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="89" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="89"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-    </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="86" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="86"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
-    </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="88"/>
-      <c r="B32" s="88"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-    </row>
-    <row r="33" spans="1:5" s="49" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="68"/>
-    </row>
-    <row r="34" spans="1:5" s="3" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="91" t="s">
-        <v>112</v>
-      </c>
-      <c r="B34" s="91"/>
-      <c r="C34" s="91"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-    </row>
-    <row r="35" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="86" t="s">
-        <v>113</v>
-      </c>
-      <c r="B35" s="86"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-    </row>
-    <row r="36" spans="1:5" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="63"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-    </row>
-    <row r="37" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="85" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="85"/>
-      <c r="C37" s="85"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="85"/>
-    </row>
-    <row r="38" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="90" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="90"/>
-      <c r="C38" s="90"/>
-      <c r="D38" s="90"/>
-      <c r="E38" s="90"/>
-    </row>
-    <row r="39" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="86"/>
-      <c r="C39" s="86"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="66"/>
-    </row>
-    <row r="40" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="84" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="84"/>
-      <c r="C40" s="84"/>
-      <c r="D40" s="84"/>
-      <c r="E40" s="84"/>
-    </row>
-    <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="84"/>
-      <c r="C41" s="84"/>
-      <c r="D41" s="84"/>
-      <c r="E41" s="84"/>
-    </row>
-    <row r="42" spans="1:5" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="86"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
-      <c r="E42" s="66"/>
-    </row>
-    <row r="43" spans="1:5" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="84" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="84"/>
-      <c r="C43" s="84"/>
-      <c r="D43" s="84"/>
-      <c r="E43" s="84"/>
-    </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="63"/>
-      <c r="B44" s="63"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-    </row>
-    <row r="45" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45" s="62"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="63"/>
-    </row>
-    <row r="46" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="90" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="90"/>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-    </row>
-    <row r="47" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="84" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" s="84"/>
-      <c r="C47" s="84"/>
-      <c r="D47" s="84"/>
-      <c r="E47" s="84"/>
-    </row>
-    <row r="48" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="84" t="s">
-        <v>41</v>
-      </c>
-      <c r="B48" s="84"/>
-      <c r="C48" s="84"/>
-      <c r="D48" s="84"/>
-      <c r="E48" s="84"/>
-    </row>
-    <row r="49" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="84" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="84"/>
-      <c r="C49" s="84"/>
-      <c r="D49" s="84"/>
-      <c r="E49" s="84"/>
-    </row>
-    <row r="50" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="84" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" s="84"/>
-      <c r="C50" s="84"/>
-      <c r="D50" s="84"/>
-      <c r="E50" s="84"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A51" s="50"/>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-    </row>
-    <row r="52" spans="1:5" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="50"/>
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-    </row>
-    <row r="53" spans="1:5" ht="100.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="B53" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" s="63"/>
-      <c r="D53" s="63"/>
-      <c r="E53" s="63"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="B54" s="71"/>
-      <c r="C54" s="64"/>
-      <c r="D54" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="E54" s="71"/>
-    </row>
-    <row r="55" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55" s="70"/>
-      <c r="C55" s="65"/>
-      <c r="D55" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="E55" s="70"/>
-    </row>
-  </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A46:E46"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="93" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="28" max="4" man="1"/>
-  </rowBreaks>
 </worksheet>
 </file>
 
@@ -2358,146 +2401,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
     </row>
     <row r="2" spans="1:5" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
     </row>
     <row r="5" spans="1:5" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="98"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="97" t="s">
+      <c r="A8" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="97"/>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="94" t="s">
+      <c r="A9" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="94"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
     </row>
     <row r="11" spans="1:5" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="101"/>
-      <c r="B11" s="101"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
+      <c r="A11" s="102"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="101"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="100"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
+      <c r="B14" s="101"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="101" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="100"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="100"/>
+      <c r="B15" s="101"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="101"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="100"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="100"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="101"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
@@ -2626,31 +2669,31 @@
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="100"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
-      <c r="E25" s="100"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="101"/>
+      <c r="E25" s="101"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="100" t="s">
+      <c r="A26" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="100"/>
-      <c r="C26" s="100"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
+      <c r="B26" s="101"/>
+      <c r="C26" s="101"/>
+      <c r="D26" s="101"/>
+      <c r="E26" s="101"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="100" t="s">
+      <c r="A27" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="100"/>
-      <c r="C27" s="100"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="100"/>
+      <c r="B27" s="101"/>
+      <c r="C27" s="101"/>
+      <c r="D27" s="101"/>
+      <c r="E27" s="101"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
@@ -2779,31 +2822,31 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="100" t="s">
+      <c r="A36" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="100"/>
-      <c r="C36" s="100"/>
-      <c r="D36" s="100"/>
-      <c r="E36" s="100"/>
+      <c r="B36" s="101"/>
+      <c r="C36" s="101"/>
+      <c r="D36" s="101"/>
+      <c r="E36" s="101"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="100" t="s">
+      <c r="A37" s="101" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="100"/>
+      <c r="B37" s="101"/>
+      <c r="C37" s="101"/>
+      <c r="D37" s="101"/>
+      <c r="E37" s="101"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="100" t="s">
+      <c r="A38" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="100"/>
-      <c r="C38" s="100"/>
-      <c r="D38" s="100"/>
-      <c r="E38" s="100"/>
+      <c r="B38" s="101"/>
+      <c r="C38" s="101"/>
+      <c r="D38" s="101"/>
+      <c r="E38" s="101"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
@@ -2932,13 +2975,13 @@
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="97" t="s">
+      <c r="A47" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="97"/>
-      <c r="C47" s="97"/>
-      <c r="D47" s="97"/>
-      <c r="E47" s="97"/>
+      <c r="B47" s="98"/>
+      <c r="C47" s="98"/>
+      <c r="D47" s="98"/>
+      <c r="E47" s="98"/>
     </row>
     <row r="48" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
@@ -2975,29 +3018,29 @@
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" s="98" t="s">
+      <c r="A52" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="98"/>
-      <c r="C52" s="98"/>
-      <c r="D52" s="98"/>
-      <c r="E52" s="98"/>
+      <c r="B52" s="99"/>
+      <c r="C52" s="99"/>
+      <c r="D52" s="99"/>
+      <c r="E52" s="99"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53" s="101" t="s">
+      <c r="A53" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="101"/>
-      <c r="C53" s="101"/>
-      <c r="D53" s="101"/>
-      <c r="E53" s="101"/>
+      <c r="B53" s="102"/>
+      <c r="C53" s="102"/>
+      <c r="D53" s="102"/>
+      <c r="E53" s="102"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="107"/>
-      <c r="B54" s="107"/>
-      <c r="C54" s="107"/>
-      <c r="D54" s="107"/>
-      <c r="E54" s="107"/>
+      <c r="A54" s="108"/>
+      <c r="B54" s="108"/>
+      <c r="C54" s="108"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="108"/>
     </row>
     <row r="55" spans="1:5" s="3" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
@@ -3008,13 +3051,13 @@
       <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="108" t="s">
+      <c r="A56" s="109" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="108"/>
-      <c r="C56" s="108"/>
-      <c r="D56" s="108"/>
-      <c r="E56" s="108"/>
+      <c r="B56" s="109"/>
+      <c r="C56" s="109"/>
+      <c r="D56" s="109"/>
+      <c r="E56" s="109"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
@@ -3025,141 +3068,141 @@
       <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" s="97" t="s">
+      <c r="A59" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="97"/>
-      <c r="C59" s="97"/>
-      <c r="D59" s="97"/>
-      <c r="E59" s="97"/>
+      <c r="B59" s="98"/>
+      <c r="C59" s="98"/>
+      <c r="D59" s="98"/>
+      <c r="E59" s="98"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" s="97" t="s">
+      <c r="A60" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="97"/>
-      <c r="C60" s="97"/>
-      <c r="D60" s="97"/>
-      <c r="E60" s="97"/>
+      <c r="B60" s="98"/>
+      <c r="C60" s="98"/>
+      <c r="D60" s="98"/>
+      <c r="E60" s="98"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" s="97" t="s">
+      <c r="A61" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="B61" s="97"/>
-      <c r="C61" s="97"/>
-      <c r="D61" s="97"/>
-      <c r="E61" s="97"/>
+      <c r="B61" s="98"/>
+      <c r="C61" s="98"/>
+      <c r="D61" s="98"/>
+      <c r="E61" s="98"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A62" s="97" t="s">
+      <c r="A62" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B62" s="97"/>
-      <c r="C62" s="97"/>
-      <c r="D62" s="97"/>
-      <c r="E62" s="97"/>
+      <c r="B62" s="98"/>
+      <c r="C62" s="98"/>
+      <c r="D62" s="98"/>
+      <c r="E62" s="98"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A63" s="97" t="s">
+      <c r="A63" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="97"/>
-      <c r="C63" s="97"/>
-      <c r="D63" s="97"/>
-      <c r="E63" s="97"/>
+      <c r="B63" s="98"/>
+      <c r="C63" s="98"/>
+      <c r="D63" s="98"/>
+      <c r="E63" s="98"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A64" s="107"/>
-      <c r="B64" s="107"/>
-      <c r="C64" s="107"/>
-      <c r="D64" s="107"/>
-      <c r="E64" s="107"/>
+      <c r="A64" s="108"/>
+      <c r="B64" s="108"/>
+      <c r="C64" s="108"/>
+      <c r="D64" s="108"/>
+      <c r="E64" s="108"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A65" s="100" t="s">
+      <c r="A65" s="101" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="100"/>
-      <c r="C65" s="100"/>
-      <c r="D65" s="100"/>
-      <c r="E65" s="100"/>
+      <c r="B65" s="101"/>
+      <c r="C65" s="101"/>
+      <c r="D65" s="101"/>
+      <c r="E65" s="101"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A66" s="100" t="s">
+      <c r="A66" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="100"/>
-      <c r="C66" s="100"/>
-      <c r="D66" s="100"/>
-      <c r="E66" s="100"/>
+      <c r="B66" s="101"/>
+      <c r="C66" s="101"/>
+      <c r="D66" s="101"/>
+      <c r="E66" s="101"/>
     </row>
     <row r="67" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="102" t="s">
+      <c r="A67" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="102"/>
-      <c r="C67" s="102"/>
-      <c r="D67" s="102"/>
-      <c r="E67" s="102"/>
+      <c r="B67" s="103"/>
+      <c r="C67" s="103"/>
+      <c r="D67" s="103"/>
+      <c r="E67" s="103"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A68" s="100" t="s">
+      <c r="A68" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="100"/>
-      <c r="C68" s="100"/>
-      <c r="D68" s="100"/>
-      <c r="E68" s="100"/>
+      <c r="B68" s="101"/>
+      <c r="C68" s="101"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="101"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A69" s="100" t="s">
+      <c r="A69" s="101" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="100"/>
-      <c r="C69" s="100"/>
-      <c r="D69" s="100"/>
-      <c r="E69" s="100"/>
+      <c r="B69" s="101"/>
+      <c r="C69" s="101"/>
+      <c r="D69" s="101"/>
+      <c r="E69" s="101"/>
     </row>
     <row r="70" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="102" t="s">
+      <c r="A70" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="102"/>
-      <c r="C70" s="102"/>
-      <c r="D70" s="102"/>
-      <c r="E70" s="102"/>
+      <c r="B70" s="103"/>
+      <c r="C70" s="103"/>
+      <c r="D70" s="103"/>
+      <c r="E70" s="103"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A71" s="100" t="s">
+      <c r="A71" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="B71" s="100"/>
-      <c r="C71" s="100"/>
-      <c r="D71" s="100"/>
-      <c r="E71" s="100"/>
+      <c r="B71" s="101"/>
+      <c r="C71" s="101"/>
+      <c r="D71" s="101"/>
+      <c r="E71" s="101"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A82" s="106" t="s">
+      <c r="A82" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="106"/>
+      <c r="B82" s="107"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="104" t="s">
+      <c r="D82" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="E82" s="104"/>
+      <c r="E82" s="105"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A83" s="105" t="s">
+      <c r="A83" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="105"/>
+      <c r="B83" s="106"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="103" t="s">
+      <c r="D83" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="E83" s="103"/>
+      <c r="E83" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -3231,108 +3274,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="96"/>
     </row>
     <row r="2" spans="1:2" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="96"/>
+      <c r="B2" s="97"/>
     </row>
     <row r="3" spans="1:2" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="109"/>
+      <c r="B3" s="110"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="98"/>
+      <c r="B4" s="99"/>
     </row>
     <row r="5" spans="1:2" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="99"/>
+      <c r="B5" s="100"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="95"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="98"/>
+      <c r="B7" s="99"/>
     </row>
     <row r="8" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="97" t="s">
+      <c r="A8" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="97"/>
+      <c r="B8" s="98"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="94" t="s">
+      <c r="A9" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="94"/>
+      <c r="B9" s="95"/>
     </row>
     <row r="10" spans="1:2" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="101"/>
+      <c r="B10" s="102"/>
     </row>
     <row r="11" spans="1:2" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="101"/>
-      <c r="B11" s="101"/>
+      <c r="A11" s="102"/>
+      <c r="B11" s="102"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="100"/>
+      <c r="B12" s="101"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="97"/>
+      <c r="B13" s="98"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="107"/>
-      <c r="B14" s="107"/>
+      <c r="A14" s="108"/>
+      <c r="B14" s="108"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="100"/>
+      <c r="B15" s="101"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="97"/>
+      <c r="B16" s="98"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="97" t="s">
+      <c r="A17" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="97"/>
+      <c r="B17" s="98"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="97" t="s">
+      <c r="A18" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="97"/>
+      <c r="B18" s="98"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
@@ -3386,30 +3429,30 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="107"/>
-      <c r="B29" s="107"/>
+      <c r="A29" s="108"/>
+      <c r="B29" s="108"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="98" t="s">
+      <c r="A30" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="98"/>
+      <c r="B30" s="99"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="101" t="s">
+      <c r="A31" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="101"/>
+      <c r="B31" s="102"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="107"/>
-      <c r="B32" s="107"/>
+      <c r="A32" s="108"/>
+      <c r="B32" s="108"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="100" t="s">
+      <c r="A33" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="100"/>
+      <c r="B33" s="101"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
@@ -3417,10 +3460,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="110" t="s">
+      <c r="A35" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="110"/>
+      <c r="B35" s="111"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
@@ -3428,8 +3471,8 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="107"/>
-      <c r="B37" s="107"/>
+      <c r="A37" s="108"/>
+      <c r="B37" s="108"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
@@ -3437,10 +3480,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="101" t="s">
+      <c r="A39" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="101"/>
+      <c r="B39" s="102"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
@@ -3453,16 +3496,16 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="97" t="s">
+      <c r="A43" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="97"/>
+      <c r="B43" s="98"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="97" t="s">
+      <c r="A44" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="97"/>
+      <c r="B44" s="98"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
@@ -3471,110 +3514,110 @@
       <c r="B45" s="14"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="97" t="s">
+      <c r="A46" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="97"/>
+      <c r="B46" s="98"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" s="97" t="s">
+      <c r="A47" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="97"/>
+      <c r="B47" s="98"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" s="97" t="s">
+      <c r="A48" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="97"/>
+      <c r="B48" s="98"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" s="97" t="s">
+      <c r="A49" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="97"/>
+      <c r="B49" s="98"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" s="97" t="s">
+      <c r="A50" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="97"/>
+      <c r="B50" s="98"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="97" t="s">
+      <c r="A51" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="97"/>
+      <c r="B51" s="98"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" s="97" t="s">
+      <c r="A52" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="97"/>
+      <c r="B52" s="98"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="97" t="s">
+      <c r="A53" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="97"/>
+      <c r="B53" s="98"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" s="97" t="s">
+      <c r="A54" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="97"/>
+      <c r="B54" s="98"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" s="97" t="s">
+      <c r="A55" s="98" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="97"/>
+      <c r="B55" s="98"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" s="107"/>
-      <c r="B56" s="107"/>
+      <c r="A56" s="108"/>
+      <c r="B56" s="108"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" s="100" t="s">
+      <c r="A57" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="100"/>
+      <c r="B57" s="101"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" s="100" t="s">
+      <c r="A58" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="100"/>
+      <c r="B58" s="101"/>
     </row>
     <row r="59" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="102" t="s">
+      <c r="A59" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="102"/>
+      <c r="B59" s="103"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" s="100" t="s">
+      <c r="A60" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="100"/>
+      <c r="B60" s="101"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" s="100" t="s">
+      <c r="A61" s="101" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="100"/>
+      <c r="B61" s="101"/>
     </row>
     <row r="62" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="102" t="s">
+      <c r="A62" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="102"/>
+      <c r="B62" s="103"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" s="100" t="s">
+      <c r="A63" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="100"/>
+      <c r="B63" s="101"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">

</xml_diff>

<commit_message>
rows modules refactored with initRowMaker closure, some fixes in sales contract
</commit_message>
<xml_diff>
--- a/templates/Sales_Purchase_Contract.xlsx
+++ b/templates/Sales_Purchase_Contract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12BBDC0-0E3E-4EDF-8350-2AE735A1A739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA44C0DF-A9E2-44D4-B463-5E6CE74AFDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" activeTab="1" xr2:uid="{36A75300-EFCB-4154-8D49-868D6DB376F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales_Contract" sheetId="4" r:id="rId1"/>
@@ -30,9 +30,9 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">Contract!$A$1:$E$83</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$32</definedName>
     <definedName name="Sign_seller_end_1">Sales_Contract!$B$27</definedName>
-    <definedName name="Sign_seller_end_2">Sales_Contract!$B$57</definedName>
+    <definedName name="Sign_seller_end_2">Sales_Contract!$B$58</definedName>
     <definedName name="Sign_seller_start_1">Sales_Contract!$A$27</definedName>
-    <definedName name="Sign_seller_start_2">Sales_Contract!$A$57</definedName>
+    <definedName name="Sign_seller_start_2">Sales_Contract!$A$58</definedName>
     <definedName name="Документация_BL">Sales_Contract!$A$54</definedName>
     <definedName name="Инвойс_адреса_адрес">Invoice!$A$24</definedName>
     <definedName name="Инвойс_адреса_банк">Invoice!$A$26</definedName>
@@ -65,13 +65,13 @@
     <definedName name="Контракт_покупатель">Sales_Contract!$A$8</definedName>
     <definedName name="Контракт_покупатель_адрес">Sales_Contract!$A$9</definedName>
     <definedName name="Контракт_покупатель_печать_подвал_1">Sales_Contract!$D$29</definedName>
-    <definedName name="Контракт_покупатель_печать_подвал_2">Sales_Contract!$D$59</definedName>
+    <definedName name="Контракт_покупатель_печать_подвал_2">Sales_Contract!$D$60</definedName>
     <definedName name="Контракт_предмет">Sales_Contract!$A$13</definedName>
     <definedName name="Контракт_предмет_массив">Sales_Contract!$A$14</definedName>
     <definedName name="Контракт_продавец">Sales_Contract!$A$5</definedName>
     <definedName name="Контракт_продавец_адрес">Sales_Contract!$A$6</definedName>
     <definedName name="Контракт_продавец_печать_подвал_1">Sales_Contract!$A$29</definedName>
-    <definedName name="Контракт_продавец_печать_подвал_2">Sales_Contract!$A$59</definedName>
+    <definedName name="Контракт_продавец_печать_подвал_2">Sales_Contract!$A$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="122">
   <si>
     <t>SALES AND PURCHASE CONTRACT</t>
   </si>
@@ -426,9 +426,6 @@
     <t>1 634 382,40 $</t>
   </si>
   <si>
-    <t>FCA, ZARUBINO</t>
-  </si>
-  <si>
     <t>40 000,00 $</t>
   </si>
   <si>
@@ -454,9 +451,6 @@
   </si>
   <si>
     <t>(hereafter called “Seller”)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.1 The payment to be in US Dollar 100% value should be made by T.T. to the designated the Seller’s or Agent’s bank account within 5 banking days after the all parties signed the contract. </t>
   </si>
   <si>
     <t>4.2 The Seller performs production tittle transfer after 100% payment to Seller’s banking account.</t>
@@ -498,6 +492,21 @@
   </si>
   <si>
     <t>_________________________________________________________________________________________________________________________</t>
+  </si>
+  <si>
+    <t>- Certificate of Origin issued by Russian chamber of commerce and industry (copy)</t>
+  </si>
+  <si>
+    <t>- IUU Catch Certificate issued by the Territory Department (copy);</t>
+  </si>
+  <si>
+    <t>4.1 The payment to be in US Dollar 100% value should be made by T.T. to the designated the Seller’s or Agent’s bank account within 5 banking days after Buyer's verification of the documents, described in 6. Documentation.</t>
+  </si>
+  <si>
+    <t>Supply of products is carried out on FCA Zarubino, Russia.</t>
+  </si>
+  <si>
+    <t>FCA ZARUBINO, RUSSIA</t>
   </si>
 </sst>
 </file>
@@ -748,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -874,9 +883,6 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -973,13 +979,25 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -987,21 +1005,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1021,6 +1027,39 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1030,46 +1069,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1406,10 +1424,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A36" zoomScale="106" zoomScaleNormal="157" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:E47"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A24" zoomScale="106" zoomScaleNormal="157" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1422,597 +1440,593 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="50.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="80" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="50"/>
+    </row>
+    <row r="5" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="52"/>
+    </row>
+    <row r="7" spans="1:5" s="48" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="85" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="53"/>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="54"/>
+    </row>
+    <row r="10" spans="1:5" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+    </row>
+    <row r="11" spans="1:5" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="82"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+    </row>
+    <row r="12" spans="1:5" s="48" customFormat="1" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="83" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+    </row>
+    <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="83"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+    </row>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="83"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="83"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="56">
+        <v>931</v>
+      </c>
+      <c r="C18" s="57">
+        <v>18620</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="58">
+        <v>1560</v>
+      </c>
+      <c r="C19" s="57">
+        <v>31200</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="58">
+        <v>952</v>
+      </c>
+      <c r="C20" s="57">
+        <v>19040</v>
+      </c>
+      <c r="D20" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="56" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="58">
         <v>114</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-    </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="51"/>
-    </row>
-    <row r="5" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="81" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="53"/>
-    </row>
-    <row r="7" spans="1:5" s="49" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="82" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="54"/>
-    </row>
-    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-    </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="55"/>
-    </row>
-    <row r="10" spans="1:5" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="84" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-    </row>
-    <row r="11" spans="1:5" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="81"/>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-    </row>
-    <row r="12" spans="1:5" s="49" customFormat="1" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="80" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-    </row>
-    <row r="13" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="81" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="81"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="80" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="80" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-    </row>
-    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="80" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-    </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="57">
-        <v>931</v>
-      </c>
-      <c r="C18" s="58">
-        <v>18620</v>
-      </c>
-      <c r="D18" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" s="57" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="59">
-        <v>1560</v>
-      </c>
-      <c r="C19" s="58">
-        <v>31200</v>
-      </c>
-      <c r="D19" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="57" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="57" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="59">
-        <v>952</v>
-      </c>
-      <c r="C20" s="58">
-        <v>19040</v>
-      </c>
-      <c r="D20" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="57" t="s">
+      <c r="C21" s="57">
+        <v>2280</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="56" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="59">
-        <v>114</v>
-      </c>
-      <c r="C21" s="58">
-        <v>2280</v>
-      </c>
-      <c r="D21" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="57" t="s">
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="58">
+        <v>13</v>
+      </c>
+      <c r="C22" s="57">
+        <v>260</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="56" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="57" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="59">
-        <v>13</v>
-      </c>
-      <c r="C22" s="58">
-        <v>260</v>
-      </c>
-      <c r="D22" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="57" t="s">
-        <v>107</v>
-      </c>
-    </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="60">
+      <c r="B23" s="59">
         <f>SUM(B18:B22)</f>
         <v>3570</v>
       </c>
-      <c r="C23" s="61">
+      <c r="C23" s="60">
         <f xml:space="preserve"> SUM(C18:C22)</f>
         <v>71400</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51" t="s">
-        <v>108</v>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="57"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
+      <c r="A24" s="56"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
     </row>
     <row r="25" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
+      <c r="A25" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
     </row>
     <row r="26" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="56"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
     </row>
     <row r="27" spans="1:5" ht="100.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" s="71"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="71"/>
+      <c r="A28" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="70"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="70"/>
     </row>
     <row r="29" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="70" t="s">
+      <c r="A29" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="70" t="s">
+      <c r="B29" s="69"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="70"/>
+      <c r="E29" s="69"/>
     </row>
     <row r="30" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="56"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
+      <c r="A30" s="55"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
     </row>
     <row r="31" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
     </row>
     <row r="32" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
+      <c r="A32" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
     </row>
     <row r="33" spans="1:5" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="56"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
     </row>
     <row r="34" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="78" t="s">
+      <c r="A34" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
     </row>
     <row r="35" spans="1:5" s="3" customFormat="1" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="55" t="s">
+      <c r="A35" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="83"/>
-      <c r="B36" s="83"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-    </row>
-    <row r="37" spans="1:5" s="49" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="67" t="s">
+      <c r="A36" s="86"/>
+      <c r="B36" s="86"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+    </row>
+    <row r="37" spans="1:5" s="48" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="67"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="68"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="67"/>
     </row>
     <row r="38" spans="1:5" s="3" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" s="85"/>
-      <c r="C38" s="85"/>
-      <c r="D38" s="85"/>
-      <c r="E38" s="85"/>
+      <c r="A38" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="87"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="87"/>
+      <c r="E38" s="87"/>
     </row>
     <row r="39" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="81" t="s">
-        <v>113</v>
-      </c>
-      <c r="B39" s="81"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
+      <c r="A39" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
     </row>
     <row r="40" spans="1:5" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="63"/>
-      <c r="B40" s="63"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="63"/>
+      <c r="A40" s="62"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="62"/>
     </row>
     <row r="41" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="80" t="s">
+      <c r="A41" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="80"/>
-      <c r="C41" s="80"/>
-      <c r="D41" s="80"/>
-      <c r="E41" s="80"/>
+      <c r="B41" s="83"/>
+      <c r="C41" s="83"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="83"/>
     </row>
     <row r="42" spans="1:5" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="84" t="s">
+      <c r="A42" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="84"/>
-      <c r="C42" s="84"/>
-      <c r="D42" s="84"/>
-      <c r="E42" s="84"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="78"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="78"/>
     </row>
     <row r="43" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="81" t="s">
+      <c r="A43" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="81"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="66"/>
+      <c r="B43" s="82"/>
+      <c r="C43" s="82"/>
+      <c r="D43" s="82"/>
+      <c r="E43" s="65"/>
     </row>
     <row r="44" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="79" t="s">
+      <c r="A44" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="79"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="79"/>
-      <c r="E44" s="79"/>
+      <c r="B44" s="84"/>
+      <c r="C44" s="84"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="84"/>
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="79" t="s">
+      <c r="A45" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="79"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="79"/>
-      <c r="E45" s="79"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="84"/>
     </row>
     <row r="46" spans="1:5" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="81" t="s">
+      <c r="A46" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="81"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="66"/>
+      <c r="B46" s="82"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="65"/>
     </row>
     <row r="47" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="79" t="s">
+      <c r="A47" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="79"/>
-      <c r="C47" s="79"/>
-      <c r="D47" s="79"/>
-      <c r="E47" s="79"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="84"/>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="63"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="63"/>
-      <c r="D48" s="63"/>
-      <c r="E48" s="63"/>
+      <c r="A48" s="62"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="62"/>
+      <c r="E48" s="62"/>
     </row>
     <row r="49" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="62" t="s">
+      <c r="A49" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="62"/>
-      <c r="C49" s="62"/>
-      <c r="D49" s="62"/>
-      <c r="E49" s="63"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="62"/>
     </row>
     <row r="50" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="84" t="s">
+      <c r="A50" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="84"/>
-      <c r="C50" s="84"/>
-      <c r="D50" s="84"/>
-      <c r="E50" s="84"/>
+      <c r="B50" s="113"/>
+      <c r="C50" s="113"/>
+      <c r="D50" s="113"/>
+      <c r="E50" s="113"/>
     </row>
     <row r="51" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="79" t="s">
+      <c r="A51" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="B51" s="79"/>
-      <c r="C51" s="79"/>
-      <c r="D51" s="79"/>
-      <c r="E51" s="79"/>
+      <c r="B51" s="112"/>
+      <c r="C51" s="112"/>
+      <c r="D51" s="112"/>
+      <c r="E51" s="112"/>
     </row>
     <row r="52" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="79" t="s">
+      <c r="A52" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="79"/>
-      <c r="C52" s="79"/>
-      <c r="D52" s="79"/>
-      <c r="E52" s="79"/>
+      <c r="B52" s="112"/>
+      <c r="C52" s="112"/>
+      <c r="D52" s="112"/>
+      <c r="E52" s="112"/>
     </row>
     <row r="53" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="79" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" s="79"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
+      <c r="A53" s="112" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" s="112"/>
+      <c r="C53" s="112"/>
+      <c r="D53" s="112"/>
+      <c r="E53" s="112"/>
     </row>
     <row r="54" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="79" t="s">
+      <c r="A54" s="112" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="79"/>
-      <c r="C54" s="79"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="79"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A55" s="50"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-    </row>
-    <row r="56" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="50"/>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-    </row>
-    <row r="57" spans="1:5" ht="100.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="63" t="s">
+      <c r="B54" s="112"/>
+      <c r="C54" s="112"/>
+      <c r="D54" s="112"/>
+      <c r="E54" s="112"/>
+    </row>
+    <row r="55" spans="1:5" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="111" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" s="111"/>
+      <c r="C55" s="111"/>
+      <c r="D55" s="111"/>
+      <c r="E55" s="111"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" s="49"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="49"/>
+    </row>
+    <row r="57" spans="1:5" ht="43.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="49"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="49"/>
+    </row>
+    <row r="58" spans="1:5" ht="100.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="B57" s="63" t="s">
+      <c r="B58" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="63"/>
-      <c r="D57" s="63"/>
-      <c r="E57" s="63"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A58" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" s="71"/>
-      <c r="C58" s="64"/>
-      <c r="D58" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="E58" s="71"/>
-    </row>
-    <row r="59" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
+      <c r="E58" s="62"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" s="70"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="E59" s="70"/>
+    </row>
+    <row r="60" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="70"/>
-      <c r="C59" s="65"/>
-      <c r="D59" s="70" t="s">
+      <c r="B60" s="69"/>
+      <c r="C60" s="64"/>
+      <c r="D60" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="E59" s="70"/>
+      <c r="E60" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
     <mergeCell ref="A52:E52"/>
     <mergeCell ref="A53:E53"/>
     <mergeCell ref="A54:E54"/>
@@ -2029,6 +2043,19 @@
     <mergeCell ref="A50:E50"/>
     <mergeCell ref="A43:D43"/>
     <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -2046,8 +2073,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A15" zoomScale="127" zoomScaleNormal="100" zoomScaleSheetLayoutView="127" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="127" zoomScaleNormal="100" zoomScaleSheetLayoutView="127" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2073,19 +2100,19 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
     </row>
     <row r="3" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="74" t="s">
-        <v>118</v>
+      <c r="A3" s="73" t="s">
+        <v>116</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -2095,15 +2122,15 @@
       <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="53.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
     </row>
     <row r="5" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="32"/>
@@ -2144,19 +2171,19 @@
         <v>88</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="91" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
     </row>
     <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="19"/>
@@ -2176,7 +2203,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F13" s="39" t="s">
         <v>96</v>
@@ -2204,7 +2231,7 @@
       <c r="F14" s="37">
         <v>25190</v>
       </c>
-      <c r="G14" s="45">
+      <c r="G14" s="114">
         <v>1410640</v>
       </c>
     </row>
@@ -2264,13 +2291,13 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="22"/>
       <c r="B20" s="26"/>
-      <c r="C20" s="75" t="s">
+      <c r="C20" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="75"/>
+      <c r="D20" s="74"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="46" t="s">
+      <c r="G20" s="45" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2284,61 +2311,61 @@
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="93"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
     </row>
     <row r="23" spans="1:7" s="17" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="93"/>
     </row>
     <row r="24" spans="1:7" s="17" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="89" t="s">
+      <c r="A24" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="89"/>
-      <c r="C24" s="89"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
     </row>
     <row r="25" spans="1:7" s="17" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="90"/>
-      <c r="C25" s="90"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
     </row>
     <row r="26" spans="1:7" s="17" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="89" t="s">
+      <c r="A26" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="89"/>
-      <c r="C26" s="89"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="88"/>
     </row>
     <row r="27" spans="1:7" s="17" customFormat="1" ht="36.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="89" t="s">
+      <c r="A27" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="89"/>
-      <c r="C27" s="89"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="88"/>
       <c r="D27" s="30"/>
     </row>
     <row r="28" spans="1:7" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="90"/>
-      <c r="C28" s="90"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="89"/>
       <c r="D28" s="29"/>
       <c r="F28" s="27"/>
       <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:7" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="72"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
+      <c r="A29" s="71"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
       <c r="D29" s="29"/>
       <c r="F29" s="27"/>
       <c r="G29" s="17"/>
@@ -2360,11 +2387,11 @@
       <c r="G31" s="17"/>
     </row>
     <row r="32" spans="1:7" ht="30.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E32" s="76" t="s">
+      <c r="E32" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="77"/>
-      <c r="G32" s="77"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2401,146 +2428,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
     </row>
     <row r="2" spans="1:5" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
     </row>
     <row r="5" spans="1:5" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="99"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="95"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="102" t="s">
+      <c r="A10" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="102"/>
-      <c r="C10" s="102"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
     </row>
     <row r="11" spans="1:5" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="102"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
+      <c r="A11" s="104"/>
+      <c r="B11" s="104"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="104"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="101"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="101"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="98"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="101" t="s">
+      <c r="A14" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="101"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="101" t="s">
+      <c r="A15" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="101"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="101" t="s">
+      <c r="A16" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
@@ -2566,14 +2593,14 @@
       <c r="B18" s="6">
         <v>931</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="46">
         <v>18620</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2583,14 +2610,14 @@
       <c r="B19" s="15">
         <v>1560</v>
       </c>
-      <c r="C19" s="47">
+      <c r="C19" s="46">
         <v>31200</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2600,14 +2627,14 @@
       <c r="B20" s="15">
         <v>952</v>
       </c>
-      <c r="C20" s="47">
+      <c r="C20" s="46">
         <v>19040</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2617,14 +2644,14 @@
       <c r="B21" s="15">
         <v>114</v>
       </c>
-      <c r="C21" s="47">
+      <c r="C21" s="46">
         <v>2280</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2634,14 +2661,14 @@
       <c r="B22" s="15">
         <v>13</v>
       </c>
-      <c r="C22" s="47">
+      <c r="C22" s="46">
         <v>260</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2652,13 +2679,13 @@
         <f>SUM(B18:B22)</f>
         <v>3570</v>
       </c>
-      <c r="C23" s="48">
+      <c r="C23" s="47">
         <f xml:space="preserve"> SUM(C18:C22)</f>
         <v>71400</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2669,31 +2696,31 @@
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="101" t="s">
+      <c r="A25" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="101"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="101"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="101" t="s">
+      <c r="A26" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="101"/>
-      <c r="C26" s="101"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="101"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="101" t="s">
+      <c r="A27" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="101"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="101"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
@@ -2723,10 +2750,10 @@
         <v>18620</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2740,10 +2767,10 @@
         <v>31200</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2757,10 +2784,10 @@
         <v>19040</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2774,10 +2801,10 @@
         <v>2280</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2791,10 +2818,10 @@
         <v>260</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2805,13 +2832,13 @@
         <f>SUM(B29:B33)</f>
         <v>3570</v>
       </c>
-      <c r="C34" s="48">
+      <c r="C34" s="47">
         <f xml:space="preserve"> SUM(C29:C33)</f>
         <v>71400</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2822,31 +2849,31 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="101" t="s">
+      <c r="A36" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="101"/>
-      <c r="C36" s="101"/>
-      <c r="D36" s="101"/>
-      <c r="E36" s="101"/>
+      <c r="B36" s="95"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="95"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="101" t="s">
+      <c r="A37" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="101"/>
-      <c r="C37" s="101"/>
-      <c r="D37" s="101"/>
-      <c r="E37" s="101"/>
+      <c r="B37" s="95"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="95"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="101"/>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
+      <c r="B38" s="95"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="95"/>
+      <c r="E38" s="95"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
@@ -2876,10 +2903,10 @@
         <v>18620</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2893,10 +2920,10 @@
         <v>31200</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2910,10 +2937,10 @@
         <v>19040</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2927,10 +2954,10 @@
         <v>2280</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -2944,10 +2971,10 @@
         <v>260</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2958,13 +2985,13 @@
         <f>SUM(B40:B44)</f>
         <v>3570</v>
       </c>
-      <c r="C45" s="48">
+      <c r="C45" s="47">
         <f xml:space="preserve"> SUM(C40:C44)</f>
         <v>71400</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -2975,17 +3002,17 @@
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="98" t="s">
+      <c r="A47" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="98"/>
-      <c r="C47" s="98"/>
-      <c r="D47" s="98"/>
-      <c r="E47" s="98"/>
+      <c r="B47" s="94"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="94"/>
+      <c r="E47" s="94"/>
     </row>
     <row r="48" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -3018,29 +3045,29 @@
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" s="99" t="s">
+      <c r="A52" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="99"/>
-      <c r="C52" s="99"/>
-      <c r="D52" s="99"/>
-      <c r="E52" s="99"/>
+      <c r="B52" s="103"/>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53" s="102" t="s">
+      <c r="A53" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="102"/>
-      <c r="C53" s="102"/>
-      <c r="D53" s="102"/>
-      <c r="E53" s="102"/>
+      <c r="B53" s="104"/>
+      <c r="C53" s="104"/>
+      <c r="D53" s="104"/>
+      <c r="E53" s="104"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="108"/>
-      <c r="B54" s="108"/>
-      <c r="C54" s="108"/>
-      <c r="D54" s="108"/>
-      <c r="E54" s="108"/>
+      <c r="A54" s="96"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="96"/>
+      <c r="D54" s="96"/>
+      <c r="E54" s="96"/>
     </row>
     <row r="55" spans="1:5" s="3" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
@@ -3051,13 +3078,13 @@
       <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="109" t="s">
+      <c r="A56" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="109"/>
-      <c r="C56" s="109"/>
-      <c r="D56" s="109"/>
-      <c r="E56" s="109"/>
+      <c r="B56" s="102"/>
+      <c r="C56" s="102"/>
+      <c r="D56" s="102"/>
+      <c r="E56" s="102"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
@@ -3068,149 +3095,167 @@
       <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" s="98" t="s">
+      <c r="A59" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="98"/>
-      <c r="C59" s="98"/>
-      <c r="D59" s="98"/>
-      <c r="E59" s="98"/>
+      <c r="B59" s="94"/>
+      <c r="C59" s="94"/>
+      <c r="D59" s="94"/>
+      <c r="E59" s="94"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" s="98" t="s">
+      <c r="A60" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="98"/>
-      <c r="C60" s="98"/>
-      <c r="D60" s="98"/>
-      <c r="E60" s="98"/>
+      <c r="B60" s="94"/>
+      <c r="C60" s="94"/>
+      <c r="D60" s="94"/>
+      <c r="E60" s="94"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" s="98" t="s">
+      <c r="A61" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B61" s="98"/>
-      <c r="C61" s="98"/>
-      <c r="D61" s="98"/>
-      <c r="E61" s="98"/>
+      <c r="B61" s="94"/>
+      <c r="C61" s="94"/>
+      <c r="D61" s="94"/>
+      <c r="E61" s="94"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A62" s="98" t="s">
+      <c r="A62" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B62" s="98"/>
-      <c r="C62" s="98"/>
-      <c r="D62" s="98"/>
-      <c r="E62" s="98"/>
+      <c r="B62" s="94"/>
+      <c r="C62" s="94"/>
+      <c r="D62" s="94"/>
+      <c r="E62" s="94"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A63" s="98" t="s">
+      <c r="A63" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="98"/>
-      <c r="C63" s="98"/>
-      <c r="D63" s="98"/>
-      <c r="E63" s="98"/>
+      <c r="B63" s="94"/>
+      <c r="C63" s="94"/>
+      <c r="D63" s="94"/>
+      <c r="E63" s="94"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A64" s="108"/>
-      <c r="B64" s="108"/>
-      <c r="C64" s="108"/>
-      <c r="D64" s="108"/>
-      <c r="E64" s="108"/>
+      <c r="A64" s="96"/>
+      <c r="B64" s="96"/>
+      <c r="C64" s="96"/>
+      <c r="D64" s="96"/>
+      <c r="E64" s="96"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A65" s="101" t="s">
+      <c r="A65" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="101"/>
-      <c r="C65" s="101"/>
-      <c r="D65" s="101"/>
-      <c r="E65" s="101"/>
+      <c r="B65" s="95"/>
+      <c r="C65" s="95"/>
+      <c r="D65" s="95"/>
+      <c r="E65" s="95"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A66" s="101" t="s">
+      <c r="A66" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="101"/>
-      <c r="C66" s="101"/>
-      <c r="D66" s="101"/>
-      <c r="E66" s="101"/>
+      <c r="B66" s="95"/>
+      <c r="C66" s="95"/>
+      <c r="D66" s="95"/>
+      <c r="E66" s="95"/>
     </row>
     <row r="67" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="103" t="s">
+      <c r="A67" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="103"/>
-      <c r="C67" s="103"/>
-      <c r="D67" s="103"/>
-      <c r="E67" s="103"/>
+      <c r="B67" s="97"/>
+      <c r="C67" s="97"/>
+      <c r="D67" s="97"/>
+      <c r="E67" s="97"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A68" s="101" t="s">
+      <c r="A68" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="101"/>
-      <c r="C68" s="101"/>
-      <c r="D68" s="101"/>
-      <c r="E68" s="101"/>
+      <c r="B68" s="95"/>
+      <c r="C68" s="95"/>
+      <c r="D68" s="95"/>
+      <c r="E68" s="95"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A69" s="101" t="s">
+      <c r="A69" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="101"/>
-      <c r="C69" s="101"/>
-      <c r="D69" s="101"/>
-      <c r="E69" s="101"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="95"/>
+      <c r="E69" s="95"/>
     </row>
     <row r="70" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="103" t="s">
+      <c r="A70" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="103"/>
-      <c r="C70" s="103"/>
-      <c r="D70" s="103"/>
-      <c r="E70" s="103"/>
+      <c r="B70" s="97"/>
+      <c r="C70" s="97"/>
+      <c r="D70" s="97"/>
+      <c r="E70" s="97"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A71" s="101" t="s">
+      <c r="A71" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="B71" s="101"/>
-      <c r="C71" s="101"/>
-      <c r="D71" s="101"/>
-      <c r="E71" s="101"/>
+      <c r="B71" s="95"/>
+      <c r="C71" s="95"/>
+      <c r="D71" s="95"/>
+      <c r="E71" s="95"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A82" s="107" t="s">
+      <c r="A82" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="107"/>
+      <c r="B82" s="101"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="105" t="s">
+      <c r="D82" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="E82" s="105"/>
+      <c r="E82" s="99"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A83" s="106" t="s">
+      <c r="A83" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="106"/>
+      <c r="B83" s="100"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="104" t="s">
+      <c r="D83" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="E83" s="104"/>
+      <c r="E83" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A47:E47"/>
     <mergeCell ref="A69:E69"/>
     <mergeCell ref="A70:E70"/>
     <mergeCell ref="A71:E71"/>
@@ -3227,29 +3272,11 @@
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A54:E54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -3274,16 +3301,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
+      <c r="B1" s="106"/>
     </row>
     <row r="2" spans="1:2" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="97"/>
+      <c r="B2" s="107"/>
     </row>
     <row r="3" spans="1:2" ht="22.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="110" t="s">
@@ -3292,90 +3319,90 @@
       <c r="B3" s="110"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99"/>
+      <c r="B4" s="103"/>
     </row>
     <row r="5" spans="1:2" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="108"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="95"/>
+      <c r="B6" s="105"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="99"/>
+      <c r="B7" s="103"/>
     </row>
     <row r="8" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="98"/>
+      <c r="B8" s="94"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="95"/>
+      <c r="B9" s="105"/>
     </row>
     <row r="10" spans="1:2" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="102" t="s">
+      <c r="A10" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="102"/>
+      <c r="B10" s="104"/>
     </row>
     <row r="11" spans="1:2" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="102"/>
-      <c r="B11" s="102"/>
+      <c r="A11" s="104"/>
+      <c r="B11" s="104"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="101"/>
+      <c r="B12" s="95"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="98"/>
+      <c r="B13" s="94"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="108"/>
-      <c r="B14" s="108"/>
+      <c r="A14" s="96"/>
+      <c r="B14" s="96"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="101" t="s">
+      <c r="A15" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="101"/>
+      <c r="B15" s="95"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="98" t="s">
+      <c r="A16" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="98"/>
+      <c r="B16" s="94"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="98" t="s">
+      <c r="A17" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="98"/>
+      <c r="B17" s="94"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="98" t="s">
+      <c r="A18" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="98"/>
+      <c r="B18" s="94"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
@@ -3429,30 +3456,30 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="108"/>
-      <c r="B29" s="108"/>
+      <c r="A29" s="96"/>
+      <c r="B29" s="96"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="99" t="s">
+      <c r="A30" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="99"/>
+      <c r="B30" s="103"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="102" t="s">
+      <c r="A31" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="102"/>
+      <c r="B31" s="104"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="108"/>
-      <c r="B32" s="108"/>
+      <c r="A32" s="96"/>
+      <c r="B32" s="96"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="101" t="s">
+      <c r="A33" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="101"/>
+      <c r="B33" s="95"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
@@ -3460,10 +3487,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="111" t="s">
+      <c r="A35" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="111"/>
+      <c r="B35" s="109"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
@@ -3471,8 +3498,8 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="108"/>
-      <c r="B37" s="108"/>
+      <c r="A37" s="96"/>
+      <c r="B37" s="96"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
@@ -3480,10 +3507,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="102" t="s">
+      <c r="A39" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="102"/>
+      <c r="B39" s="104"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
@@ -3496,16 +3523,16 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="98" t="s">
+      <c r="A43" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="98"/>
+      <c r="B43" s="94"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="98" t="s">
+      <c r="A44" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="98"/>
+      <c r="B44" s="94"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
@@ -3514,110 +3541,110 @@
       <c r="B45" s="14"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="98" t="s">
+      <c r="A46" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="98"/>
+      <c r="B46" s="94"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" s="98" t="s">
+      <c r="A47" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="98"/>
+      <c r="B47" s="94"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" s="98" t="s">
+      <c r="A48" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="98"/>
+      <c r="B48" s="94"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" s="98" t="s">
+      <c r="A49" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="98"/>
+      <c r="B49" s="94"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" s="98" t="s">
+      <c r="A50" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="98"/>
+      <c r="B50" s="94"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="98" t="s">
+      <c r="A51" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="98"/>
+      <c r="B51" s="94"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" s="98" t="s">
+      <c r="A52" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="98"/>
+      <c r="B52" s="94"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="98" t="s">
+      <c r="A53" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="98"/>
+      <c r="B53" s="94"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" s="98" t="s">
+      <c r="A54" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="98"/>
+      <c r="B54" s="94"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" s="98" t="s">
+      <c r="A55" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="98"/>
+      <c r="B55" s="94"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" s="108"/>
-      <c r="B56" s="108"/>
+      <c r="A56" s="96"/>
+      <c r="B56" s="96"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" s="101" t="s">
+      <c r="A57" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="101"/>
+      <c r="B57" s="95"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" s="101" t="s">
+      <c r="A58" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="101"/>
+      <c r="B58" s="95"/>
     </row>
     <row r="59" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="103" t="s">
+      <c r="A59" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="103"/>
+      <c r="B59" s="97"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" s="101" t="s">
+      <c r="A60" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="101"/>
+      <c r="B60" s="95"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" s="101" t="s">
+      <c r="A61" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="101"/>
+      <c r="B61" s="95"/>
     </row>
     <row r="62" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="103" t="s">
+      <c r="A62" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="103"/>
+      <c r="B62" s="97"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" s="101" t="s">
+      <c r="A63" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="101"/>
+      <c r="B63" s="95"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
@@ -3637,6 +3664,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A58:B58"/>
@@ -3653,36 +3710,6 @@
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>

</xml_diff>